<commit_message>
Format first two columns in template XLSX as date columns
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damiand/Projects/MoJ/CCD/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4F6A1F-4DB3-4341-8AD8-8E7464A4A184}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B436534-D35D-0243-B3BF-79047E9B4447}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" firstSheet="11" activeTab="17" xr2:uid="{6814ABA7-9773-3248-9354-D8EFB3344628}"/>
+    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{6814ABA7-9773-3248-9354-D8EFB3344628}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -602,6 +602,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -764,7 +767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -819,6 +822,7 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1135,11 +1139,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A95678C-FB6E-0F4C-82CE-06AAFD1C109E}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1200,10 +1207,13 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1271,10 +1281,13 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1342,10 +1355,13 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1413,10 +1429,13 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
@@ -1484,10 +1503,13 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1553,10 +1575,13 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1617,10 +1642,13 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
@@ -1688,10 +1716,13 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1758,11 +1789,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633DD08F-00C2-6541-8FCD-9FC10AE68C6E}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1830,10 +1864,13 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
@@ -1922,10 +1959,13 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -2035,10 +2075,13 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -2141,10 +2184,13 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:O3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -2275,10 +2321,13 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -2360,10 +2409,13 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:T3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -2529,10 +2581,13 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -2593,10 +2648,13 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="38"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Added MidEvent columns to caseEventToFields
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damiand/Projects/MoJ/CCD/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelc/app/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B436534-D35D-0243-B3BF-79047E9B4447}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE2FAB5-0565-B84A-9743-955D0DE326AC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{6814ABA7-9773-3248-9354-D8EFB3344628}"/>
+    <workbookView xWindow="5120" yWindow="3660" windowWidth="27640" windowHeight="16940" activeTab="4" xr2:uid="{6814ABA7-9773-3248-9354-D8EFB3344628}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId17"/>
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="164">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -596,6 +596,18 @@
   </si>
   <si>
     <t>CaseStateID</t>
+  </si>
+  <si>
+    <t>CallBackURLMidEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLMidEvent</t>
+  </si>
+  <si>
+    <t>URL to call back to the service for uniqueness. </t>
+  </si>
+  <si>
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). </t>
   </si>
 </sst>
 </file>
@@ -605,7 +617,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -746,6 +758,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -767,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -823,6 +849,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1139,7 +1167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A95678C-FB6E-0F4C-82CE-06AAFD1C109E}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C2" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2181,18 +2209,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790F2027-3175-F945-9DC5-62CDA1AF2757}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="38"/>
+    <col min="15" max="15" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
@@ -2217,7 +2246,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" ht="253" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="253" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -2263,8 +2292,14 @@
       <c r="O2" s="6" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q2" s="40" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -2309,6 +2344,12 @@
       </c>
       <c r="O3" s="9" t="s">
         <v>81</v>
+      </c>
+      <c r="P3" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q3" s="39" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2408,7 +2449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C95A00A-1FD5-404B-9CAE-5EDF553D40AA}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H2" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added MidEvent columns to caseEventToFields (#14)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damiand/Projects/MoJ/CCD/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelc/app/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B436534-D35D-0243-B3BF-79047E9B4447}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7BC1EE-5EAC-E44D-AED4-14BA00FDB9CC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{6814ABA7-9773-3248-9354-D8EFB3344628}"/>
+    <workbookView xWindow="1160" yWindow="1060" windowWidth="27640" windowHeight="16940" activeTab="4" xr2:uid="{6814ABA7-9773-3248-9354-D8EFB3344628}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId17"/>
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="164">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -596,6 +596,18 @@
   </si>
   <si>
     <t>CaseStateID</t>
+  </si>
+  <si>
+    <t>CallBackURLMidEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLMidEvent</t>
+  </si>
+  <si>
+    <t>URL to call back to the service for uniqueness. </t>
+  </si>
+  <si>
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). </t>
   </si>
 </sst>
 </file>
@@ -605,7 +617,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -746,6 +758,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -767,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -823,6 +849,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1139,7 +1169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A95678C-FB6E-0F4C-82CE-06AAFD1C109E}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C2" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2181,18 +2211,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790F2027-3175-F945-9DC5-62CDA1AF2757}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="38"/>
+    <col min="15" max="15" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
@@ -2217,7 +2248,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" ht="253" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="253" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -2263,8 +2294,14 @@
       <c r="O2" s="6" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="40" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q2" s="40" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -2309,6 +2346,12 @@
       </c>
       <c r="O3" s="9" t="s">
         <v>81</v>
+      </c>
+      <c r="P3" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q3" s="39" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2408,7 +2451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C95A00A-1FD5-404B-9CAE-5EDF553D40AA}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H2" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add Authrization Complext Type Tab
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelc/app/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qianghmcts/workspace/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7BC1EE-5EAC-E44D-AED4-14BA00FDB9CC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6C01A9-87B6-0140-94D7-EB61F5DB33BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1060" windowWidth="27640" windowHeight="16940" activeTab="4" xr2:uid="{6814ABA7-9773-3248-9354-D8EFB3344628}"/>
+    <workbookView xWindow="1160" yWindow="1060" windowWidth="27640" windowHeight="16940" firstSheet="12" activeTab="18" xr2:uid="{6814ABA7-9773-3248-9354-D8EFB3344628}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId16"/>
     <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId17"/>
     <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId18"/>
+    <sheet name="AuthorisationComplexType" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="167">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -608,6 +609,17 @@
   </si>
   <si>
     <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). </t>
+  </si>
+  <si>
+    <t>AuthorisationComplexType</t>
+  </si>
+  <si>
+    <t>The Field ID should match an ID in the CaseField Tab
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>C - Create, R - Read, U - Update, D - Delete
+MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
   </si>
 </sst>
 </file>
@@ -617,7 +629,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -771,6 +783,63 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF984807"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -790,10 +859,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -853,9 +923,24 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2 3" xfId="1" xr:uid="{81F74F0A-CD53-1449-8F0E-21C059BF91B0}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1889,6 +1974,80 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E19DBFA4-A604-4544-8A99-C507A8AFEA24}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+    </row>
+    <row r="2" spans="1:7" ht="253" x14ac:dyDescent="0.2">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1ED2F3-56C7-2C44-829E-D1B4DF60B639}">
   <dimension ref="A1:I3"/>
@@ -2213,7 +2372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790F2027-3175-F945-9DC5-62CDA1AF2757}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
RDM-2986: added AuthorisationComplexType into default template
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -27,6 +27,7 @@
     <sheet name="AuthorisationCaseField" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="AuthorisationCaseEvent" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="AuthorisationCaseState" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="AuthorisationComplexType" sheetId="20" state="visible" r:id="rId21"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="175">
   <si>
     <t xml:space="preserve">Jurisdiction</t>
   </si>
@@ -629,6 +630,17 @@
   </si>
   <si>
     <t xml:space="preserve">CaseStateID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AuthorisationComplexType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Field ID should match an ID in the CaseField Tab
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C - Create, R - Read, U - Update, D - Delete
+MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
   </si>
 </sst>
 </file>
@@ -665,6 +677,12 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
@@ -688,12 +706,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF984807"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -836,7 +848,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -860,12 +872,16 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="65">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -874,11 +890,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -891,6 +903,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -914,7 +930,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -938,7 +954,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -950,71 +966,71 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1074,15 +1090,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1090,15 +1106,52 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal 2 3" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1171,7 +1224,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="A:B C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1248,7 +1301,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1381,7 +1434,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1465,7 +1518,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1549,7 +1602,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1633,7 +1686,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1717,7 +1770,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1799,7 +1852,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1876,7 +1929,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1960,7 +2013,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2044,7 +2097,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2128,7 +2181,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2221,6 +2274,92 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.49"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+    </row>
+    <row r="2" customFormat="false" ht="128.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="61"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="62" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="62" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" s="62" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="64" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="63" t="s">
+        <v>162</v>
+      </c>
+      <c r="G3" s="63" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2233,7 +2372,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2359,7 +2498,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2478,7 +2617,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2639,7 +2778,7 @@
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2776,7 +2915,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2874,7 +3013,7 @@
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3056,7 +3195,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A:B"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add SearchAlias tab (#23)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Projects/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markry/workspace/hmcts/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998E719D-9D37-824E-A32A-D5EDE0E67DE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7150401A-DC12-AE4B-8B26-C41BD6F143F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27660" windowHeight="13840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27660" windowHeight="13840" tabRatio="500" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,16 @@
     <sheet name="FixedLists" sheetId="9" r:id="rId10"/>
     <sheet name="ComplexTypes" sheetId="10" r:id="rId11"/>
     <sheet name="SearchInputFields" sheetId="11" r:id="rId12"/>
-    <sheet name="SearchResultFields" sheetId="12" r:id="rId13"/>
-    <sheet name="WorkBasketResultFields" sheetId="13" r:id="rId14"/>
-    <sheet name="WorkBasketInputFields" sheetId="14" r:id="rId15"/>
-    <sheet name="UserProfile" sheetId="15" r:id="rId16"/>
-    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId17"/>
-    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId18"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId19"/>
-    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId20"/>
-    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId21"/>
+    <sheet name="SearchAlias" sheetId="22" r:id="rId13"/>
+    <sheet name="SearchResultFields" sheetId="12" r:id="rId14"/>
+    <sheet name="WorkBasketResultFields" sheetId="13" r:id="rId15"/>
+    <sheet name="WorkBasketInputFields" sheetId="14" r:id="rId16"/>
+    <sheet name="UserProfile" sheetId="15" r:id="rId17"/>
+    <sheet name="AuthorisationCaseType" sheetId="16" r:id="rId18"/>
+    <sheet name="AuthorisationCaseField" sheetId="17" r:id="rId19"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="18" r:id="rId20"/>
+    <sheet name="AuthorisationCaseState" sheetId="19" r:id="rId21"/>
+    <sheet name="AuthorisationComplexType" sheetId="20" r:id="rId22"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="182">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -656,6 +657,18 @@
   </si>
   <si>
     <t>MaxLength:128</t>
+  </si>
+  <si>
+    <t>SearchAlias</t>
+  </si>
+  <si>
+    <t>Unique alias id for a case field of a case type</t>
+  </si>
+  <si>
+    <t>This is just the CaseField ID for top level fields, or object notation pointing to a complex type field e.g. applicantAddress.AddressLine1</t>
+  </si>
+  <si>
+    <t>SearchAliasID</t>
   </si>
 </sst>
 </file>
@@ -1537,7 +1550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1663,7 +1676,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1735,6 +1748,66 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F890146-8CBA-D54C-80DE-8CB5C69F30BD}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="44"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1810,7 +1883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1886,7 +1959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1962,7 +2035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2036,7 +2109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2105,7 +2178,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2181,7 +2254,112 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A1F9531-C488-E44F-88C9-2FD2D5D8808A}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="65" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="F2" s="69" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="70" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="71" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="72" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="73"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="73"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="73"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="73"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="73"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2257,112 +2435,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A1F9531-C488-E44F-88C9-2FD2D5D8808A}">
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="65" t="s">
-        <v>175</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="67" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="68" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="69" t="s">
-        <v>176</v>
-      </c>
-      <c r="B2" s="69" t="s">
-        <v>176</v>
-      </c>
-      <c r="C2" s="69" t="s">
-        <v>176</v>
-      </c>
-      <c r="D2" s="69" t="s">
-        <v>176</v>
-      </c>
-      <c r="E2" s="69" t="s">
-        <v>176</v>
-      </c>
-      <c r="F2" s="69" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="71" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="72" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="72" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="73"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="73"/>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="73"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="73"/>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="73"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2438,7 +2511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added display order to fixed lists tab
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markry/workspace/hmcts/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesne@kainos.com/Documents/HMCTS/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7150401A-DC12-AE4B-8B26-C41BD6F143F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417E6340-8942-BE4E-8EF8-C8D38CF15417}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27660" windowHeight="13840" tabRatio="500" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27660" windowHeight="13840" tabRatio="500" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="183">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -669,6 +669,9 @@
   </si>
   <si>
     <t>SearchAliasID</t>
+  </si>
+  <si>
+    <t>Numbered order of fixed list items</t>
   </si>
 </sst>
 </file>
@@ -1479,10 +1482,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1491,7 +1494,7 @@
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>128</v>
       </c>
@@ -1506,7 +1509,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1522,8 +1525,11 @@
       <c r="E2" s="13" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1538,6 +1544,9 @@
       </c>
       <c r="E3" s="9" t="s">
         <v>132</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1751,7 +1760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F890146-8CBA-D54C-80DE-8CB5C69F30BD}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update template with new field
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markry/workspace/hmcts/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7150401A-DC12-AE4B-8B26-C41BD6F143F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEB92CE-F18C-7245-BC80-7E39C36B7899}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27660" windowHeight="13840" tabRatio="500" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="1480" windowWidth="27660" windowHeight="13840" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="184">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -669,6 +669,13 @@
   </si>
   <si>
     <t>SearchAliasID</t>
+  </si>
+  <si>
+    <t>DisplayContextParameter</t>
+  </si>
+  <si>
+    <t>Text should begin with #LIST( or #TABLE(
+MaxLength: 1000</t>
   </si>
 </sst>
 </file>
@@ -1751,7 +1758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F890146-8CBA-D54C-80DE-8CB5C69F30BD}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2810,19 +2817,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
+    <col min="3" max="10" width="10.5" customWidth="1"/>
+    <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
@@ -2843,7 +2853,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" ht="183" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="183" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2877,8 +2887,11 @@
       <c r="K2" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -2911,6 +2924,9 @@
       </c>
       <c r="K3" s="10" t="s">
         <v>59</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add DisplayContextParameter to CaseTypeTab fields (#26)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markry/workspace/hmcts/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7150401A-DC12-AE4B-8B26-C41BD6F143F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEB92CE-F18C-7245-BC80-7E39C36B7899}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27660" windowHeight="13840" tabRatio="500" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="1480" windowWidth="27660" windowHeight="13840" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="184">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -669,6 +669,13 @@
   </si>
   <si>
     <t>SearchAliasID</t>
+  </si>
+  <si>
+    <t>DisplayContextParameter</t>
+  </si>
+  <si>
+    <t>Text should begin with #LIST( or #TABLE(
+MaxLength: 1000</t>
   </si>
 </sst>
 </file>
@@ -1751,7 +1758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F890146-8CBA-D54C-80DE-8CB5C69F30BD}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2810,19 +2817,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
+    <col min="3" max="10" width="10.5" customWidth="1"/>
+    <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
@@ -2843,7 +2853,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11" ht="183" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="183" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2877,8 +2887,11 @@
       <c r="K2" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -2911,6 +2924,9 @@
       </c>
       <c r="K3" s="10" t="s">
         <v>59</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added description for fixedlist displayorder
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesne@kainos.com/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesne@kainos.com/Documents/HMCTS/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35CEC39-EB06-C14A-90D5-CD1E02FA4109}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C5389F-44E9-5543-AEAF-D28FD1EF5269}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35200" yWindow="1500" windowWidth="27660" windowHeight="13840" tabRatio="500" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-50300" yWindow="2100" windowWidth="27660" windowHeight="13840" tabRatio="500" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="185">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -676,6 +676,9 @@
   <si>
     <t>Text should begin with #LIST( or #TABLE(
 MaxLength: 1000</t>
+  </si>
+  <si>
+    <t>The display order of list items. Positive integers e.g 1, 2, 3</t>
   </si>
 </sst>
 </file>
@@ -1489,7 +1492,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1528,6 +1531,9 @@
       </c>
       <c r="E2" s="13" t="s">
         <v>131</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added display order to fixed lists tab (#25)
* Added display order to fixed lists tab

* Updated definition processor assets to support FixedLists's DisplayOrder

* Updated FixedLists fixture displayOrder value

* Added description for fixedlist displayorder
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markry/workspace/hmcts/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesne@kainos.com/Documents/HMCTS/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEB92CE-F18C-7245-BC80-7E39C36B7899}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C5389F-44E9-5543-AEAF-D28FD1EF5269}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="1480" windowWidth="27660" windowHeight="13840" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-50300" yWindow="2100" windowWidth="27660" windowHeight="13840" tabRatio="500" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="185">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -676,6 +676,9 @@
   <si>
     <t>Text should begin with #LIST( or #TABLE(
 MaxLength: 1000</t>
+  </si>
+  <si>
+    <t>The display order of list items. Positive integers e.g 1, 2, 3</t>
   </si>
 </sst>
 </file>
@@ -1486,10 +1489,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1498,7 +1501,7 @@
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>128</v>
       </c>
@@ -1513,7 +1516,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1529,8 +1532,11 @@
       <c r="E2" s="13" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1545,6 +1551,9 @@
       </c>
       <c r="E3" s="9" t="s">
         <v>132</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2819,7 +2828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
DIV-4872 - added UserRole tab to the template
To be able to show/hide tabs based on a user role
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesne@kainos.com/Documents/HMCTS/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Dev/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C5389F-44E9-5543-AEAF-D28FD1EF5269}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CF64E5-3CB6-F646-BD67-5509257ADBF5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50300" yWindow="2100" windowWidth="27660" windowHeight="13840" tabRatio="500" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="186">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -679,6 +679,9 @@
   </si>
   <si>
     <t>The display order of list items. Positive integers e.g 1, 2, 3</t>
+  </si>
+  <si>
+    <t>MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
   </si>
 </sst>
 </file>
@@ -1491,7 +1494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -2826,22 +2829,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="10" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="1025" width="10.5" customWidth="1"/>
+    <col min="3" max="11" width="10.5" customWidth="1"/>
+    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="1026" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
@@ -2861,8 +2864,9 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
-    </row>
-    <row r="2" spans="1:12" ht="183" x14ac:dyDescent="0.2">
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="1:13" ht="183" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2888,19 +2892,22 @@
         <v>48</v>
       </c>
       <c r="I2" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -2925,16 +2932,19 @@
       <c r="H3" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>182</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DIV-4872 - Add UserRole column to CaseTypeTab (#29)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesne@kainos.com/Documents/HMCTS/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Dev/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C5389F-44E9-5543-AEAF-D28FD1EF5269}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CF64E5-3CB6-F646-BD67-5509257ADBF5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50300" yWindow="2100" windowWidth="27660" windowHeight="13840" tabRatio="500" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="186">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -679,6 +679,9 @@
   </si>
   <si>
     <t>The display order of list items. Positive integers e.g 1, 2, 3</t>
+  </si>
+  <si>
+    <t>MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
   </si>
 </sst>
 </file>
@@ -1491,7 +1494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -2826,22 +2829,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="10" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="1025" width="10.5" customWidth="1"/>
+    <col min="3" max="11" width="10.5" customWidth="1"/>
+    <col min="12" max="12" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="1026" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
@@ -2861,8 +2864,9 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
-    </row>
-    <row r="2" spans="1:12" ht="183" x14ac:dyDescent="0.2">
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="1:13" ht="183" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2888,19 +2892,22 @@
         <v>48</v>
       </c>
       <c r="I2" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -2925,16 +2932,19 @@
       <c r="H3" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>182</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add listElementCode for workbasket result fields
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Dev/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharmendrak/development/moj/ccd/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CF64E5-3CB6-F646-BD67-5509257ADBF5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F2BE06-1CDE-D540-9BB9-CC8685551735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="187">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -682,6 +682,9 @@
   </si>
   <si>
     <t>MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
   </si>
 </sst>
 </file>
@@ -922,7 +925,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -930,12 +933,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1040,6 +1058,12 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1904,19 +1928,21 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
+    <col min="3" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="1026" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>148</v>
       </c>
@@ -1929,10 +1955,12 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+      <c r="G1" s="6"/>
+      <c r="H1" s="74"/>
+    </row>
+    <row r="2" spans="1:8" ht="141" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1945,14 +1973,20 @@
       <c r="D2" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="75" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H2" s="75" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -1965,11 +1999,17 @@
       <c r="D3" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="76" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>101</v>
+      </c>
+      <c r="H3" s="77" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2831,7 +2871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add listElementCode for workbasket result fields (#32)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Dev/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharmendrak/development/moj/ccd/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CF64E5-3CB6-F646-BD67-5509257ADBF5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F2BE06-1CDE-D540-9BB9-CC8685551735}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="187">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -682,6 +682,9 @@
   </si>
   <si>
     <t>MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
   </si>
 </sst>
 </file>
@@ -922,7 +925,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -930,12 +933,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1040,6 +1058,12 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1904,19 +1928,21 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
+    <col min="3" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="1026" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>148</v>
       </c>
@@ -1929,10 +1955,12 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6"/>
+      <c r="E1" s="74"/>
       <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+      <c r="G1" s="6"/>
+      <c r="H1" s="74"/>
+    </row>
+    <row r="2" spans="1:8" ht="141" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1945,14 +1973,20 @@
       <c r="D2" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="75" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H2" s="75" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -1965,11 +1999,17 @@
       <c r="D3" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="76" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>101</v>
+      </c>
+      <c r="H3" s="77" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2831,7 +2871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding ResultsOrdering to WorkbasketResults Tab
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,37 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harryh/DIV/ccd-definition-processor/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A976087-33D7-6E4C-96A7-1B3D8CC0F30B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Jurisdiction" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="CaseRoles" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="CaseType" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="CaseField" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="CaseTypeTab" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="CaseEventToFields" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="CaseEventToComplexTypes" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="State" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="CaseEvent" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="FixedLists" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="ComplexTypes" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="SearchInputFields" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="SearchAlias" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="SearchResultFields" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="WorkBasketResultFields" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="WorkBasketInputFields" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="UserProfile" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="AuthorisationCaseType" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="AuthorisationCaseField" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="AuthorisationCaseState" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="AuthorisationComplexType" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
+    <sheet name="CaseRoles" sheetId="2" r:id="rId2"/>
+    <sheet name="CaseType" sheetId="3" r:id="rId3"/>
+    <sheet name="CaseField" sheetId="4" r:id="rId4"/>
+    <sheet name="CaseTypeTab" sheetId="5" r:id="rId5"/>
+    <sheet name="CaseEventToFields" sheetId="6" r:id="rId6"/>
+    <sheet name="CaseEventToComplexTypes" sheetId="7" r:id="rId7"/>
+    <sheet name="State" sheetId="8" r:id="rId8"/>
+    <sheet name="CaseEvent" sheetId="9" r:id="rId9"/>
+    <sheet name="FixedLists" sheetId="10" r:id="rId10"/>
+    <sheet name="ComplexTypes" sheetId="11" r:id="rId11"/>
+    <sheet name="SearchInputFields" sheetId="12" r:id="rId12"/>
+    <sheet name="SearchAlias" sheetId="13" r:id="rId13"/>
+    <sheet name="SearchResultFields" sheetId="14" r:id="rId14"/>
+    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId15"/>
+    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId16"/>
+    <sheet name="UserProfile" sheetId="17" r:id="rId17"/>
+    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId18"/>
+    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId19"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId20"/>
+    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId21"/>
+    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId22"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -41,670 +46,674 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="191">
-  <si>
-    <t xml:space="preserve">Jurisdiction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrimaryKeyInRed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrimaryAndForeignKey Orange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ForeignKey Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start date from which the data will be valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End date until which the data will be valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The identifier which defines the casetype code
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="193">
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t>PrimaryKeyInRed</t>
+  </si>
+  <si>
+    <t>PrimaryAndForeignKey Orange</t>
+  </si>
+  <si>
+    <t>ForeignKey Brown</t>
+  </si>
+  <si>
+    <t>Start date from which the data will be valid</t>
+  </si>
+  <si>
+    <t>End date until which the data will be valid</t>
+  </si>
+  <si>
+    <t>The identifier which defines the casetype code
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The short description to describe the jurisdiction used on UI display
+    <t>The short description to describe the jurisdiction used on UI display
 MaxLength: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">The long description to describe the jurisdiction.
+    <t>The long description to describe the jurisdiction.
 MaxLength: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">LiveFrom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LiveTo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseRoles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength: 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength:128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The short description to describe the case type used on the UI.
+    <t>LiveFrom</t>
+  </si>
+  <si>
+    <t>LiveTo</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>CaseRoles</t>
+  </si>
+  <si>
+    <t>MaxLength: 40</t>
+  </si>
+  <si>
+    <t>MaxLength:128</t>
+  </si>
+  <si>
+    <t>CaseTypeID</t>
+  </si>
+  <si>
+    <t>CaseType</t>
+  </si>
+  <si>
+    <t>The short description to describe the case type used on the UI.
 MaxLength: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">The long description to decribe the case type.
+    <t>The long description to decribe the case type.
 MaxLength: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">The jurisdiction code should match the one defined in 'Jurisdiction' tab
+    <t>The jurisdiction code should match the one defined in 'Jurisdiction' tab
 MaxLength:70</t>
   </si>
   <si>
-    <t xml:space="preserve">The absolute URL to the microservice which lists the documents that the services wants to provide for print. 
+    <t>The absolute URL to the microservice which lists the documents that the services wants to provide for print. 
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). Max Length: 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It is a mandatory field which can define if the data classification of the field
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). Max Length: 20</t>
+  </si>
+  <si>
+    <t>It is a mandatory field which can define if the data classification of the field
 MustBe: &lt;Public, Private, Retricted&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">JurisdictionID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrintableDocumentsUrl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLPrintEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SecurityClassification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseField</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The code of casetype has to be defined in 'CaseType' tab
+    <t>JurisdictionID</t>
+  </si>
+  <si>
+    <t>PrintableDocumentsUrl</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLPrintEvent</t>
+  </si>
+  <si>
+    <t>SecurityClassification</t>
+  </si>
+  <si>
+    <t>CaseField</t>
+  </si>
+  <si>
+    <t>The code of casetype has to be defined in 'CaseType' tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The field ID should match the field attribute name used by the service team in creating the case
+    <t>The field ID should match the field attribute name used by the service team in creating the case
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
+    <t>The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
 MaxLength:&lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The hint text that is present for each field type
+    <t>The hint text that is present for each field type
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The type of field. This can be a CCD Base type (see confluence) or a ComplexType ID as per the ComplexType tab).  
+    <t>The type of field. This can be a CCD Base type (see confluence) or a ComplexType ID as per the ComplexType tab).  
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Some FieldTypes require or have an optional addition parameter that can be set (e.g. Collection - the parameter is the collecion of What FieldType ?, FixedList the parameter is the ID from the fixedList tab). See confluence for details
+    <t>Some FieldTypes require or have an optional addition parameter that can be set (e.g. Collection - the parameter is the collecion of What FieldType ?, FixedList the parameter is the ID from the fixedList tab). See confluence for details
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">The regex that can define the type of data accepted in the fields E.g: alphanumeric etc. This will override the regex, if defined internally for any type.
+    <t>The regex that can define the type of data accepted in the fields E.g: alphanumeric etc. This will override the regex, if defined internally for any type.
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The minimum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
+    <t>The minimum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The maximum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
+    <t>The maximum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HintText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldTypeParameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RegularExpression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseTypeTab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not used yet - maybe used for roletype type view later
+    <t>Label</t>
+  </si>
+  <si>
+    <t>HintText</t>
+  </si>
+  <si>
+    <t>FieldType</t>
+  </si>
+  <si>
+    <t>FieldTypeParameter</t>
+  </si>
+  <si>
+    <t>RegularExpression</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>CaseTypeTab</t>
+  </si>
+  <si>
+    <t>Not used yet - maybe used for roletype type view later
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">Unique Id for tab. MaxLength: 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name to be displayed on the tab
+    <t>Unique Id for tab. MaxLength: 40</t>
+  </si>
+  <si>
+    <t>Name to be displayed on the tab
 MaxLengh: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">Order of Tab on screen - left to right.
+    <t>Order of Tab on screen - left to right.
 PositiveInteger</t>
   </si>
   <si>
-    <t xml:space="preserve">Unique ID for field - must match an ID on the CaseField tab or be a metadata item. 
+    <t>Unique ID for field - must match an ID on the CaseField tab or be a metadata item. 
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order of Fields within a tab - top to bottom
+    <t>MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
+  </si>
+  <si>
+    <t>Order of Fields within a tab - top to bottom
 PositiveInteger</t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
+    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
 MaxLength:1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean expression rules for hiding a tab: 
+    <t>Boolean expression rules for hiding a tab: 
 MaxLength:1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Text should begin with #LIST( or #TABLE(
+    <t>Text should begin with #LIST( or #TABLE(
 MaxLength: 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Channel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseFieldID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserRole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabFieldDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldShowCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabShowCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DisplayContextParameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventToFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique ID for the event. Not listing an case event means that All Fields are displayed. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This defines with Fields can be changed / viewed during an case event. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The order of the fields on the screen.
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>TabID</t>
+  </si>
+  <si>
+    <t>TabLabel</t>
+  </si>
+  <si>
+    <t>TabDisplayOrder</t>
+  </si>
+  <si>
+    <t>CaseFieldID</t>
+  </si>
+  <si>
+    <t>UserRole</t>
+  </si>
+  <si>
+    <t>TabFieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>FieldShowCondition</t>
+  </si>
+  <si>
+    <t>TabShowCondition</t>
+  </si>
+  <si>
+    <t>DisplayContextParameter</t>
+  </si>
+  <si>
+    <t>CaseEventToFields</t>
+  </si>
+  <si>
+    <t>Unique ID for the event. Not listing an case event means that All Fields are displayed. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>This defines with Fields can be changed / viewed during an case event. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>The order of the fields on the screen.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted Values:  for mandatory, readonly and optional data on UI
+    <t>Accepted Values:  for mandatory, readonly and optional data on UI
 MustBe: MANDATORY, READONLY, OPTIONAL</t>
   </si>
   <si>
-    <t xml:space="preserve">This is a string value which defines the Wizard pages' ID
+    <t>This is a string value which defines the Wizard pages' ID
 MaxLength:40</t>
   </si>
   <si>
-    <t xml:space="preserve">This is a string value which defines the Wizard pages' Label
+    <t>This is a string value which defines the Wizard pages' Label
 MaxLength:40</t>
   </si>
   <si>
-    <t xml:space="preserve">The order to display the pages
+    <t>The order to display the pages
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Currently blank 1 or 2.  2 currently will display the yellow review column.
+    <t>Currently blank 1 or 2.  2 currently will display the yellow review column.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
+    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
 MaxLength: 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean expression rules for hiding a page: MaxLength:1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">States a field should appear on check your answers However these fields will be considered only "ShowSummary" column in CaseEvent tab is set to Y
+    <t>Boolean expression rules for hiding a page: MaxLength:1000</t>
+  </si>
+  <si>
+    <t>States a field should appear on check your answers However these fields will be considered only "ShowSummary" column in CaseEvent tab is set to Y
 CouldBe: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">URL to call back to the service for uniqueness. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a string value overrides label from CaseField tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a string value overrides hint from CaseField tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageFieldDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DisplayContext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageColumnNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageShowCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowSummaryChangeOption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowSummaryContentOption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLMidEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLMidEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventFieldLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventFieldHint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventToComplexTypes</t>
+    <t>URL to call back to the service for uniqueness. </t>
+  </si>
+  <si>
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). </t>
+  </si>
+  <si>
+    <t>This is a string value overrides label from CaseField tab</t>
+  </si>
+  <si>
+    <t>This is a string value overrides hint from CaseField tab</t>
+  </si>
+  <si>
+    <t>CaseEventID</t>
+  </si>
+  <si>
+    <t>PageFieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>DisplayContext</t>
+  </si>
+  <si>
+    <t>PageID</t>
+  </si>
+  <si>
+    <t>PageLabel</t>
+  </si>
+  <si>
+    <t>PageDisplayOrder</t>
+  </si>
+  <si>
+    <t>PageColumnNumber</t>
+  </si>
+  <si>
+    <t>PageShowCondition</t>
+  </si>
+  <si>
+    <t>ShowSummaryChangeOption</t>
+  </si>
+  <si>
+    <t>ShowSummaryContentOption</t>
+  </si>
+  <si>
+    <t>CallBackURLMidEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLMidEvent</t>
+  </si>
+  <si>
+    <t>CaseEventFieldLabel</t>
+  </si>
+  <si>
+    <t>CaseEventFieldHint</t>
+  </si>
+  <si>
+    <t>EventToComplexTypes</t>
   </si>
   <si>
     <t xml:space="preserve">
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">MaxLength:70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength:200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength:300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ListElementCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventElementLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventHintText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State with ID '*' and Name 'DEFAULT' is a reserved state. The state can be used for events where states do not change.
+    <t>MaxLength:70</t>
+  </si>
+  <si>
+    <t>MaxLength:200</t>
+  </si>
+  <si>
+    <t>MaxLength:300</t>
+  </si>
+  <si>
+    <t>ListElementCode</t>
+  </si>
+  <si>
+    <t>EventElementLabel</t>
+  </si>
+  <si>
+    <t>EventHintText</t>
+  </si>
+  <si>
+    <t>FieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>State with ID '*' and Name 'DEFAULT' is a reserved state. The state can be used for events where states do not change.
 MaxLength:70</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the name of the state as displayed on UI
+    <t>This is the name of the state as displayed on UI
 MaxLength:100</t>
   </si>
   <si>
-    <t xml:space="preserve">This gives longer decription of the case state
+    <t>This gives longer decription of the case state
 Max Length: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">The order of the states on the screen.
+    <t>The order of the states on the screen.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Optional override of title used in the CaseTabView. Markdown , concat supported
+    <t>Optional override of title used in the CaseTabView. Markdown , concat supported
 MaxLength: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">DisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TitleDisplay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique ID for the event
+    <t>DisplayOrder</t>
+  </si>
+  <si>
+    <t>TitleDisplay</t>
+  </si>
+  <si>
+    <t>CaseEvent</t>
+  </si>
+  <si>
+    <t>Unique ID for the event
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the name of the event as displayed on UI Dropdown list - hence limited to 30
+    <t>This is the name of the event as displayed on UI Dropdown list - hence limited to 30
 MaxLength: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">This gives further details of an event of a case
+    <t>This gives further details of an event of a case
 MaxLength:100</t>
   </si>
   <si>
-    <t xml:space="preserve">The display order of displaying the events in the list
+    <t>The display order of displaying the events in the list
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Future Elements not for MVP (what about multiple state) (semicolon ; seprated list).
+    <t>Future Elements not for MVP (what about multiple state) (semicolon ; seprated list).
 If '*' is provided, then precondition will not be validated and will be considered as current state
  MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Future Elements not for MVP. 
+    <t>Future Elements not for MVP. 
 If '*' is provided, then the current state will not change and will be same as pre condition state
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">URL to call back to the service for uniqueness. 
+    <t>URL to call back to the service for uniqueness. 
 Max Length: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). 
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). 
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Y, N and empty. TheCheck your answer section will be shown on Y (true) and empty(null) values, but not shown on N (false) values. Fields on CaseEventTo Field tab have Y in "ShowSummaryChangeOption" column.
+    <t>Y, N and empty. TheCheck your answer section will be shown on Y (true) and empty(null) values, but not shown on N (false) values. Fields on CaseEventTo Field tab have Y in "ShowSummaryChangeOption" column.
 CouldBe: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean value to say if the enter summary and event description fields are to be shown
+    <t>Boolean value to say if the enter summary and event description fields are to be shown
 CouldBeh: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean value to say if a draft of a create event can be saved
+    <t>Boolean value to say if a draft of a create event can be saved
 CouldBe: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The label of the button on the final event screen - default is Submit
+    <t>The label of the button on the final event screen - default is Submit
 MaxLength: 200</t>
   </si>
   <si>
-    <t xml:space="preserve">PreConditionState(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PostConditionState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLAboutToStartEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutAboutToStartEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLAboutToSubmitEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLAboutToSubmitEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLSubmittedEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLSubmittedEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowSummary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowEventNotes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CanSaveDraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndButtonLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FixedLists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The unique identifier of the Fixed list
+    <t>PreConditionState(s)</t>
+  </si>
+  <si>
+    <t>PostConditionState</t>
+  </si>
+  <si>
+    <t>CallBackURLAboutToStartEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutAboutToStartEvent</t>
+  </si>
+  <si>
+    <t>CallBackURLAboutToSubmitEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLAboutToSubmitEvent</t>
+  </si>
+  <si>
+    <t>CallBackURLSubmittedEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLSubmittedEvent</t>
+  </si>
+  <si>
+    <t>ShowSummary</t>
+  </si>
+  <si>
+    <t>ShowEventNotes</t>
+  </si>
+  <si>
+    <t>CanSaveDraft</t>
+  </si>
+  <si>
+    <t>EndButtonLabel</t>
+  </si>
+  <si>
+    <t>FixedLists</t>
+  </si>
+  <si>
+    <t>The unique identifier of the Fixed list
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">The unque ID of an element in the list (ID)
+    <t>The unque ID of an element in the list (ID)
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">The Display name for the list item
+    <t>The Display name for the list item
 MaxLength: 250</t>
   </si>
   <si>
-    <t xml:space="preserve">The display order of list items. Positive integers e.g 1, 2, 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ListElement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ComplexTypes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The ComplexType ID should match the field attribute name on the CaseField Tab
+    <t>The display order of list items. Positive integers e.g 1, 2, 3</t>
+  </si>
+  <si>
+    <t>ListElement</t>
+  </si>
+  <si>
+    <t>ComplexTypes</t>
+  </si>
+  <si>
+    <t>The ComplexType ID should match the field attribute name on the CaseField Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The complex type element (field) ID (ListElementId) should match the field attribute name used by the service team in creating the case
+    <t>The complex type element (field) ID (ListElementId) should match the field attribute name used by the service team in creating the case
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
+    <t>The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
 MaxLength:200</t>
   </si>
   <si>
-    <t xml:space="preserve">Within a complex type any field can be hidden or shown based on another field's values in the same level.
+    <t>Within a complex type any field can be hidden or shown based on another field's values in the same level.
 Currently only single boolean or string conditions are supported. Eg: country="Italy" or country startWith: "Uni"
 MaxLength: 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">The hint text that is present for each field type
+    <t>The hint text that is present for each field type
 MaxLength: &lt;unlmited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">ElementLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchInputFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fields that can be searched on. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label next to search field on UI.
+    <t>ElementLabel</t>
+  </si>
+  <si>
+    <t>SearchInputFields</t>
+  </si>
+  <si>
+    <t>Fields that can be searched on. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Label next to search field on UI.
 MaxLength: 200</t>
   </si>
   <si>
-    <t xml:space="preserve">Order of fields on UI 
+    <t>Order of fields on UI 
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">SearchAlias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique alias id for a case field of a case type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is just the CaseField ID for top level fields, or object notation pointing to a complex type field e.g. applicantAddress.AddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchAliasID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchResultFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fields to be displayed in results list. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name on the results column.for the field
+    <t>SearchAlias</t>
+  </si>
+  <si>
+    <t>Unique alias id for a case field of a case type</t>
+  </si>
+  <si>
+    <t>This is just the CaseField ID for top level fields, or object notation pointing to a complex type field e.g. applicantAddress.AddressLine1</t>
+  </si>
+  <si>
+    <t>SearchAliasID</t>
+  </si>
+  <si>
+    <t>SearchResultFields</t>
+  </si>
+  <si>
+    <t>Fields to be displayed in results list. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Name on the results column.for the field
 MaxLength: 200</t>
   </si>
   <si>
-    <t xml:space="preserve">Order the columns are displayed.
+    <t>Order the columns are displayed.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">WorkBasketResultFields</t>
+    <t>WorkBasketResultFields</t>
   </si>
   <si>
     <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
   </si>
   <si>
-    <t xml:space="preserve">WorkBasketInputFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserProfile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID from Jurisdiction Tab
+    <t>WorkBasketInputFields</t>
+  </si>
+  <si>
+    <t>UserProfile</t>
+  </si>
+  <si>
+    <t>Must match ID from Jurisdiction Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID from CaseType Tab
+    <t>Must match ID from CaseType Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID from State Tab
+    <t>Must match ID from State Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">UserIDAMId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketDefaultJurisdiction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketDefaultCaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketDefaultState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthorisationCaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID in 'CaseType' tab
+    <t>UserIDAMId</t>
+  </si>
+  <si>
+    <t>WorkBasketDefaultJurisdiction</t>
+  </si>
+  <si>
+    <t>WorkBasketDefaultCaseType</t>
+  </si>
+  <si>
+    <t>WorkBasketDefaultState</t>
+  </si>
+  <si>
+    <t>AuthorisationCaseType</t>
+  </si>
+  <si>
+    <t>Must match ID in 'CaseType' tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID role.  If a role doesn’t have a Row below that mean no access to.
+    <t>Must match ID role.  If a role doesn’t have a Row below that mean no access to.
 MaxLength: 100.</t>
   </si>
   <si>
-    <t xml:space="preserve">C - Create, R - Read, U - Update, D - Delete
+    <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">CRUD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthorisationCaseField</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID on 'CaseType' tab
+    <t>CRUD</t>
+  </si>
+  <si>
+    <t>AuthorisationCaseField</t>
+  </si>
+  <si>
+    <t>Must match ID on 'CaseType' tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID on CaseField tab.
+    <t>Must match ID on CaseField tab.
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">AuthorisationCaseEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID on Event tabe.
+    <t>AuthorisationCaseEvent</t>
+  </si>
+  <si>
+    <t>Must match ID on Event tabe.
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">AuthorisationCaseState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Muust match an ID on State tab.
+    <t>AuthorisationCaseState</t>
+  </si>
+  <si>
+    <t>Muust match an ID on State tab.
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">CaseStateID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthorisationComplexType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Field ID should match an ID in the CaseField Tab
+    <t>CaseStateID</t>
+  </si>
+  <si>
+    <t>AuthorisationComplexType</t>
+  </si>
+  <si>
+    <t>The Field ID should match an ID in the CaseField Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">C - Create, R - Read, U - Update, D - Delete
+    <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
+  </si>
+  <si>
+    <t>ResultsOrdering</t>
+  </si>
+  <si>
+    <t>Fields can be ordered on by user role</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY;@"/>
-    <numFmt numFmtId="166" formatCode="@"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -713,22 +722,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -762,14 +756,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -777,14 +771,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -792,7 +786,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -800,7 +794,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -815,7 +809,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFFC000"/>
       <name val="Arial"/>
@@ -823,7 +817,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFF6600"/>
       <name val="Arial"/>
@@ -831,7 +825,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF984807"/>
       <name val="Arial"/>
@@ -839,7 +833,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -867,7 +861,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFC000"/>
       <name val="Calibri"/>
@@ -875,7 +869,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
@@ -906,349 +900,145 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="72">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1307,29 +1097,337 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1344,7 +1442,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1361,7 +1459,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1379,34 +1477,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>139</v>
       </c>
@@ -1421,7 +1511,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1441,7 +1531,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1462,34 +1552,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>145</v>
       </c>
@@ -1512,7 +1594,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="409.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1553,7 +1635,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1595,34 +1677,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>152</v>
       </c>
@@ -1638,7 +1712,7 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
     </row>
-    <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1658,7 +1732,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -1679,36 +1753,28 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.49"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>156</v>
       </c>
@@ -1722,7 +1788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
         <v>157</v>
@@ -1734,7 +1800,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="48" t="s">
         <v>17</v>
       </c>
@@ -1749,34 +1815,26 @@
       <c r="F3" s="10"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>160</v>
       </c>
@@ -1792,7 +1850,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1812,7 +1870,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -1833,36 +1891,32 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>164</v>
       </c>
@@ -1880,7 +1934,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="49"/>
     </row>
-    <row r="2" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" ht="141" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1905,8 +1959,11 @@
       <c r="H2" s="50" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I2" s="50" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -1931,36 +1988,31 @@
       <c r="H3" s="52" t="s">
         <v>62</v>
       </c>
+      <c r="I3" s="52" t="s">
+        <v>191</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>166</v>
       </c>
@@ -1976,7 +2028,7 @@
       <c r="E1" s="56"/>
       <c r="F1" s="56"/>
     </row>
-    <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1996,7 +2048,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -2017,34 +2069,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>167</v>
       </c>
@@ -2060,7 +2104,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2078,7 +2122,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -2099,34 +2143,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>175</v>
       </c>
@@ -2141,7 +2177,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2158,7 +2194,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -2176,34 +2212,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="57" t="s">
         <v>180</v>
       </c>
@@ -2219,7 +2247,7 @@
       <c r="E1" s="58"/>
       <c r="F1" s="58"/>
     </row>
-    <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2239,7 +2267,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>9</v>
       </c>
@@ -2260,37 +2288,29 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.49"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>14</v>
       </c>
@@ -2304,7 +2324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>15</v>
       </c>
@@ -2324,11 +2344,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -2345,34 +2365,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>183</v>
       </c>
@@ -2388,7 +2400,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2408,7 +2420,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -2429,34 +2441,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>185</v>
       </c>
@@ -2472,7 +2476,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2492,7 +2496,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -2513,33 +2517,25 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.5"/>
+    <col min="1" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
         <v>188</v>
       </c>
@@ -2556,7 +2552,7 @@
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
     </row>
-    <row r="2" customFormat="false" ht="253" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" ht="253" x14ac:dyDescent="0.2">
       <c r="A2" s="68"/>
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
@@ -2575,7 +2571,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="70" t="s">
         <v>9</v>
       </c>
@@ -2599,10 +2595,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
@@ -2610,23 +2605,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>18</v>
       </c>
@@ -2645,7 +2637,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="211" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" ht="211" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2674,7 +2666,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="43" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" ht="43" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -2704,34 +2696,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -2753,7 +2737,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="409.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2791,7 +2775,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12" ht="29" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -2830,37 +2814,29 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="11" width="10.5" customWidth="1"/>
+    <col min="12" max="12" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="14" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
@@ -2882,7 +2858,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="183" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13" ht="183" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2923,7 +2899,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -2965,38 +2941,30 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:T5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R4" activeCellId="0" sqref="R4"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="14" width="10.5" customWidth="1"/>
+    <col min="15" max="15" width="24.33203125" customWidth="1"/>
+    <col min="16" max="18" width="10.5" customWidth="1"/>
+    <col min="19" max="19" width="15.1640625" customWidth="1"/>
+    <col min="20" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>67</v>
       </c>
@@ -3021,7 +2989,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:20" ht="253" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3080,7 +3048,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -3140,47 +3108,38 @@
       </c>
       <c r="T3" s="10"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:X3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AMK3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="26" width="30.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="26" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="26" width="9.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="26" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="26" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="26" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="26" width="6.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="14" style="27" width="6.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="28" width="6.33"/>
+    <col min="1" max="1" width="19.5" style="25" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="26" customWidth="1"/>
+    <col min="5" max="6" width="30.1640625" style="26" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" style="26" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="26" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" style="26" customWidth="1"/>
+    <col min="11" max="11" width="16" style="26" customWidth="1"/>
+    <col min="12" max="13" width="6.33203125" style="26" customWidth="1"/>
+    <col min="14" max="1021" width="6.33203125" style="27" customWidth="1"/>
+    <col min="1022" max="1025" width="6.33203125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>97</v>
       </c>
@@ -3194,7 +3153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" s="37" customFormat="true" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:24" s="37" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
@@ -3242,7 +3201,7 @@
       <c r="W2" s="36"/>
       <c r="X2" s="36"/>
     </row>
-    <row r="3" s="27" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:24" s="27" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
@@ -3278,10 +3237,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
@@ -3289,23 +3247,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>106</v>
       </c>
@@ -3323,7 +3278,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="225" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="225" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3349,7 +3304,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -3376,34 +3331,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>114</v>
       </c>
@@ -3433,7 +3380,7 @@
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="333" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:20" ht="333" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3495,7 +3442,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:20" ht="57" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -3558,12 +3505,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding ResultsOrdering to WorkbasketResults Tab (#46)
* Adding ResultsOrdering to WorkbasketResults Tab
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,37 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harryh/DIV/ccd-definition-processor/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A976087-33D7-6E4C-96A7-1B3D8CC0F30B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Jurisdiction" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="CaseRoles" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="CaseType" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="CaseField" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="CaseTypeTab" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="CaseEventToFields" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="CaseEventToComplexTypes" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="State" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="CaseEvent" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="FixedLists" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="ComplexTypes" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="SearchInputFields" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="SearchAlias" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="SearchResultFields" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="WorkBasketResultFields" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="WorkBasketInputFields" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="UserProfile" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="AuthorisationCaseType" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="AuthorisationCaseField" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="AuthorisationCaseState" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="AuthorisationComplexType" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
+    <sheet name="CaseRoles" sheetId="2" r:id="rId2"/>
+    <sheet name="CaseType" sheetId="3" r:id="rId3"/>
+    <sheet name="CaseField" sheetId="4" r:id="rId4"/>
+    <sheet name="CaseTypeTab" sheetId="5" r:id="rId5"/>
+    <sheet name="CaseEventToFields" sheetId="6" r:id="rId6"/>
+    <sheet name="CaseEventToComplexTypes" sheetId="7" r:id="rId7"/>
+    <sheet name="State" sheetId="8" r:id="rId8"/>
+    <sheet name="CaseEvent" sheetId="9" r:id="rId9"/>
+    <sheet name="FixedLists" sheetId="10" r:id="rId10"/>
+    <sheet name="ComplexTypes" sheetId="11" r:id="rId11"/>
+    <sheet name="SearchInputFields" sheetId="12" r:id="rId12"/>
+    <sheet name="SearchAlias" sheetId="13" r:id="rId13"/>
+    <sheet name="SearchResultFields" sheetId="14" r:id="rId14"/>
+    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId15"/>
+    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId16"/>
+    <sheet name="UserProfile" sheetId="17" r:id="rId17"/>
+    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId18"/>
+    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId19"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId20"/>
+    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId21"/>
+    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId22"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -41,670 +46,674 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="191">
-  <si>
-    <t xml:space="preserve">Jurisdiction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrimaryKeyInRed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrimaryAndForeignKey Orange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ForeignKey Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start date from which the data will be valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End date until which the data will be valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The identifier which defines the casetype code
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="193">
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t>PrimaryKeyInRed</t>
+  </si>
+  <si>
+    <t>PrimaryAndForeignKey Orange</t>
+  </si>
+  <si>
+    <t>ForeignKey Brown</t>
+  </si>
+  <si>
+    <t>Start date from which the data will be valid</t>
+  </si>
+  <si>
+    <t>End date until which the data will be valid</t>
+  </si>
+  <si>
+    <t>The identifier which defines the casetype code
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The short description to describe the jurisdiction used on UI display
+    <t>The short description to describe the jurisdiction used on UI display
 MaxLength: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">The long description to describe the jurisdiction.
+    <t>The long description to describe the jurisdiction.
 MaxLength: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">LiveFrom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LiveTo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseRoles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength: 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength:128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The short description to describe the case type used on the UI.
+    <t>LiveFrom</t>
+  </si>
+  <si>
+    <t>LiveTo</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>CaseRoles</t>
+  </si>
+  <si>
+    <t>MaxLength: 40</t>
+  </si>
+  <si>
+    <t>MaxLength:128</t>
+  </si>
+  <si>
+    <t>CaseTypeID</t>
+  </si>
+  <si>
+    <t>CaseType</t>
+  </si>
+  <si>
+    <t>The short description to describe the case type used on the UI.
 MaxLength: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">The long description to decribe the case type.
+    <t>The long description to decribe the case type.
 MaxLength: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">The jurisdiction code should match the one defined in 'Jurisdiction' tab
+    <t>The jurisdiction code should match the one defined in 'Jurisdiction' tab
 MaxLength:70</t>
   </si>
   <si>
-    <t xml:space="preserve">The absolute URL to the microservice which lists the documents that the services wants to provide for print. 
+    <t>The absolute URL to the microservice which lists the documents that the services wants to provide for print. 
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). Max Length: 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It is a mandatory field which can define if the data classification of the field
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). Max Length: 20</t>
+  </si>
+  <si>
+    <t>It is a mandatory field which can define if the data classification of the field
 MustBe: &lt;Public, Private, Retricted&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">JurisdictionID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrintableDocumentsUrl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLPrintEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SecurityClassification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseField</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The code of casetype has to be defined in 'CaseType' tab
+    <t>JurisdictionID</t>
+  </si>
+  <si>
+    <t>PrintableDocumentsUrl</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLPrintEvent</t>
+  </si>
+  <si>
+    <t>SecurityClassification</t>
+  </si>
+  <si>
+    <t>CaseField</t>
+  </si>
+  <si>
+    <t>The code of casetype has to be defined in 'CaseType' tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The field ID should match the field attribute name used by the service team in creating the case
+    <t>The field ID should match the field attribute name used by the service team in creating the case
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
+    <t>The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
 MaxLength:&lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The hint text that is present for each field type
+    <t>The hint text that is present for each field type
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The type of field. This can be a CCD Base type (see confluence) or a ComplexType ID as per the ComplexType tab).  
+    <t>The type of field. This can be a CCD Base type (see confluence) or a ComplexType ID as per the ComplexType tab).  
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Some FieldTypes require or have an optional addition parameter that can be set (e.g. Collection - the parameter is the collecion of What FieldType ?, FixedList the parameter is the ID from the fixedList tab). See confluence for details
+    <t>Some FieldTypes require or have an optional addition parameter that can be set (e.g. Collection - the parameter is the collecion of What FieldType ?, FixedList the parameter is the ID from the fixedList tab). See confluence for details
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">The regex that can define the type of data accepted in the fields E.g: alphanumeric etc. This will override the regex, if defined internally for any type.
+    <t>The regex that can define the type of data accepted in the fields E.g: alphanumeric etc. This will override the regex, if defined internally for any type.
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The minimum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
+    <t>The minimum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The maximum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
+    <t>The maximum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HintText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldTypeParameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RegularExpression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseTypeTab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not used yet - maybe used for roletype type view later
+    <t>Label</t>
+  </si>
+  <si>
+    <t>HintText</t>
+  </si>
+  <si>
+    <t>FieldType</t>
+  </si>
+  <si>
+    <t>FieldTypeParameter</t>
+  </si>
+  <si>
+    <t>RegularExpression</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>CaseTypeTab</t>
+  </si>
+  <si>
+    <t>Not used yet - maybe used for roletype type view later
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">Unique Id for tab. MaxLength: 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name to be displayed on the tab
+    <t>Unique Id for tab. MaxLength: 40</t>
+  </si>
+  <si>
+    <t>Name to be displayed on the tab
 MaxLengh: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">Order of Tab on screen - left to right.
+    <t>Order of Tab on screen - left to right.
 PositiveInteger</t>
   </si>
   <si>
-    <t xml:space="preserve">Unique ID for field - must match an ID on the CaseField tab or be a metadata item. 
+    <t>Unique ID for field - must match an ID on the CaseField tab or be a metadata item. 
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order of Fields within a tab - top to bottom
+    <t>MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
+  </si>
+  <si>
+    <t>Order of Fields within a tab - top to bottom
 PositiveInteger</t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
+    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
 MaxLength:1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean expression rules for hiding a tab: 
+    <t>Boolean expression rules for hiding a tab: 
 MaxLength:1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Text should begin with #LIST( or #TABLE(
+    <t>Text should begin with #LIST( or #TABLE(
 MaxLength: 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Channel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseFieldID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserRole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabFieldDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldShowCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabShowCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DisplayContextParameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventToFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique ID for the event. Not listing an case event means that All Fields are displayed. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This defines with Fields can be changed / viewed during an case event. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The order of the fields on the screen.
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>TabID</t>
+  </si>
+  <si>
+    <t>TabLabel</t>
+  </si>
+  <si>
+    <t>TabDisplayOrder</t>
+  </si>
+  <si>
+    <t>CaseFieldID</t>
+  </si>
+  <si>
+    <t>UserRole</t>
+  </si>
+  <si>
+    <t>TabFieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>FieldShowCondition</t>
+  </si>
+  <si>
+    <t>TabShowCondition</t>
+  </si>
+  <si>
+    <t>DisplayContextParameter</t>
+  </si>
+  <si>
+    <t>CaseEventToFields</t>
+  </si>
+  <si>
+    <t>Unique ID for the event. Not listing an case event means that All Fields are displayed. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>This defines with Fields can be changed / viewed during an case event. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>The order of the fields on the screen.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted Values:  for mandatory, readonly and optional data on UI
+    <t>Accepted Values:  for mandatory, readonly and optional data on UI
 MustBe: MANDATORY, READONLY, OPTIONAL</t>
   </si>
   <si>
-    <t xml:space="preserve">This is a string value which defines the Wizard pages' ID
+    <t>This is a string value which defines the Wizard pages' ID
 MaxLength:40</t>
   </si>
   <si>
-    <t xml:space="preserve">This is a string value which defines the Wizard pages' Label
+    <t>This is a string value which defines the Wizard pages' Label
 MaxLength:40</t>
   </si>
   <si>
-    <t xml:space="preserve">The order to display the pages
+    <t>The order to display the pages
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Currently blank 1 or 2.  2 currently will display the yellow review column.
+    <t>Currently blank 1 or 2.  2 currently will display the yellow review column.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
+    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
 MaxLength: 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean expression rules for hiding a page: MaxLength:1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">States a field should appear on check your answers However these fields will be considered only "ShowSummary" column in CaseEvent tab is set to Y
+    <t>Boolean expression rules for hiding a page: MaxLength:1000</t>
+  </si>
+  <si>
+    <t>States a field should appear on check your answers However these fields will be considered only "ShowSummary" column in CaseEvent tab is set to Y
 CouldBe: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">URL to call back to the service for uniqueness. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a string value overrides label from CaseField tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a string value overrides hint from CaseField tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageFieldDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DisplayContext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageColumnNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageShowCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowSummaryChangeOption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowSummaryContentOption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLMidEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLMidEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventFieldLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventFieldHint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventToComplexTypes</t>
+    <t>URL to call back to the service for uniqueness. </t>
+  </si>
+  <si>
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). </t>
+  </si>
+  <si>
+    <t>This is a string value overrides label from CaseField tab</t>
+  </si>
+  <si>
+    <t>This is a string value overrides hint from CaseField tab</t>
+  </si>
+  <si>
+    <t>CaseEventID</t>
+  </si>
+  <si>
+    <t>PageFieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>DisplayContext</t>
+  </si>
+  <si>
+    <t>PageID</t>
+  </si>
+  <si>
+    <t>PageLabel</t>
+  </si>
+  <si>
+    <t>PageDisplayOrder</t>
+  </si>
+  <si>
+    <t>PageColumnNumber</t>
+  </si>
+  <si>
+    <t>PageShowCondition</t>
+  </si>
+  <si>
+    <t>ShowSummaryChangeOption</t>
+  </si>
+  <si>
+    <t>ShowSummaryContentOption</t>
+  </si>
+  <si>
+    <t>CallBackURLMidEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLMidEvent</t>
+  </si>
+  <si>
+    <t>CaseEventFieldLabel</t>
+  </si>
+  <si>
+    <t>CaseEventFieldHint</t>
+  </si>
+  <si>
+    <t>EventToComplexTypes</t>
   </si>
   <si>
     <t xml:space="preserve">
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">MaxLength:70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength:200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength:300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ListElementCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventElementLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventHintText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State with ID '*' and Name 'DEFAULT' is a reserved state. The state can be used for events where states do not change.
+    <t>MaxLength:70</t>
+  </si>
+  <si>
+    <t>MaxLength:200</t>
+  </si>
+  <si>
+    <t>MaxLength:300</t>
+  </si>
+  <si>
+    <t>ListElementCode</t>
+  </si>
+  <si>
+    <t>EventElementLabel</t>
+  </si>
+  <si>
+    <t>EventHintText</t>
+  </si>
+  <si>
+    <t>FieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>State with ID '*' and Name 'DEFAULT' is a reserved state. The state can be used for events where states do not change.
 MaxLength:70</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the name of the state as displayed on UI
+    <t>This is the name of the state as displayed on UI
 MaxLength:100</t>
   </si>
   <si>
-    <t xml:space="preserve">This gives longer decription of the case state
+    <t>This gives longer decription of the case state
 Max Length: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">The order of the states on the screen.
+    <t>The order of the states on the screen.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Optional override of title used in the CaseTabView. Markdown , concat supported
+    <t>Optional override of title used in the CaseTabView. Markdown , concat supported
 MaxLength: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">DisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TitleDisplay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique ID for the event
+    <t>DisplayOrder</t>
+  </si>
+  <si>
+    <t>TitleDisplay</t>
+  </si>
+  <si>
+    <t>CaseEvent</t>
+  </si>
+  <si>
+    <t>Unique ID for the event
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the name of the event as displayed on UI Dropdown list - hence limited to 30
+    <t>This is the name of the event as displayed on UI Dropdown list - hence limited to 30
 MaxLength: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">This gives further details of an event of a case
+    <t>This gives further details of an event of a case
 MaxLength:100</t>
   </si>
   <si>
-    <t xml:space="preserve">The display order of displaying the events in the list
+    <t>The display order of displaying the events in the list
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Future Elements not for MVP (what about multiple state) (semicolon ; seprated list).
+    <t>Future Elements not for MVP (what about multiple state) (semicolon ; seprated list).
 If '*' is provided, then precondition will not be validated and will be considered as current state
  MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Future Elements not for MVP. 
+    <t>Future Elements not for MVP. 
 If '*' is provided, then the current state will not change and will be same as pre condition state
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">URL to call back to the service for uniqueness. 
+    <t>URL to call back to the service for uniqueness. 
 Max Length: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). 
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). 
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Y, N and empty. TheCheck your answer section will be shown on Y (true) and empty(null) values, but not shown on N (false) values. Fields on CaseEventTo Field tab have Y in "ShowSummaryChangeOption" column.
+    <t>Y, N and empty. TheCheck your answer section will be shown on Y (true) and empty(null) values, but not shown on N (false) values. Fields on CaseEventTo Field tab have Y in "ShowSummaryChangeOption" column.
 CouldBe: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean value to say if the enter summary and event description fields are to be shown
+    <t>Boolean value to say if the enter summary and event description fields are to be shown
 CouldBeh: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean value to say if a draft of a create event can be saved
+    <t>Boolean value to say if a draft of a create event can be saved
 CouldBe: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The label of the button on the final event screen - default is Submit
+    <t>The label of the button on the final event screen - default is Submit
 MaxLength: 200</t>
   </si>
   <si>
-    <t xml:space="preserve">PreConditionState(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PostConditionState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLAboutToStartEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutAboutToStartEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLAboutToSubmitEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLAboutToSubmitEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLSubmittedEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLSubmittedEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowSummary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowEventNotes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CanSaveDraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndButtonLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FixedLists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The unique identifier of the Fixed list
+    <t>PreConditionState(s)</t>
+  </si>
+  <si>
+    <t>PostConditionState</t>
+  </si>
+  <si>
+    <t>CallBackURLAboutToStartEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutAboutToStartEvent</t>
+  </si>
+  <si>
+    <t>CallBackURLAboutToSubmitEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLAboutToSubmitEvent</t>
+  </si>
+  <si>
+    <t>CallBackURLSubmittedEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLSubmittedEvent</t>
+  </si>
+  <si>
+    <t>ShowSummary</t>
+  </si>
+  <si>
+    <t>ShowEventNotes</t>
+  </si>
+  <si>
+    <t>CanSaveDraft</t>
+  </si>
+  <si>
+    <t>EndButtonLabel</t>
+  </si>
+  <si>
+    <t>FixedLists</t>
+  </si>
+  <si>
+    <t>The unique identifier of the Fixed list
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">The unque ID of an element in the list (ID)
+    <t>The unque ID of an element in the list (ID)
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">The Display name for the list item
+    <t>The Display name for the list item
 MaxLength: 250</t>
   </si>
   <si>
-    <t xml:space="preserve">The display order of list items. Positive integers e.g 1, 2, 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ListElement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ComplexTypes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The ComplexType ID should match the field attribute name on the CaseField Tab
+    <t>The display order of list items. Positive integers e.g 1, 2, 3</t>
+  </si>
+  <si>
+    <t>ListElement</t>
+  </si>
+  <si>
+    <t>ComplexTypes</t>
+  </si>
+  <si>
+    <t>The ComplexType ID should match the field attribute name on the CaseField Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The complex type element (field) ID (ListElementId) should match the field attribute name used by the service team in creating the case
+    <t>The complex type element (field) ID (ListElementId) should match the field attribute name used by the service team in creating the case
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
+    <t>The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
 MaxLength:200</t>
   </si>
   <si>
-    <t xml:space="preserve">Within a complex type any field can be hidden or shown based on another field's values in the same level.
+    <t>Within a complex type any field can be hidden or shown based on another field's values in the same level.
 Currently only single boolean or string conditions are supported. Eg: country="Italy" or country startWith: "Uni"
 MaxLength: 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">The hint text that is present for each field type
+    <t>The hint text that is present for each field type
 MaxLength: &lt;unlmited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">ElementLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchInputFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fields that can be searched on. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label next to search field on UI.
+    <t>ElementLabel</t>
+  </si>
+  <si>
+    <t>SearchInputFields</t>
+  </si>
+  <si>
+    <t>Fields that can be searched on. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Label next to search field on UI.
 MaxLength: 200</t>
   </si>
   <si>
-    <t xml:space="preserve">Order of fields on UI 
+    <t>Order of fields on UI 
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">SearchAlias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique alias id for a case field of a case type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is just the CaseField ID for top level fields, or object notation pointing to a complex type field e.g. applicantAddress.AddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchAliasID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchResultFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fields to be displayed in results list. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name on the results column.for the field
+    <t>SearchAlias</t>
+  </si>
+  <si>
+    <t>Unique alias id for a case field of a case type</t>
+  </si>
+  <si>
+    <t>This is just the CaseField ID for top level fields, or object notation pointing to a complex type field e.g. applicantAddress.AddressLine1</t>
+  </si>
+  <si>
+    <t>SearchAliasID</t>
+  </si>
+  <si>
+    <t>SearchResultFields</t>
+  </si>
+  <si>
+    <t>Fields to be displayed in results list. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Name on the results column.for the field
 MaxLength: 200</t>
   </si>
   <si>
-    <t xml:space="preserve">Order the columns are displayed.
+    <t>Order the columns are displayed.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">WorkBasketResultFields</t>
+    <t>WorkBasketResultFields</t>
   </si>
   <si>
     <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
   </si>
   <si>
-    <t xml:space="preserve">WorkBasketInputFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserProfile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID from Jurisdiction Tab
+    <t>WorkBasketInputFields</t>
+  </si>
+  <si>
+    <t>UserProfile</t>
+  </si>
+  <si>
+    <t>Must match ID from Jurisdiction Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID from CaseType Tab
+    <t>Must match ID from CaseType Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID from State Tab
+    <t>Must match ID from State Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">UserIDAMId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketDefaultJurisdiction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketDefaultCaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketDefaultState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthorisationCaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID in 'CaseType' tab
+    <t>UserIDAMId</t>
+  </si>
+  <si>
+    <t>WorkBasketDefaultJurisdiction</t>
+  </si>
+  <si>
+    <t>WorkBasketDefaultCaseType</t>
+  </si>
+  <si>
+    <t>WorkBasketDefaultState</t>
+  </si>
+  <si>
+    <t>AuthorisationCaseType</t>
+  </si>
+  <si>
+    <t>Must match ID in 'CaseType' tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID role.  If a role doesn’t have a Row below that mean no access to.
+    <t>Must match ID role.  If a role doesn’t have a Row below that mean no access to.
 MaxLength: 100.</t>
   </si>
   <si>
-    <t xml:space="preserve">C - Create, R - Read, U - Update, D - Delete
+    <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">CRUD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthorisationCaseField</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID on 'CaseType' tab
+    <t>CRUD</t>
+  </si>
+  <si>
+    <t>AuthorisationCaseField</t>
+  </si>
+  <si>
+    <t>Must match ID on 'CaseType' tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID on CaseField tab.
+    <t>Must match ID on CaseField tab.
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">AuthorisationCaseEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID on Event tabe.
+    <t>AuthorisationCaseEvent</t>
+  </si>
+  <si>
+    <t>Must match ID on Event tabe.
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">AuthorisationCaseState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Muust match an ID on State tab.
+    <t>AuthorisationCaseState</t>
+  </si>
+  <si>
+    <t>Muust match an ID on State tab.
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">CaseStateID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthorisationComplexType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Field ID should match an ID in the CaseField Tab
+    <t>CaseStateID</t>
+  </si>
+  <si>
+    <t>AuthorisationComplexType</t>
+  </si>
+  <si>
+    <t>The Field ID should match an ID in the CaseField Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">C - Create, R - Read, U - Update, D - Delete
+    <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
+  </si>
+  <si>
+    <t>ResultsOrdering</t>
+  </si>
+  <si>
+    <t>Fields can be ordered on by user role</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY;@"/>
-    <numFmt numFmtId="166" formatCode="@"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -713,22 +722,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -762,14 +756,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -777,14 +771,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -792,7 +786,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -800,7 +794,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -815,7 +809,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFFC000"/>
       <name val="Arial"/>
@@ -823,7 +817,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFF6600"/>
       <name val="Arial"/>
@@ -831,7 +825,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF984807"/>
       <name val="Arial"/>
@@ -839,7 +833,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -867,7 +861,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFC000"/>
       <name val="Calibri"/>
@@ -875,7 +869,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
@@ -906,349 +900,145 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="72">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1307,29 +1097,337 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1344,7 +1442,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1361,7 +1459,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1379,34 +1477,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>139</v>
       </c>
@@ -1421,7 +1511,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1441,7 +1531,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1462,34 +1552,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>145</v>
       </c>
@@ -1512,7 +1594,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="409.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1553,7 +1635,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1595,34 +1677,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>152</v>
       </c>
@@ -1638,7 +1712,7 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
     </row>
-    <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1658,7 +1732,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -1679,36 +1753,28 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.49"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>156</v>
       </c>
@@ -1722,7 +1788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
         <v>157</v>
@@ -1734,7 +1800,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="48" t="s">
         <v>17</v>
       </c>
@@ -1749,34 +1815,26 @@
       <c r="F3" s="10"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>160</v>
       </c>
@@ -1792,7 +1850,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1812,7 +1870,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -1833,36 +1891,32 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>164</v>
       </c>
@@ -1880,7 +1934,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="49"/>
     </row>
-    <row r="2" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" ht="141" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1905,8 +1959,11 @@
       <c r="H2" s="50" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I2" s="50" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -1931,36 +1988,31 @@
       <c r="H3" s="52" t="s">
         <v>62</v>
       </c>
+      <c r="I3" s="52" t="s">
+        <v>191</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>166</v>
       </c>
@@ -1976,7 +2028,7 @@
       <c r="E1" s="56"/>
       <c r="F1" s="56"/>
     </row>
-    <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1996,7 +2048,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -2017,34 +2069,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>167</v>
       </c>
@@ -2060,7 +2104,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2078,7 +2122,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -2099,34 +2143,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>175</v>
       </c>
@@ -2141,7 +2177,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2158,7 +2194,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -2176,34 +2212,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="57" t="s">
         <v>180</v>
       </c>
@@ -2219,7 +2247,7 @@
       <c r="E1" s="58"/>
       <c r="F1" s="58"/>
     </row>
-    <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2239,7 +2267,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>9</v>
       </c>
@@ -2260,37 +2288,29 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.49"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>14</v>
       </c>
@@ -2304,7 +2324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>15</v>
       </c>
@@ -2324,11 +2344,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -2345,34 +2365,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>183</v>
       </c>
@@ -2388,7 +2400,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2408,7 +2420,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -2429,34 +2441,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>185</v>
       </c>
@@ -2472,7 +2476,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2492,7 +2496,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -2513,33 +2517,25 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.5"/>
+    <col min="1" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
         <v>188</v>
       </c>
@@ -2556,7 +2552,7 @@
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
     </row>
-    <row r="2" customFormat="false" ht="253" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" ht="253" x14ac:dyDescent="0.2">
       <c r="A2" s="68"/>
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
@@ -2575,7 +2571,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="70" t="s">
         <v>9</v>
       </c>
@@ -2599,10 +2595,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
@@ -2610,23 +2605,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>18</v>
       </c>
@@ -2645,7 +2637,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="211" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" ht="211" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2674,7 +2666,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="43" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" ht="43" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -2704,34 +2696,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -2753,7 +2737,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="409.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2791,7 +2775,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12" ht="29" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -2830,37 +2814,29 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="11" width="10.5" customWidth="1"/>
+    <col min="12" max="12" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="14" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
@@ -2882,7 +2858,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="183" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13" ht="183" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2923,7 +2899,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -2965,38 +2941,30 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:T5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R4" activeCellId="0" sqref="R4"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="14" width="10.5" customWidth="1"/>
+    <col min="15" max="15" width="24.33203125" customWidth="1"/>
+    <col min="16" max="18" width="10.5" customWidth="1"/>
+    <col min="19" max="19" width="15.1640625" customWidth="1"/>
+    <col min="20" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>67</v>
       </c>
@@ -3021,7 +2989,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:20" ht="253" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3080,7 +3048,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -3140,47 +3108,38 @@
       </c>
       <c r="T3" s="10"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:X3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AMK3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="26" width="30.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="26" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="26" width="9.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="26" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="26" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="26" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="26" width="6.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="14" style="27" width="6.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="28" width="6.33"/>
+    <col min="1" max="1" width="19.5" style="25" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="26" customWidth="1"/>
+    <col min="5" max="6" width="30.1640625" style="26" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" style="26" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="26" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" style="26" customWidth="1"/>
+    <col min="11" max="11" width="16" style="26" customWidth="1"/>
+    <col min="12" max="13" width="6.33203125" style="26" customWidth="1"/>
+    <col min="14" max="1021" width="6.33203125" style="27" customWidth="1"/>
+    <col min="1022" max="1025" width="6.33203125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>97</v>
       </c>
@@ -3194,7 +3153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" s="37" customFormat="true" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:24" s="37" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
@@ -3242,7 +3201,7 @@
       <c r="W2" s="36"/>
       <c r="X2" s="36"/>
     </row>
-    <row r="3" s="27" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:24" s="27" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
@@ -3278,10 +3237,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
@@ -3289,23 +3247,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>106</v>
       </c>
@@ -3323,7 +3278,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="225" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="225" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3349,7 +3304,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -3376,34 +3331,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>114</v>
       </c>
@@ -3433,7 +3380,7 @@
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="333" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:20" ht="333" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3495,7 +3442,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:20" ht="57" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -3558,12 +3505,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add jurisdiction in shutter
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harryh/DIV/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharmendrak/development/moj/ccd/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A976087-33D7-6E4C-96A7-1B3D8CC0F30B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3B4AB7-FB6E-DE41-BB73-DD2B2EBDBE15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="194">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -703,6 +703,9 @@
   </si>
   <si>
     <t>Fields can be ordered on by user role</t>
+  </si>
+  <si>
+    <t>Shuttered</t>
   </si>
 </sst>
 </file>
@@ -1415,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1427,7 +1430,7 @@
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1442,7 +1445,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1459,7 +1462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1474,6 +1477,9 @@
       </c>
       <c r="E3" s="10" t="s">
         <v>13</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -1900,7 +1906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add shuttered column in jurisdiction tab (#71)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harryh/DIV/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharmendrak/development/moj/ccd/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A976087-33D7-6E4C-96A7-1B3D8CC0F30B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A51E89-01FA-3346-AC12-2A585C6CE95C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId21"/>
     <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId22"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="195">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -703,6 +703,12 @@
   </si>
   <si>
     <t>Fields can be ordered on by user role</t>
+  </si>
+  <si>
+    <t>Shuttered</t>
+  </si>
+  <si>
+    <t>This can have value TRUE/FALSE</t>
   </si>
 </sst>
 </file>
@@ -1415,10 +1421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1427,7 +1433,7 @@
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1442,7 +1448,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1458,8 +1464,11 @@
       <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1474,6 +1483,9 @@
       </c>
       <c r="E3" s="10" t="s">
         <v>13</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -1900,7 +1912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ResultsOrdering field added to SearchResultFields.json and updated template with new columns under SearchResultFields tab
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharmendrak/development/moj/ccd/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikhilkkainos.com/Fpla-code/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A51E89-01FA-3346-AC12-2A585C6CE95C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57947AE-2CBB-4345-8D2C-BBBB616A48C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="195">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1423,7 +1423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1834,10 +1834,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1846,7 +1846,7 @@
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>160</v>
       </c>
@@ -1862,7 +1862,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="141" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1881,8 +1881,14 @@
       <c r="F2" s="8" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="50" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -1900,6 +1906,12 @@
       </c>
       <c r="F3" s="10" t="s">
         <v>112</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -1913,7 +1925,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="H2" sqref="H2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
ResultsOrdering field added to SearchResultFields.json and updated template with new columns under SearchResultFields tab (#77)
Co-authored-by: Nikhil Koranne <nikhilkkainos.com@Geona.local>
feat: add ResultsOrdering to SearchResultsField tab
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharmendrak/development/moj/ccd/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikhilkkainos.com/Fpla-code/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A51E89-01FA-3346-AC12-2A585C6CE95C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57947AE-2CBB-4345-8D2C-BBBB616A48C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="195">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1423,7 +1423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1834,10 +1834,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1846,7 +1846,7 @@
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>160</v>
       </c>
@@ -1862,7 +1862,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="141" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1881,8 +1881,14 @@
       <c r="F2" s="8" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="50" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -1900,6 +1906,12 @@
       </c>
       <c r="F3" s="10" t="s">
         <v>112</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -1913,7 +1925,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="H2" sqref="H2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add banner tab (#78)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikhilkkainos.com/Fpla-code/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharmendrak/development/moj/ccd/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57947AE-2CBB-4345-8D2C-BBBB616A48C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725172BC-9DD5-934F-8F01-D4FA534E3158}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -27,14 +27,15 @@
     <sheet name="SearchInputFields" sheetId="12" r:id="rId12"/>
     <sheet name="SearchAlias" sheetId="13" r:id="rId13"/>
     <sheet name="SearchResultFields" sheetId="14" r:id="rId14"/>
-    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId15"/>
-    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId16"/>
-    <sheet name="UserProfile" sheetId="17" r:id="rId17"/>
-    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId18"/>
-    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId19"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId20"/>
-    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId21"/>
-    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId22"/>
+    <sheet name="Banner" sheetId="23" r:id="rId15"/>
+    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId16"/>
+    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId17"/>
+    <sheet name="UserProfile" sheetId="17" r:id="rId18"/>
+    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId19"/>
+    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId20"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId21"/>
+    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId22"/>
+    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId23"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="204">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -709,6 +710,33 @@
   </si>
   <si>
     <t>This can have value TRUE/FALSE</t>
+  </si>
+  <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>Yes or No, to enable or disable the banner.                          MaxLength: 30</t>
+  </si>
+  <si>
+    <t>Content to display in the banner         MaxLength: 300</t>
+  </si>
+  <si>
+    <t>Optional link text in the banner                   MaxLength:50</t>
+  </si>
+  <si>
+    <t>The URL for the link text.                                               Max Length: 1000</t>
+  </si>
+  <si>
+    <t>BannerEnabled</t>
+  </si>
+  <si>
+    <t>BannerDescription</t>
+  </si>
+  <si>
+    <t>BannerUrlText</t>
+  </si>
+  <si>
+    <t>BannerUrl</t>
   </si>
 </sst>
 </file>
@@ -719,7 +747,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -896,16 +924,52 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF6A8759"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0563C1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -928,12 +992,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1038,9 +1142,21 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="26" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1836,7 +1952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -1921,6 +2037,111 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B87178-516D-C449-B2C2-346849889C36}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="72" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="74"/>
+    </row>
+    <row r="2" spans="1:4" ht="43" x14ac:dyDescent="0.2">
+      <c r="A2" s="75" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" s="75" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="75" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="76" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="76" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="76" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" s="76" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="79"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="80"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="80"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="80"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="80"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="80"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="80"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="80"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -2022,7 +2243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2098,7 +2319,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2172,7 +2393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2232,82 +2453,6 @@
         <v>62</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
-        <v>180</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-    </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="59" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="24" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2395,6 +2540,82 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="57" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+    </row>
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2470,7 +2691,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2546,7 +2767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Format the banner in template
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharmendrak/development/moj/ccd/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725172BC-9DD5-934F-8F01-D4FA534E3158}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066EEEE5-5613-8A42-9AB3-9C8E1B0E159E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -747,7 +747,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -924,52 +924,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF6A8759"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -992,52 +956,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1142,21 +1066,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2038,103 +1950,59 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B87178-516D-C449-B2C2-346849889C36}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.5" customWidth="1"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="72" t="s">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="74"/>
-    </row>
-    <row r="2" spans="1:4" ht="43" x14ac:dyDescent="0.2">
-      <c r="A2" s="75" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="D2" s="75" t="s">
+      <c r="D2" s="7" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="76" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="20" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="77"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="79"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="80"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="80"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="80"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="80"/>
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="80"/>
-      <c r="B9" s="80"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="80"/>
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="80"/>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2324,7 +2192,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Format the banner in template (#82)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharmendrak/development/moj/ccd/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725172BC-9DD5-934F-8F01-D4FA534E3158}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066EEEE5-5613-8A42-9AB3-9C8E1B0E159E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -747,7 +747,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -924,52 +924,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF6A8759"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0563C1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -992,52 +956,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1142,21 +1066,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2038,103 +1950,59 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B87178-516D-C449-B2C2-346849889C36}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.5" customWidth="1"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="72" t="s">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="74"/>
-    </row>
-    <row r="2" spans="1:4" ht="43" x14ac:dyDescent="0.2">
-      <c r="A2" s="75" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="D2" s="75" t="s">
+      <c r="D2" s="7" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="76" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="20" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="77"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="79"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="80"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="80"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="80"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="80"/>
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="80"/>
-      <c r="B9" s="80"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="80"/>
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="80"/>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2324,7 +2192,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Make banner tab disabled
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharmendrak/development/moj/ccd/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066EEEE5-5613-8A42-9AB3-9C8E1B0E159E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB18CFE-0E73-6A46-9C04-9D8963D1FFE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="206">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -737,6 +737,12 @@
   </si>
   <si>
     <t>BannerUrl</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Banner is not enabled</t>
   </si>
 </sst>
 </file>
@@ -1950,16 +1956,19 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B87178-516D-C449-B2C2-346849889C36}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -2003,6 +2012,14 @@
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>205</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
impr: add support for DefaultValue in CaseEventToComplexTypes
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharmendrak/development/moj/ccd/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamko/Work/FPLA/code/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066EEEE5-5613-8A42-9AB3-9C8E1B0E159E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959BF888-43EE-FD49-A05E-D191EA996C1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="205">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -737,6 +737,9 @@
   </si>
   <si>
     <t>BannerUrl</t>
+  </si>
+  <si>
+    <t>DefaultValue</t>
   </si>
 </sst>
 </file>
@@ -1551,7 +1554,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="99" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1752,7 +1755,7 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1952,7 +1955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B87178-516D-C449-B2C2-346849889C36}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1972,7 +1975,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>196</v>
       </c>
@@ -2047,7 +2050,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="49"/>
     </row>
-    <row r="2" spans="1:9" ht="141" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="155" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2141,7 +2144,7 @@
       <c r="E1" s="56"/>
       <c r="F1" s="56"/>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2217,7 +2220,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="99" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2290,7 +2293,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="169" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2437,7 +2440,7 @@
       <c r="E1" s="58"/>
       <c r="F1" s="58"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="169" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2513,7 +2516,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="169" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2589,7 +2592,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="169" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3102,7 +3105,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="253" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="281" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3229,10 +3232,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AMK3"/>
+  <dimension ref="A1:AML3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3241,18 +3244,18 @@
     <col min="2" max="2" width="11.1640625" style="25" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" style="26" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" style="26" customWidth="1"/>
-    <col min="5" max="6" width="30.1640625" style="26" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" style="26" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="26" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="26" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" style="26" customWidth="1"/>
-    <col min="11" max="11" width="16" style="26" customWidth="1"/>
-    <col min="12" max="13" width="6.33203125" style="26" customWidth="1"/>
-    <col min="14" max="1021" width="6.33203125" style="27" customWidth="1"/>
-    <col min="1022" max="1025" width="6.33203125" style="28" customWidth="1"/>
+    <col min="5" max="7" width="30.1640625" style="26" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="26" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" style="26" customWidth="1"/>
+    <col min="12" max="12" width="16" style="26" customWidth="1"/>
+    <col min="13" max="14" width="6.33203125" style="26" customWidth="1"/>
+    <col min="15" max="1022" width="6.33203125" style="27" customWidth="1"/>
+    <col min="1023" max="1026" width="6.33203125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>97</v>
       </c>
@@ -3266,7 +3269,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="37" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" s="37" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
@@ -3285,22 +3288,22 @@
       <c r="F2" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="35"/>
+      <c r="H2" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="I2" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="J2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="K2" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="L2" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="L2" s="36"/>
       <c r="M2" s="36"/>
       <c r="N2" s="36"/>
       <c r="O2" s="36"/>
@@ -3313,8 +3316,9 @@
       <c r="V2" s="36"/>
       <c r="W2" s="36"/>
       <c r="X2" s="36"/>
-    </row>
-    <row r="3" spans="1:24" s="27" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Y2" s="36"/>
+    </row>
+    <row r="3" spans="1:25" s="27" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
@@ -3333,19 +3337,22 @@
       <c r="F3" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="71" t="s">
+        <v>204</v>
+      </c>
+      <c r="H3" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="I3" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="J3" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="J3" s="40" t="s">
+      <c r="K3" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="L3" s="41" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3493,7 +3500,7 @@
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="333" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="359" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
impr: add support for DefaultValue in CaseEventToComplexTypes (#107)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharmendrak/development/moj/ccd/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamko/Work/FPLA/code/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066EEEE5-5613-8A42-9AB3-9C8E1B0E159E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959BF888-43EE-FD49-A05E-D191EA996C1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="205">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -737,6 +737,9 @@
   </si>
   <si>
     <t>BannerUrl</t>
+  </si>
+  <si>
+    <t>DefaultValue</t>
   </si>
 </sst>
 </file>
@@ -1551,7 +1554,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="99" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1752,7 +1755,7 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1952,7 +1955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B87178-516D-C449-B2C2-346849889C36}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -1972,7 +1975,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>196</v>
       </c>
@@ -2047,7 +2050,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="49"/>
     </row>
-    <row r="2" spans="1:9" ht="141" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="155" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2141,7 +2144,7 @@
       <c r="E1" s="56"/>
       <c r="F1" s="56"/>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2217,7 +2220,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="99" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2290,7 +2293,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="169" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2437,7 +2440,7 @@
       <c r="E1" s="58"/>
       <c r="F1" s="58"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="169" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2513,7 +2516,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="169" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2589,7 +2592,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="169" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3102,7 +3105,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="253" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="281" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3229,10 +3232,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AMK3"/>
+  <dimension ref="A1:AML3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3241,18 +3244,18 @@
     <col min="2" max="2" width="11.1640625" style="25" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" style="26" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" style="26" customWidth="1"/>
-    <col min="5" max="6" width="30.1640625" style="26" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" style="26" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="26" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="26" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" style="26" customWidth="1"/>
-    <col min="11" max="11" width="16" style="26" customWidth="1"/>
-    <col min="12" max="13" width="6.33203125" style="26" customWidth="1"/>
-    <col min="14" max="1021" width="6.33203125" style="27" customWidth="1"/>
-    <col min="1022" max="1025" width="6.33203125" style="28" customWidth="1"/>
+    <col min="5" max="7" width="30.1640625" style="26" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="26" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" style="26" customWidth="1"/>
+    <col min="12" max="12" width="16" style="26" customWidth="1"/>
+    <col min="13" max="14" width="6.33203125" style="26" customWidth="1"/>
+    <col min="15" max="1022" width="6.33203125" style="27" customWidth="1"/>
+    <col min="1023" max="1026" width="6.33203125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>97</v>
       </c>
@@ -3266,7 +3269,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="37" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" s="37" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
@@ -3285,22 +3288,22 @@
       <c r="F2" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="35"/>
+      <c r="H2" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="I2" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="J2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="K2" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="L2" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="L2" s="36"/>
       <c r="M2" s="36"/>
       <c r="N2" s="36"/>
       <c r="O2" s="36"/>
@@ -3313,8 +3316,9 @@
       <c r="V2" s="36"/>
       <c r="W2" s="36"/>
       <c r="X2" s="36"/>
-    </row>
-    <row r="3" spans="1:24" s="27" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Y2" s="36"/>
+    </row>
+    <row r="3" spans="1:25" s="27" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
@@ -3333,19 +3337,22 @@
       <c r="F3" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="71" t="s">
+        <v>204</v>
+      </c>
+      <c r="H3" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="40" t="s">
+      <c r="I3" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="J3" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="J3" s="40" t="s">
+      <c r="K3" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="L3" s="41" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3493,7 +3500,7 @@
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="333" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="359" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Added new SearchCasesResultFields tab that is required for resp solicitor journeys
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamko/Work/FPLA/code/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnon/Development/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959BF888-43EE-FD49-A05E-D191EA996C1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A2648B-0336-0F48-8A12-8996541972F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -26,16 +26,17 @@
     <sheet name="ComplexTypes" sheetId="11" r:id="rId11"/>
     <sheet name="SearchInputFields" sheetId="12" r:id="rId12"/>
     <sheet name="SearchAlias" sheetId="13" r:id="rId13"/>
-    <sheet name="SearchResultFields" sheetId="14" r:id="rId14"/>
-    <sheet name="Banner" sheetId="23" r:id="rId15"/>
-    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId16"/>
-    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId17"/>
-    <sheet name="UserProfile" sheetId="17" r:id="rId18"/>
-    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId19"/>
-    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId20"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId21"/>
-    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId22"/>
-    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId23"/>
+    <sheet name="SearchCasesResultFields" sheetId="24" r:id="rId14"/>
+    <sheet name="SearchResultFields" sheetId="14" r:id="rId15"/>
+    <sheet name="Banner" sheetId="23" r:id="rId16"/>
+    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId17"/>
+    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId18"/>
+    <sheet name="UserProfile" sheetId="17" r:id="rId19"/>
+    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId20"/>
+    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId21"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId22"/>
+    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId23"/>
+    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId24"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="207">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -740,6 +741,12 @@
   </si>
   <si>
     <t>DefaultValue</t>
+  </si>
+  <si>
+    <t>SearchCasesResultFields</t>
+  </si>
+  <si>
+    <t>UseCase</t>
   </si>
 </sst>
 </file>
@@ -750,7 +757,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -927,6 +934,36 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF800000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -936,7 +973,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -959,12 +996,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1069,6 +1121,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="26" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1554,7 +1612,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="99" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1755,7 +1813,7 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1864,6 +1922,96 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C102A7D-12CD-E147-A7E2-0594ABFE8C9D}">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="A4:K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="72" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="72" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="72" t="s">
+        <v>112</v>
+      </c>
+      <c r="I3" s="72" t="s">
+        <v>191</v>
+      </c>
+      <c r="J3" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" s="72" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="73"/>
+      <c r="G4" s="74"/>
+      <c r="I4" s="75"/>
+      <c r="K4" s="76"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="1"/>
+      <c r="K5" s="76"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="73"/>
+      <c r="G6" s="74"/>
+      <c r="K6" s="76"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="K7" s="76"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="K8" s="76"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="K9" s="76"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="K10" s="76"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -1951,7 +2099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B87178-516D-C449-B2C2-346849889C36}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1975,7 +2123,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>196</v>
       </c>
@@ -2012,7 +2160,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -2050,7 +2198,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="49"/>
     </row>
-    <row r="2" spans="1:9" ht="155" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="141" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2114,7 +2262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2144,7 +2292,7 @@
       <c r="E1" s="56"/>
       <c r="F1" s="56"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2190,7 +2338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2220,7 +2368,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="99" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2256,75 +2404,6 @@
       </c>
       <c r="F3" s="20" t="s">
         <v>174</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" ht="169" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2411,6 +2490,75 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2440,7 +2588,7 @@
       <c r="E1" s="58"/>
       <c r="F1" s="58"/>
     </row>
-    <row r="2" spans="1:6" ht="169" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2486,7 +2634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2516,7 +2664,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="169" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2562,7 +2710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2592,7 +2740,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="169" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2638,7 +2786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -3105,7 +3253,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="281" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="253" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3234,7 +3382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AML3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -3500,7 +3648,7 @@
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="359" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="333" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Added new SearchCasesResultFields tab that is required for resp solic… (#118)
* Added new SearchCasesResultFields tab that is required for resp solicitor journeys

* Updated tests to verify new tab
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamko/Work/FPLA/code/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnon/Development/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959BF888-43EE-FD49-A05E-D191EA996C1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A2648B-0336-0F48-8A12-8996541972F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -26,16 +26,17 @@
     <sheet name="ComplexTypes" sheetId="11" r:id="rId11"/>
     <sheet name="SearchInputFields" sheetId="12" r:id="rId12"/>
     <sheet name="SearchAlias" sheetId="13" r:id="rId13"/>
-    <sheet name="SearchResultFields" sheetId="14" r:id="rId14"/>
-    <sheet name="Banner" sheetId="23" r:id="rId15"/>
-    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId16"/>
-    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId17"/>
-    <sheet name="UserProfile" sheetId="17" r:id="rId18"/>
-    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId19"/>
-    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId20"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId21"/>
-    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId22"/>
-    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId23"/>
+    <sheet name="SearchCasesResultFields" sheetId="24" r:id="rId14"/>
+    <sheet name="SearchResultFields" sheetId="14" r:id="rId15"/>
+    <sheet name="Banner" sheetId="23" r:id="rId16"/>
+    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId17"/>
+    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId18"/>
+    <sheet name="UserProfile" sheetId="17" r:id="rId19"/>
+    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId20"/>
+    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId21"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId22"/>
+    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId23"/>
+    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId24"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="207">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -740,6 +741,12 @@
   </si>
   <si>
     <t>DefaultValue</t>
+  </si>
+  <si>
+    <t>SearchCasesResultFields</t>
+  </si>
+  <si>
+    <t>UseCase</t>
   </si>
 </sst>
 </file>
@@ -750,7 +757,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -927,6 +934,36 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF800000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -936,7 +973,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -959,12 +996,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1069,6 +1121,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="26" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1554,7 +1612,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="99" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1755,7 +1813,7 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1864,6 +1922,96 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C102A7D-12CD-E147-A7E2-0594ABFE8C9D}">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="A4:K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="72" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="72" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="72" t="s">
+        <v>112</v>
+      </c>
+      <c r="I3" s="72" t="s">
+        <v>191</v>
+      </c>
+      <c r="J3" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" s="72" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="73"/>
+      <c r="G4" s="74"/>
+      <c r="I4" s="75"/>
+      <c r="K4" s="76"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="1"/>
+      <c r="K5" s="76"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="73"/>
+      <c r="G6" s="74"/>
+      <c r="K6" s="76"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="K7" s="76"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="K8" s="76"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="K9" s="76"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="K10" s="76"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -1951,7 +2099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B87178-516D-C449-B2C2-346849889C36}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1975,7 +2123,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>196</v>
       </c>
@@ -2012,7 +2160,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -2050,7 +2198,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="49"/>
     </row>
-    <row r="2" spans="1:9" ht="155" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="141" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2114,7 +2262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2144,7 +2292,7 @@
       <c r="E1" s="56"/>
       <c r="F1" s="56"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2190,7 +2338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2220,7 +2368,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="99" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2256,75 +2404,6 @@
       </c>
       <c r="F3" s="20" t="s">
         <v>174</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" ht="169" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2411,6 +2490,75 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2440,7 +2588,7 @@
       <c r="E1" s="58"/>
       <c r="F1" s="58"/>
     </row>
-    <row r="2" spans="1:6" ht="169" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2486,7 +2634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2516,7 +2664,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="169" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2562,7 +2710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2592,7 +2740,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="169" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2638,7 +2786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -3105,7 +3253,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="281" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="253" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3234,7 +3382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AML3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -3500,7 +3648,7 @@
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="359" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="333" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
feat: Support searchable filed
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnon/Development/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomaszp/fpla/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A2648B-0336-0F48-8A12-8996541972F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AEF7C1-576E-8A46-BE62-FBE721575EDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="209">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -747,6 +747,12 @@
   </si>
   <si>
     <t>UseCase</t>
+  </si>
+  <si>
+    <t>Searchable</t>
+  </si>
+  <si>
+    <t>Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
   </si>
 </sst>
 </file>
@@ -1660,10 +1666,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1672,7 +1678,7 @@
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>145</v>
       </c>
@@ -1695,7 +1701,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1735,8 +1741,11 @@
       <c r="M2" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1775,6 +1784,9 @@
       </c>
       <c r="M3" s="9" t="s">
         <v>45</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -1925,7 +1937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C102A7D-12CD-E147-A7E2-0594ABFE8C9D}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="A4:K10"/>
     </sheetView>
   </sheetViews>
@@ -2967,10 +2979,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2979,7 +2991,7 @@
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3001,7 +3013,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3038,8 +3050,11 @@
       <c r="L2" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="29" x14ac:dyDescent="0.2">
+      <c r="M2" s="18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -3075,6 +3090,9 @@
       </c>
       <c r="L3" s="9" t="s">
         <v>45</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Support searchable filed (#120)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnon/Development/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomaszp/fpla/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A2648B-0336-0F48-8A12-8996541972F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AEF7C1-576E-8A46-BE62-FBE721575EDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="209">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -747,6 +747,12 @@
   </si>
   <si>
     <t>UseCase</t>
+  </si>
+  <si>
+    <t>Searchable</t>
+  </si>
+  <si>
+    <t>Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
   </si>
 </sst>
 </file>
@@ -1660,10 +1666,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1672,7 +1678,7 @@
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>145</v>
       </c>
@@ -1695,7 +1701,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1735,8 +1741,11 @@
       <c r="M2" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1775,6 +1784,9 @@
       </c>
       <c r="M3" s="9" t="s">
         <v>45</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -1925,7 +1937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C102A7D-12CD-E147-A7E2-0594ABFE8C9D}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="A4:K10"/>
     </sheetView>
   </sheetViews>
@@ -2967,10 +2979,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2979,7 +2991,7 @@
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3001,7 +3013,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3038,8 +3050,11 @@
       <c r="L2" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="29" x14ac:dyDescent="0.2">
+      <c r="M2" s="18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -3075,6 +3090,9 @@
       </c>
       <c r="L3" s="9" t="s">
         <v>45</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: support retain hidden field in case field and complex types
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomaszp/fpla/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samw/Development/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AEF7C1-576E-8A46-BE62-FBE721575EDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC588FE0-08CF-2B4F-BBBD-FF5F67C3F933}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="211">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -753,6 +753,12 @@
   </si>
   <si>
     <t>Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
+  </si>
+  <si>
+    <t>RetainHiddenValue</t>
+  </si>
+  <si>
+    <t>Y if hidden field should have value retained in DB</t>
   </si>
 </sst>
 </file>
@@ -1666,10 +1672,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1678,7 +1684,7 @@
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>145</v>
       </c>
@@ -1701,7 +1707,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1744,8 +1750,11 @@
       <c r="N2" s="18" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2" s="18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1787,6 +1796,9 @@
       </c>
       <c r="N3" s="9" t="s">
         <v>207</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2979,19 +2991,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
+    <col min="3" max="13" width="10.5" customWidth="1"/>
+    <col min="14" max="14" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3013,7 +3027,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3053,8 +3067,11 @@
       <c r="M2" s="18" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.2">
+      <c r="N2" s="18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -3093,6 +3110,9 @@
       </c>
       <c r="M3" s="9" t="s">
         <v>207</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: Support retainHiddenValue (#124)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomaszp/fpla/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AEF7C1-576E-8A46-BE62-FBE721575EDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B14B33-BA3D-3E4F-9B82-A1A7A76FB1B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
     <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId23"/>
     <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId24"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="210">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -753,6 +753,9 @@
   </si>
   <si>
     <t>Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
+  </si>
+  <si>
+    <t>RetainHiddenValue</t>
   </si>
 </sst>
 </file>
@@ -1666,19 +1669,21 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
+    <col min="3" max="14" width="10.5" customWidth="1"/>
+    <col min="15" max="15" width="26.83203125" customWidth="1"/>
+    <col min="16" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>145</v>
       </c>
@@ -1701,7 +1706,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1745,7 +1750,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1787,6 +1792,9 @@
       </c>
       <c r="N3" s="9" t="s">
         <v>207</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -3232,18 +3240,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="14" width="10.5" customWidth="1"/>
+    <col min="3" max="9" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="26.1640625" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" customWidth="1"/>
+    <col min="12" max="14" width="10.5" customWidth="1"/>
     <col min="15" max="15" width="24.33203125" customWidth="1"/>
     <col min="16" max="18" width="10.5" customWidth="1"/>
-    <col min="19" max="19" width="15.1640625" customWidth="1"/>
-    <col min="20" max="1025" width="10.5" customWidth="1"/>
+    <col min="19" max="19" width="23.6640625" customWidth="1"/>
+    <col min="20" max="20" width="20.5" customWidth="1"/>
+    <col min="21" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.2">
@@ -3388,7 +3400,9 @@
       <c r="S3" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="T3" s="10"/>
+      <c r="T3" s="10" t="s">
+        <v>209</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Challenge Question tab for Notice of Change
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomaszp/fpla/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brad.Sorour/Engine/hmcts/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B14B33-BA3D-3E4F-9B82-A1A7A76FB1B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C148134-567C-7947-B63A-CCF1251E7769}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29580" windowHeight="17420" tabRatio="500" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -24,19 +24,20 @@
     <sheet name="CaseEvent" sheetId="9" r:id="rId9"/>
     <sheet name="FixedLists" sheetId="10" r:id="rId10"/>
     <sheet name="ComplexTypes" sheetId="11" r:id="rId11"/>
-    <sheet name="SearchInputFields" sheetId="12" r:id="rId12"/>
-    <sheet name="SearchAlias" sheetId="13" r:id="rId13"/>
-    <sheet name="SearchCasesResultFields" sheetId="24" r:id="rId14"/>
-    <sheet name="SearchResultFields" sheetId="14" r:id="rId15"/>
-    <sheet name="Banner" sheetId="23" r:id="rId16"/>
-    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId17"/>
-    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId18"/>
-    <sheet name="UserProfile" sheetId="17" r:id="rId19"/>
-    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId20"/>
-    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId21"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId22"/>
-    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId23"/>
-    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId24"/>
+    <sheet name="ChallengeQuestion" sheetId="25" r:id="rId12"/>
+    <sheet name="SearchInputFields" sheetId="12" r:id="rId13"/>
+    <sheet name="SearchAlias" sheetId="13" r:id="rId14"/>
+    <sheet name="SearchCasesResultFields" sheetId="24" r:id="rId15"/>
+    <sheet name="SearchResultFields" sheetId="14" r:id="rId16"/>
+    <sheet name="Banner" sheetId="23" r:id="rId17"/>
+    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId18"/>
+    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId19"/>
+    <sheet name="UserProfile" sheetId="17" r:id="rId20"/>
+    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId21"/>
+    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId22"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId23"/>
+    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId24"/>
+    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId25"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="218">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -756,6 +757,31 @@
   </si>
   <si>
     <t>RetainHiddenValue</t>
+  </si>
+  <si>
+    <t>ChallengeQuestion</t>
+  </si>
+  <si>
+    <t>The type of the field that the answer will contain</t>
+  </si>
+  <si>
+    <t>In the form of a comma separated list of potential answer field(s) for each of the (n) litigant types on possible on the case.</t>
+  </si>
+  <si>
+    <t>QuestionText</t>
+  </si>
+  <si>
+    <t>AnswerFieldType</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>QuestionId</t>
+  </si>
+  <si>
+    <t>Order of fields on UI
+Positive Integer</t>
   </si>
 </sst>
 </file>
@@ -766,7 +792,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -973,6 +999,45 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF6600"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF984807"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1025,7 +1090,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1136,6 +1201,12 @@
     <xf numFmtId="1" fontId="26" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1671,7 +1742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
@@ -1804,11 +1875,111 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD9C6E9-A135-BB4B-AB3F-8180231A4906}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="78" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="80" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="81" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="83" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="82" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="82" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="82" t="s">
+        <v>213</v>
+      </c>
+      <c r="G3" s="82" t="s">
+        <v>214</v>
+      </c>
+      <c r="H3" s="82" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="82" t="s">
+        <v>215</v>
+      </c>
+      <c r="J3" s="82" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1879,7 +2050,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1941,12 +2112,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C102A7D-12CD-E147-A7E2-0594ABFE8C9D}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="A4:K10"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2031,7 +2202,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -2119,7 +2290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B87178-516D-C449-B2C2-346849889C36}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2180,7 +2351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -2282,7 +2453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2350,80 +2521,6 @@
       </c>
       <c r="F3" s="10" t="s">
         <v>112</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2510,6 +2607,80 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2578,7 +2749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2654,7 +2825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2730,7 +2901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2806,7 +2977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Challenge Question tab for Notice of Change (#129)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomaszp/fpla/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brad.Sorour/Engine/hmcts/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B14B33-BA3D-3E4F-9B82-A1A7A76FB1B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C148134-567C-7947-B63A-CCF1251E7769}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29580" windowHeight="17420" tabRatio="500" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -24,19 +24,20 @@
     <sheet name="CaseEvent" sheetId="9" r:id="rId9"/>
     <sheet name="FixedLists" sheetId="10" r:id="rId10"/>
     <sheet name="ComplexTypes" sheetId="11" r:id="rId11"/>
-    <sheet name="SearchInputFields" sheetId="12" r:id="rId12"/>
-    <sheet name="SearchAlias" sheetId="13" r:id="rId13"/>
-    <sheet name="SearchCasesResultFields" sheetId="24" r:id="rId14"/>
-    <sheet name="SearchResultFields" sheetId="14" r:id="rId15"/>
-    <sheet name="Banner" sheetId="23" r:id="rId16"/>
-    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId17"/>
-    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId18"/>
-    <sheet name="UserProfile" sheetId="17" r:id="rId19"/>
-    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId20"/>
-    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId21"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId22"/>
-    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId23"/>
-    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId24"/>
+    <sheet name="ChallengeQuestion" sheetId="25" r:id="rId12"/>
+    <sheet name="SearchInputFields" sheetId="12" r:id="rId13"/>
+    <sheet name="SearchAlias" sheetId="13" r:id="rId14"/>
+    <sheet name="SearchCasesResultFields" sheetId="24" r:id="rId15"/>
+    <sheet name="SearchResultFields" sheetId="14" r:id="rId16"/>
+    <sheet name="Banner" sheetId="23" r:id="rId17"/>
+    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId18"/>
+    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId19"/>
+    <sheet name="UserProfile" sheetId="17" r:id="rId20"/>
+    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId21"/>
+    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId22"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId23"/>
+    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId24"/>
+    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId25"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="218">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -756,6 +757,31 @@
   </si>
   <si>
     <t>RetainHiddenValue</t>
+  </si>
+  <si>
+    <t>ChallengeQuestion</t>
+  </si>
+  <si>
+    <t>The type of the field that the answer will contain</t>
+  </si>
+  <si>
+    <t>In the form of a comma separated list of potential answer field(s) for each of the (n) litigant types on possible on the case.</t>
+  </si>
+  <si>
+    <t>QuestionText</t>
+  </si>
+  <si>
+    <t>AnswerFieldType</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>QuestionId</t>
+  </si>
+  <si>
+    <t>Order of fields on UI
+Positive Integer</t>
   </si>
 </sst>
 </file>
@@ -766,7 +792,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -973,6 +999,45 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF6600"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF984807"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1025,7 +1090,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1136,6 +1201,12 @@
     <xf numFmtId="1" fontId="26" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1671,7 +1742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
@@ -1804,11 +1875,111 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD9C6E9-A135-BB4B-AB3F-8180231A4906}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="78" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="80" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="81" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="83" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="82" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="82" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="82" t="s">
+        <v>213</v>
+      </c>
+      <c r="G3" s="82" t="s">
+        <v>214</v>
+      </c>
+      <c r="H3" s="82" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="82" t="s">
+        <v>215</v>
+      </c>
+      <c r="J3" s="82" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1879,7 +2050,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1941,12 +2112,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C102A7D-12CD-E147-A7E2-0594ABFE8C9D}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="A4:K10"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2031,7 +2202,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -2119,7 +2290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B87178-516D-C449-B2C2-346849889C36}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2180,7 +2351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -2282,7 +2453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2350,80 +2521,6 @@
       </c>
       <c r="F3" s="10" t="s">
         <v>112</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2510,6 +2607,80 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2578,7 +2749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2654,7 +2825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2730,7 +2901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2806,7 +2977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added new column Publish to caseEvents
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23815"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brad.Sorour/Engine/hmcts/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharmendrak/development/moj/ccd/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C148134-567C-7947-B63A-CCF1251E7769}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{725172BC-9DD5-934F-8F01-D4FA534E3158}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A54B7FF8-4B2C-452E-A043-FCC066D45FD1}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29580" windowHeight="17420" tabRatio="500" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" firstSheet="14" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -24,23 +24,30 @@
     <sheet name="CaseEvent" sheetId="9" r:id="rId9"/>
     <sheet name="FixedLists" sheetId="10" r:id="rId10"/>
     <sheet name="ComplexTypes" sheetId="11" r:id="rId11"/>
-    <sheet name="ChallengeQuestion" sheetId="25" r:id="rId12"/>
-    <sheet name="SearchInputFields" sheetId="12" r:id="rId13"/>
-    <sheet name="SearchAlias" sheetId="13" r:id="rId14"/>
-    <sheet name="SearchCasesResultFields" sheetId="24" r:id="rId15"/>
-    <sheet name="SearchResultFields" sheetId="14" r:id="rId16"/>
-    <sheet name="Banner" sheetId="23" r:id="rId17"/>
-    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId18"/>
-    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId19"/>
-    <sheet name="UserProfile" sheetId="17" r:id="rId20"/>
-    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId21"/>
-    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId22"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId23"/>
-    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId24"/>
-    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId25"/>
+    <sheet name="SearchInputFields" sheetId="12" r:id="rId12"/>
+    <sheet name="SearchAlias" sheetId="13" r:id="rId13"/>
+    <sheet name="SearchResultFields" sheetId="14" r:id="rId14"/>
+    <sheet name="Banner" sheetId="23" r:id="rId15"/>
+    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId16"/>
+    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId17"/>
+    <sheet name="UserProfile" sheetId="17" r:id="rId18"/>
+    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId19"/>
+    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId20"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId21"/>
+    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId22"/>
+    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId23"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -49,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="206">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -81,6 +88,9 @@
 MaxLength: 100</t>
   </si>
   <si>
+    <t>This can have value TRUE/FALSE</t>
+  </si>
+  <si>
     <t>LiveFrom</t>
   </si>
   <si>
@@ -94,6 +104,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Shuttered</t>
   </si>
   <si>
     <t>CaseRoles</t>
@@ -485,6 +498,9 @@
 MaxLength: 200</t>
   </si>
   <si>
+    <t>Boolean value to say if an event can be published</t>
+  </si>
+  <si>
     <t>PreConditionState(s)</t>
   </si>
   <si>
@@ -519,6 +535,9 @@
   </si>
   <si>
     <t>EndButtonLabel</t>
+  </si>
+  <si>
+    <t>Publish</t>
   </si>
   <si>
     <t>FixedLists</t>
@@ -609,10 +628,43 @@
 Positive Integer</t>
   </si>
   <si>
+    <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
+  </si>
+  <si>
+    <t>Fields can be ordered on by user role</t>
+  </si>
+  <si>
+    <t>ResultsOrdering</t>
+  </si>
+  <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>Yes or No, to enable or disable the banner.                          MaxLength: 30</t>
+  </si>
+  <si>
+    <t>Content to display in the banner         MaxLength: 300</t>
+  </si>
+  <si>
+    <t>Optional link text in the banner                   MaxLength:50</t>
+  </si>
+  <si>
+    <t>The URL for the link text.                                               Max Length: 1000</t>
+  </si>
+  <si>
+    <t>BannerEnabled</t>
+  </si>
+  <si>
+    <t>BannerDescription</t>
+  </si>
+  <si>
+    <t>BannerUrlText</t>
+  </si>
+  <si>
+    <t>BannerUrl</t>
+  </si>
+  <si>
     <t>WorkBasketResultFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
   </si>
   <si>
     <t>WorkBasketInputFields</t>
@@ -700,88 +752,6 @@
   <si>
     <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
-  </si>
-  <si>
-    <t>ResultsOrdering</t>
-  </si>
-  <si>
-    <t>Fields can be ordered on by user role</t>
-  </si>
-  <si>
-    <t>Shuttered</t>
-  </si>
-  <si>
-    <t>This can have value TRUE/FALSE</t>
-  </si>
-  <si>
-    <t>Banner</t>
-  </si>
-  <si>
-    <t>Yes or No, to enable or disable the banner.                          MaxLength: 30</t>
-  </si>
-  <si>
-    <t>Content to display in the banner         MaxLength: 300</t>
-  </si>
-  <si>
-    <t>Optional link text in the banner                   MaxLength:50</t>
-  </si>
-  <si>
-    <t>The URL for the link text.                                               Max Length: 1000</t>
-  </si>
-  <si>
-    <t>BannerEnabled</t>
-  </si>
-  <si>
-    <t>BannerDescription</t>
-  </si>
-  <si>
-    <t>BannerUrlText</t>
-  </si>
-  <si>
-    <t>BannerUrl</t>
-  </si>
-  <si>
-    <t>DefaultValue</t>
-  </si>
-  <si>
-    <t>SearchCasesResultFields</t>
-  </si>
-  <si>
-    <t>UseCase</t>
-  </si>
-  <si>
-    <t>Searchable</t>
-  </si>
-  <si>
-    <t>Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
-  </si>
-  <si>
-    <t>RetainHiddenValue</t>
-  </si>
-  <si>
-    <t>ChallengeQuestion</t>
-  </si>
-  <si>
-    <t>The type of the field that the answer will contain</t>
-  </si>
-  <si>
-    <t>In the form of a comma separated list of potential answer field(s) for each of the (n) litigant types on possible on the case.</t>
-  </si>
-  <si>
-    <t>QuestionText</t>
-  </si>
-  <si>
-    <t>AnswerFieldType</t>
-  </si>
-  <si>
-    <t>Answer</t>
-  </si>
-  <si>
-    <t>QuestionId</t>
-  </si>
-  <si>
-    <t>Order of fields on UI
-Positive Integer</t>
   </si>
 </sst>
 </file>
@@ -792,7 +762,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="29">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -970,84 +940,51 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF333333"/>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF800000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica"/>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFF6600"/>
-      <name val="Helvetica"/>
+      <sz val="9"/>
+      <color rgb="FF6A8759"/>
+      <name val="Menlo"/>
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="10"/>
-      <color rgb="FFFFC000"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF984807"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFFC000"/>
-      <name val="Helvetica"/>
+      <color rgb="FF0563C1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1071,26 +1008,51 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF000080"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="FF000080"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color rgb="FF000080"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000080"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1195,21 +1157,21 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="26" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="26" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1596,13 +1558,13 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1617,7 +1579,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="126.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1634,27 +1596,27 @@
         <v>8</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>193</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1671,15 +1633,15 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1692,7 +1654,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="84.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1700,36 +1662,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1740,23 +1702,21 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="14" width="10.5" customWidth="1"/>
-    <col min="15" max="15" width="26.83203125" customWidth="1"/>
-    <col min="16" max="1025" width="10.5" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="18">
       <c r="A1" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1777,7 +1737,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="409.6">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1785,87 +1745,78 @@
         <v>5</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K3" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>209</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1875,40 +1826,36 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD9C6E9-A135-BB4B-AB3F-8180231A4906}">
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="78" t="s">
-        <v>210</v>
-      </c>
-      <c r="C1" s="79" t="s">
+    <row r="1" spans="1:6" ht="18">
+      <c r="A1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+    </row>
+    <row r="2" spans="1:6" ht="113.1">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1916,81 +1863,63 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>217</v>
+        <v>158</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="83" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="82" t="s">
+      <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="82" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" s="82" t="s">
-        <v>213</v>
-      </c>
-      <c r="G3" s="82" t="s">
-        <v>214</v>
-      </c>
-      <c r="H3" s="82" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="82" t="s">
-        <v>215</v>
-      </c>
-      <c r="J3" s="82" t="s">
-        <v>216</v>
+      <c r="C3" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>1</v>
@@ -2001,48 +1930,32 @@
       <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-    </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
+    </row>
+    <row r="2" spans="1:6" ht="113.1">
+      <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
-        <v>5</v>
+        <v>161</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>162</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>163</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>112</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D3" s="48"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2051,60 +1964,86 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="1025" width="10.5" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B1" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" ht="141">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>159</v>
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="48"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+        <v>19</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>170</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2113,89 +2052,104 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C102A7D-12CD-E147-A7E2-0594ABFE8C9D}">
-  <dimension ref="A1:K10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B87178-516D-C449-B2C2-346849889C36}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="31.875" customWidth="1"/>
+    <col min="3" max="3" width="31.625" customWidth="1"/>
+    <col min="4" max="4" width="30.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="72" t="s">
-        <v>102</v>
-      </c>
-      <c r="G3" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="72" t="s">
-        <v>112</v>
-      </c>
-      <c r="I3" s="72" t="s">
-        <v>191</v>
-      </c>
-      <c r="J3" s="72" t="s">
-        <v>66</v>
-      </c>
-      <c r="K3" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="73"/>
-      <c r="G4" s="74"/>
-      <c r="I4" s="75"/>
-      <c r="K4" s="76"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="1"/>
-      <c r="K5" s="76"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="73"/>
-      <c r="G6" s="74"/>
-      <c r="K6" s="76"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="K7" s="76"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="K8" s="76"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="K9" s="76"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="K10" s="76"/>
+    <row r="1" spans="1:4">
+      <c r="A1" s="72" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="74"/>
+    </row>
+    <row r="2" spans="1:4" ht="42.95">
+      <c r="A2" s="75" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="75" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" s="75" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="76" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="76" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="76" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="76" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="79"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="80"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="80"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="80"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="80"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="80"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="80"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="80"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2203,155 +2157,6 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:8" ht="141" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="G2" s="50" t="s">
-        <v>165</v>
-      </c>
-      <c r="H2" s="50" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="G3" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="52" t="s">
-        <v>191</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B87178-516D-C449-B2C2-346849889C36}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -2359,9 +2164,9 @@
       <selection activeCell="H2" sqref="H2:I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="10.5" customWidth="1"/>
@@ -2371,9 +2176,9 @@
     <col min="10" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" s="2" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2389,7 +2194,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="49"/>
     </row>
-    <row r="2" spans="1:9" ht="141" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="141">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2397,54 +2202,204 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="I2" s="50" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="52" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
+  <cols>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.95">
+      <c r="A1" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+    </row>
+    <row r="2" spans="1:6" ht="113.1">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
+      <c r="B3" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="C3" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="51" t="s">
-        <v>102</v>
+        <v>63</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="H3" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="I3" s="52" t="s">
-        <v>191</v>
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
+  <cols>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18">
+      <c r="A1" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="84.95">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2454,36 +2409,35 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
-        <v>166</v>
-      </c>
-      <c r="B1" s="54" t="s">
+    <row r="1" spans="1:5" ht="18">
+      <c r="A1" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-    </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" ht="126.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2491,36 +2445,30 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>191</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>112</v>
+      <c r="B3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2537,18 +2485,18 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.375" customWidth="1"/>
+    <col min="3" max="3" width="27.375" customWidth="1"/>
+    <col min="4" max="4" width="30.625" customWidth="1"/>
     <col min="5" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
@@ -2560,44 +2508,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2607,22 +2555,22 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>167</v>
+    <row r="1" spans="1:6" ht="18">
+      <c r="A1" s="57" t="s">
+        <v>195</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2633,45 +2581,47 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+    </row>
+    <row r="2" spans="1:6" ht="126.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="C2" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>174</v>
+      <c r="B3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2681,22 +2631,22 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2708,8 +2658,9 @@
         <v>3</v>
       </c>
       <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="126.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2717,30 +2668,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>179</v>
+        <v>11</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2750,36 +2707,36 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
-        <v>180</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:6" ht="18">
+      <c r="A1" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-    </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="126.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2787,36 +2744,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>182</v>
+        <v>196</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>201</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="24" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="B3" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C3" s="59" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>61</v>
+        <v>202</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>179</v>
+        <v>64</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2826,158 +2783,6 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="59" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B1" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="61" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="62" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="D2" s="63" t="s">
-        <v>186</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="59" t="s">
-        <v>187</v>
-      </c>
-      <c r="E3" s="59" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -2985,14 +2790,14 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="18">
       <c r="A1" s="64" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="B1" s="65" t="s">
         <v>1</v>
@@ -3007,46 +2812,46 @@
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
     </row>
-    <row r="2" spans="1:7" ht="253" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="252.95">
       <c r="A2" s="68"/>
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="D2" s="69" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="E2" s="69" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F2" s="69" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
       <c r="G2" s="69" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="70" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="70" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="71" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="71" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E3" s="71" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F3" s="70" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G3" s="70" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -3067,15 +2872,15 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" s="17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3092,7 +2897,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="211" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="210.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3103,51 +2908,51 @@
         <v>6</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="43" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="42.95">
       <c r="A3" s="19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3158,21 +2963,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="18">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3192,7 +2997,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="409.6">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3200,78 +3005,72 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="29.1">
+      <c r="A3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="K3" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>207</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3288,18 +3087,18 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="11" width="10.5" customWidth="1"/>
     <col min="12" max="12" width="16.5" customWidth="1"/>
-    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="13" max="13" width="22.375" customWidth="1"/>
     <col min="14" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="18">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="3" t="s">
@@ -3319,7 +3118,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="183" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="183">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3327,78 +3126,78 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3411,27 +3210,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="9" width="10.5" customWidth="1"/>
-    <col min="10" max="10" width="26.1640625" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" customWidth="1"/>
-    <col min="12" max="14" width="10.5" customWidth="1"/>
-    <col min="15" max="15" width="24.33203125" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
+    <col min="3" max="14" width="10.5" customWidth="1"/>
+    <col min="15" max="15" width="24.375" customWidth="1"/>
     <col min="16" max="18" width="10.5" customWidth="1"/>
-    <col min="19" max="19" width="23.6640625" customWidth="1"/>
-    <col min="20" max="20" width="20.5" customWidth="1"/>
-    <col min="21" max="1025" width="10.5" customWidth="1"/>
+    <col min="19" max="19" width="15.125" customWidth="1"/>
+    <col min="20" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="18">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3454,7 +3249,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="253" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="252.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3462,118 +3257,116 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M3" s="24" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>209</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="T3" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3583,32 +3376,32 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AML3"/>
+  <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="19.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" style="25" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="26" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" style="26" customWidth="1"/>
-    <col min="5" max="7" width="30.1640625" style="26" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="26" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="26" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="26" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" style="26" customWidth="1"/>
-    <col min="12" max="12" width="16" style="26" customWidth="1"/>
-    <col min="13" max="14" width="6.33203125" style="26" customWidth="1"/>
-    <col min="15" max="1022" width="6.33203125" style="27" customWidth="1"/>
-    <col min="1023" max="1026" width="6.33203125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="11.125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="17.875" style="26" customWidth="1"/>
+    <col min="4" max="4" width="16.875" style="26" customWidth="1"/>
+    <col min="5" max="6" width="30.125" style="26" customWidth="1"/>
+    <col min="7" max="7" width="12.125" style="26" customWidth="1"/>
+    <col min="8" max="8" width="9.625" style="26" customWidth="1"/>
+    <col min="9" max="9" width="14.625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="16.375" style="26" customWidth="1"/>
+    <col min="11" max="11" width="16" style="26" customWidth="1"/>
+    <col min="12" max="13" width="6.375" style="26" customWidth="1"/>
+    <col min="14" max="1021" width="6.375" style="27" customWidth="1"/>
+    <col min="1022" max="1025" width="6.375" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="18" customHeight="1">
       <c r="A1" s="29" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>1</v>
@@ -3620,7 +3413,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="37" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:24" s="37" customFormat="1" ht="111.95">
       <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
@@ -3628,33 +3421,33 @@
         <v>5</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="G2" s="35"/>
+        <v>101</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>102</v>
+      </c>
       <c r="H2" s="35" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="K2" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" s="36" t="s">
-        <v>76</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" s="36"/>
       <c r="M2" s="36"/>
       <c r="N2" s="36"/>
       <c r="O2" s="36"/>
@@ -3667,44 +3460,40 @@
       <c r="V2" s="36"/>
       <c r="W2" s="36"/>
       <c r="X2" s="36"/>
-      <c r="Y2" s="36"/>
-    </row>
-    <row r="3" spans="1:25" s="27" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:24" s="27" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="G3" s="71" t="s">
-        <v>204</v>
+        <v>104</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>105</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I3" s="40" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="K3" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="L3" s="41" t="s">
-        <v>64</v>
+        <v>87</v>
+      </c>
+      <c r="K3" s="41" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -3725,15 +3514,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3749,7 +3538,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="225" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="225">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3757,48 +3546,48 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -3809,21 +3598,23 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
+    <col min="3" max="19" width="10.5" customWidth="1"/>
+    <col min="20" max="20" width="17.875" customWidth="1"/>
+    <col min="21" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="18">
       <c r="A1" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3851,7 +3642,7 @@
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="333" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="306">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3859,120 +3650,126 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="51">
+      <c r="A3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="L3" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="M3" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="N3" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="O3" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="P3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="57" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="J3" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="K3" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="L3" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="M3" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="N3" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="O3" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="Q3" s="9" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="R3" s="19" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="T3" s="19" t="s">
-        <v>138</v>
+        <v>141</v>
+      </c>
+      <c r="U3" s="19" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated on latest template
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23815"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23821"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharmendrak/development/moj/ccd/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brad.Sorour/Engine/hmcts/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{725172BC-9DD5-934F-8F01-D4FA534E3158}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A54B7FF8-4B2C-452E-A043-FCC066D45FD1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{12EB3A57-41B9-487D-8977-86D9C3B5FB0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" tabRatio="500" firstSheet="14" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29580" windowHeight="17420" tabRatio="500" firstSheet="11" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -24,20 +24,22 @@
     <sheet name="CaseEvent" sheetId="9" r:id="rId9"/>
     <sheet name="FixedLists" sheetId="10" r:id="rId10"/>
     <sheet name="ComplexTypes" sheetId="11" r:id="rId11"/>
-    <sheet name="SearchInputFields" sheetId="12" r:id="rId12"/>
-    <sheet name="SearchAlias" sheetId="13" r:id="rId13"/>
-    <sheet name="SearchResultFields" sheetId="14" r:id="rId14"/>
-    <sheet name="Banner" sheetId="23" r:id="rId15"/>
-    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId16"/>
-    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId17"/>
-    <sheet name="UserProfile" sheetId="17" r:id="rId18"/>
-    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId19"/>
-    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId20"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId21"/>
-    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId22"/>
-    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId23"/>
+    <sheet name="ChallengeQuestion" sheetId="25" r:id="rId12"/>
+    <sheet name="SearchInputFields" sheetId="12" r:id="rId13"/>
+    <sheet name="SearchAlias" sheetId="13" r:id="rId14"/>
+    <sheet name="SearchCasesResultFields" sheetId="24" r:id="rId15"/>
+    <sheet name="SearchResultFields" sheetId="14" r:id="rId16"/>
+    <sheet name="Banner" sheetId="23" r:id="rId17"/>
+    <sheet name="WorkBasketResultFields" sheetId="15" r:id="rId18"/>
+    <sheet name="WorkBasketInputFields" sheetId="16" r:id="rId19"/>
+    <sheet name="UserProfile" sheetId="17" r:id="rId20"/>
+    <sheet name="AuthorisationCaseType" sheetId="18" r:id="rId21"/>
+    <sheet name="AuthorisationCaseField" sheetId="19" r:id="rId22"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="20" r:id="rId23"/>
+    <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId24"/>
+    <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028" iterateDelta="1E-4" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -56,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="220">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -198,6 +200,9 @@
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
+    <t>Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
+  </si>
+  <si>
     <t>Label</t>
   </si>
   <si>
@@ -217,6 +222,9 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>Searchable</t>
   </si>
   <si>
     <t>CaseTypeTab</t>
@@ -388,6 +396,9 @@
     <t>CaseEventFieldHint</t>
   </si>
   <si>
+    <t>RetainHiddenValue</t>
+  </si>
+  <si>
     <t>EventToComplexTypes</t>
   </si>
   <si>
@@ -405,6 +416,9 @@
   </si>
   <si>
     <t>ListElementCode</t>
+  </si>
+  <si>
+    <t>DefaultValue</t>
   </si>
   <si>
     <t>EventElementLabel</t>
@@ -588,6 +602,31 @@
     <t>ElementLabel</t>
   </si>
   <si>
+    <t>ChallengeQuestion</t>
+  </si>
+  <si>
+    <t>Order of fields on UI
+Positive Integer</t>
+  </si>
+  <si>
+    <t>The type of the field that the answer will contain</t>
+  </si>
+  <si>
+    <t>In the form of a comma separated list of potential answer field(s) for each of the (n) litigant types on possible on the case.</t>
+  </si>
+  <si>
+    <t>QuestionText</t>
+  </si>
+  <si>
+    <t>AnswerFieldType</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>QuestionId</t>
+  </si>
+  <si>
     <t>SearchInputFields</t>
   </si>
   <si>
@@ -614,6 +653,15 @@
     <t>SearchAliasID</t>
   </si>
   <si>
+    <t>SearchCasesResultFields</t>
+  </si>
+  <si>
+    <t>ResultsOrdering</t>
+  </si>
+  <si>
+    <t>UseCase</t>
+  </si>
+  <si>
     <t>SearchResultFields</t>
   </si>
   <si>
@@ -632,9 +680,6 @@
   </si>
   <si>
     <t>Fields can be ordered on by user role</t>
-  </si>
-  <si>
-    <t>ResultsOrdering</t>
   </si>
   <si>
     <t>Banner</t>
@@ -762,7 +807,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="35">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -940,51 +985,84 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF800000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <i/>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF6A8759"/>
-      <name val="Menlo"/>
+      <sz val="10"/>
+      <color rgb="FFFF6600"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
     <font>
-      <u/>
       <sz val="10"/>
-      <color rgb="FF0563C1"/>
-      <name val="Arial"/>
+      <color rgb="FFFFC000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF984807"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1008,51 +1086,26 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000080"/>
+      </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000080"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000080"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000080"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1157,21 +1210,21 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="26" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="25" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="26" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1641,7 +1694,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1662,16 +1715,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1685,13 +1738,13 @@
         <v>12</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1702,21 +1755,23 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
+    <col min="3" max="14" width="10.5" customWidth="1"/>
+    <col min="15" max="15" width="26.875" customWidth="1"/>
+    <col min="16" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18">
+    <row r="1" spans="1:15" ht="18">
       <c r="A1" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1737,7 +1792,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="409.6">
+    <row r="2" spans="1:15" ht="409.6">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1745,10 +1800,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>36</v>
@@ -1757,16 +1812,16 @@
         <v>37</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="I2" s="18" t="s">
         <v>38</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>26</v>
@@ -1777,8 +1832,11 @@
       <c r="M2" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -1789,34 +1847,40 @@
         <v>12</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>30</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1826,11 +1890,111 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD9C6E9-A135-BB4B-AB3F-8180231A4906}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <cols>
+    <col min="1" max="1" width="22.875" customWidth="1"/>
+    <col min="2" max="2" width="21.625" customWidth="1"/>
+    <col min="3" max="3" width="26.625" customWidth="1"/>
+    <col min="4" max="4" width="19.375" customWidth="1"/>
+    <col min="5" max="5" width="16.875" customWidth="1"/>
+    <col min="6" max="6" width="16.625" customWidth="1"/>
+    <col min="7" max="7" width="22.375" customWidth="1"/>
+    <col min="8" max="8" width="16.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18">
+      <c r="A1" s="78" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="80" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="81" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="111.95" customHeight="1">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="82" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="83" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="82" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="82" t="s">
+        <v>164</v>
+      </c>
+      <c r="G3" s="82" t="s">
+        <v>165</v>
+      </c>
+      <c r="H3" s="82" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="82" t="s">
+        <v>166</v>
+      </c>
+      <c r="J3" s="82" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
@@ -1841,7 +2005,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>1</v>
@@ -1866,13 +2030,13 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1886,13 +2050,13 @@
         <v>19</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1901,7 +2065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1919,7 +2083,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>1</v>
@@ -1934,10 +2098,10 @@
     <row r="2" spans="1:6" ht="113.1">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -1948,10 +2112,10 @@
         <v>19</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D3" s="48"/>
       <c r="E3" s="10"/>
@@ -1963,7 +2127,97 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C102A7D-12CD-E147-A7E2-0594ABFE8C9D}">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="18">
+      <c r="A3" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="72" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="72" t="s">
+        <v>118</v>
+      </c>
+      <c r="I3" s="72" t="s">
+        <v>177</v>
+      </c>
+      <c r="J3" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="K3" s="72" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1"/>
+      <c r="B4" s="73"/>
+      <c r="G4" s="74"/>
+      <c r="I4" s="75"/>
+      <c r="K4" s="76"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="1"/>
+      <c r="K5" s="76"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1"/>
+      <c r="B6" s="73"/>
+      <c r="G6" s="74"/>
+      <c r="K6" s="76"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1"/>
+      <c r="K7" s="76"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1"/>
+      <c r="K8" s="76"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1"/>
+      <c r="K9" s="76"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1"/>
+      <c r="K10" s="76"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -1979,7 +2233,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18">
       <c r="A1" s="2" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2004,19 +2258,19 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="G2" s="50" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -2030,19 +2284,19 @@
         <v>19</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H3" s="52" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2051,112 +2305,68 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B87178-516D-C449-B2C2-346849889C36}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="31.875" customWidth="1"/>
-    <col min="3" max="3" width="31.625" customWidth="1"/>
-    <col min="4" max="4" width="30.5" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="72" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="74"/>
-    </row>
-    <row r="2" spans="1:4" ht="42.95">
-      <c r="A2" s="75" t="s">
-        <v>172</v>
-      </c>
-      <c r="B2" s="75" t="s">
-        <v>173</v>
-      </c>
-      <c r="C2" s="75" t="s">
-        <v>174</v>
-      </c>
-      <c r="D2" s="75" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="B3" s="76" t="s">
-        <v>177</v>
-      </c>
-      <c r="C3" s="76" t="s">
-        <v>178</v>
-      </c>
-      <c r="D3" s="76" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="77"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="79"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="80"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="80"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="80"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="80"/>
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="80"/>
-      <c r="B9" s="80"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="80"/>
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="80"/>
-      <c r="B11" s="80"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
+    <row r="1" spans="1:6" ht="18">
+      <c r="A1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="84.95">
+      <c r="A2" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -2178,7 +2388,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18">
       <c r="A1" s="2" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2205,22 +2415,22 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="I2" s="50" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2234,22 +2444,22 @@
         <v>19</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E3" s="51" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="H3" s="52" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I3" s="52" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2258,7 +2468,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2274,7 +2484,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.95">
       <c r="A1" s="53" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="B1" s="54" t="s">
         <v>1</v>
@@ -2299,13 +2509,13 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2319,156 +2529,13 @@
         <v>19</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
-  <cols>
-    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="18">
-      <c r="A1" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" ht="84.95">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>189</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
-  <cols>
-    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18">
-      <c r="A1" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" ht="126.95">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>194</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2555,6 +2622,149 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
+  <cols>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18">
+      <c r="A1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="84.95">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
+  <cols>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18">
+      <c r="A1" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" ht="126.95">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2570,7 +2780,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18">
       <c r="A1" s="57" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2592,16 +2802,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2615,13 +2825,13 @@
         <v>19</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2630,7 +2840,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2646,7 +2856,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2668,16 +2878,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2691,13 +2901,13 @@
         <v>19</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2706,7 +2916,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2722,7 +2932,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="B1" s="60" t="s">
         <v>1</v>
@@ -2744,16 +2954,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="D2" s="63" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2767,13 +2977,13 @@
         <v>19</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>202</v>
+        <v>216</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2782,7 +2992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -2797,7 +3007,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18">
       <c r="A1" s="64" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="B1" s="65" t="s">
         <v>1</v>
@@ -2816,19 +3026,19 @@
       <c r="A2" s="68"/>
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="D2" s="69" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="E2" s="69" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="F2" s="69" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="G2" s="69" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2842,16 +3052,16 @@
         <v>19</v>
       </c>
       <c r="D3" s="71" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E3" s="71" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F3" s="70" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G3" s="70" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2963,10 +3173,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
@@ -2975,7 +3185,7 @@
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18">
+    <row r="1" spans="1:13" ht="18">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -2997,7 +3207,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:12" ht="409.6">
+    <row r="2" spans="1:13" ht="409.6">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3034,8 +3244,11 @@
       <c r="L2" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="29.1">
+      <c r="M2" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="29.1">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -3049,28 +3262,31 @@
         <v>12</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>30</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -3098,7 +3314,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="3" t="s">
@@ -3129,34 +3345,34 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -3170,34 +3386,34 @@
         <v>19</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3210,23 +3426,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
-    <col min="3" max="14" width="10.5" customWidth="1"/>
+    <col min="3" max="9" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="26.125" customWidth="1"/>
+    <col min="11" max="11" width="22.125" customWidth="1"/>
+    <col min="12" max="14" width="10.5" customWidth="1"/>
     <col min="15" max="15" width="24.375" customWidth="1"/>
     <col min="16" max="18" width="10.5" customWidth="1"/>
-    <col min="19" max="19" width="15.125" customWidth="1"/>
-    <col min="20" max="1025" width="10.5" customWidth="1"/>
+    <col min="19" max="19" width="23.625" customWidth="1"/>
+    <col min="20" max="20" width="20.5" customWidth="1"/>
+    <col min="21" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18">
       <c r="A1" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3260,52 +3480,52 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -3319,54 +3539,56 @@
         <v>19</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M3" s="24" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="T3" s="10"/>
+        <v>100</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -3376,10 +3598,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AMK3"/>
+  <dimension ref="A1:AML3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
@@ -3388,20 +3610,20 @@
     <col min="2" max="2" width="11.125" style="25" customWidth="1"/>
     <col min="3" max="3" width="17.875" style="26" customWidth="1"/>
     <col min="4" max="4" width="16.875" style="26" customWidth="1"/>
-    <col min="5" max="6" width="30.125" style="26" customWidth="1"/>
-    <col min="7" max="7" width="12.125" style="26" customWidth="1"/>
-    <col min="8" max="8" width="9.625" style="26" customWidth="1"/>
-    <col min="9" max="9" width="14.625" style="26" customWidth="1"/>
-    <col min="10" max="10" width="16.375" style="26" customWidth="1"/>
-    <col min="11" max="11" width="16" style="26" customWidth="1"/>
-    <col min="12" max="13" width="6.375" style="26" customWidth="1"/>
-    <col min="14" max="1021" width="6.375" style="27" customWidth="1"/>
-    <col min="1022" max="1025" width="6.375" style="28" customWidth="1"/>
+    <col min="5" max="7" width="30.125" style="26" customWidth="1"/>
+    <col min="8" max="8" width="12.125" style="26" customWidth="1"/>
+    <col min="9" max="9" width="9.625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="14.625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="16.375" style="26" customWidth="1"/>
+    <col min="12" max="12" width="16" style="26" customWidth="1"/>
+    <col min="13" max="14" width="6.375" style="26" customWidth="1"/>
+    <col min="15" max="1022" width="6.375" style="27" customWidth="1"/>
+    <col min="1023" max="1026" width="6.375" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="18" customHeight="1">
+    <row r="1" spans="1:25" ht="18" customHeight="1">
       <c r="A1" s="29" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>1</v>
@@ -3413,7 +3635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="37" customFormat="1" ht="111.95">
+    <row r="2" spans="1:25" s="37" customFormat="1" ht="111.95">
       <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
@@ -3421,33 +3643,33 @@
         <v>5</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>102</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="G2" s="35"/>
       <c r="H2" s="35" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="L2" s="36"/>
+        <v>74</v>
+      </c>
+      <c r="K2" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>80</v>
+      </c>
       <c r="M2" s="36"/>
       <c r="N2" s="36"/>
       <c r="O2" s="36"/>
@@ -3460,8 +3682,9 @@
       <c r="V2" s="36"/>
       <c r="W2" s="36"/>
       <c r="X2" s="36"/>
-    </row>
-    <row r="3" spans="1:24" s="27" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="Y2" s="36"/>
+    </row>
+    <row r="3" spans="1:25" s="27" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="38" t="s">
         <v>10</v>
       </c>
@@ -3472,28 +3695,31 @@
         <v>12</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="G3" s="40" t="s">
-        <v>105</v>
+        <v>107</v>
+      </c>
+      <c r="G3" s="71" t="s">
+        <v>108</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="I3" s="40" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="K3" s="41" t="s">
-        <v>66</v>
+        <v>111</v>
+      </c>
+      <c r="K3" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" s="41" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3522,7 +3748,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3549,19 +3775,19 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3584,10 +3810,10 @@
         <v>14</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3600,21 +3826,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="19" width="10.5" customWidth="1"/>
-    <col min="20" max="20" width="17.875" customWidth="1"/>
+    <col min="20" max="20" width="14.75" customWidth="1"/>
     <col min="21" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18">
       <c r="A1" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3653,58 +3879,58 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>26</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="51">
@@ -3727,49 +3953,49 @@
         <v>14</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="J3" s="42" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="K3" s="42" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="L3" s="42" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="M3" s="42" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="N3" s="42" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="O3" s="42" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>30</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="R3" s="19" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="T3" s="19" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="U3" s="19" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new column Publish to caseEvents (#132)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23821"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brad.Sorour/Engine/hmcts/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C148134-567C-7947-B63A-CCF1251E7769}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{12EB3A57-41B9-487D-8977-86D9C3B5FB0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29580" windowHeight="17420" tabRatio="500" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29580" windowHeight="17420" tabRatio="500" firstSheet="11" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -39,8 +39,17 @@
     <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId24"/>
     <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191028" iterateDelta="1E-4" calcCompleted="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -49,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="220">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -81,6 +90,9 @@
 MaxLength: 100</t>
   </si>
   <si>
+    <t>This can have value TRUE/FALSE</t>
+  </si>
+  <si>
     <t>LiveFrom</t>
   </si>
   <si>
@@ -94,6 +106,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Shuttered</t>
   </si>
   <si>
     <t>CaseRoles</t>
@@ -185,6 +200,9 @@
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
+    <t>Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
+  </si>
+  <si>
     <t>Label</t>
   </si>
   <si>
@@ -204,6 +222,9 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>Searchable</t>
   </si>
   <si>
     <t>CaseTypeTab</t>
@@ -375,6 +396,9 @@
     <t>CaseEventFieldHint</t>
   </si>
   <si>
+    <t>RetainHiddenValue</t>
+  </si>
+  <si>
     <t>EventToComplexTypes</t>
   </si>
   <si>
@@ -392,6 +416,9 @@
   </si>
   <si>
     <t>ListElementCode</t>
+  </si>
+  <si>
+    <t>DefaultValue</t>
   </si>
   <si>
     <t>EventElementLabel</t>
@@ -485,6 +512,9 @@
 MaxLength: 200</t>
   </si>
   <si>
+    <t>Boolean value to say if an event can be published</t>
+  </si>
+  <si>
     <t>PreConditionState(s)</t>
   </si>
   <si>
@@ -519,6 +549,9 @@
   </si>
   <si>
     <t>EndButtonLabel</t>
+  </si>
+  <si>
+    <t>Publish</t>
   </si>
   <si>
     <t>FixedLists</t>
@@ -569,6 +602,31 @@
     <t>ElementLabel</t>
   </si>
   <si>
+    <t>ChallengeQuestion</t>
+  </si>
+  <si>
+    <t>Order of fields on UI
+Positive Integer</t>
+  </si>
+  <si>
+    <t>The type of the field that the answer will contain</t>
+  </si>
+  <si>
+    <t>In the form of a comma separated list of potential answer field(s) for each of the (n) litigant types on possible on the case.</t>
+  </si>
+  <si>
+    <t>QuestionText</t>
+  </si>
+  <si>
+    <t>AnswerFieldType</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>QuestionId</t>
+  </si>
+  <si>
     <t>SearchInputFields</t>
   </si>
   <si>
@@ -595,6 +653,15 @@
     <t>SearchAliasID</t>
   </si>
   <si>
+    <t>SearchCasesResultFields</t>
+  </si>
+  <si>
+    <t>ResultsOrdering</t>
+  </si>
+  <si>
+    <t>UseCase</t>
+  </si>
+  <si>
     <t>SearchResultFields</t>
   </si>
   <si>
@@ -609,10 +676,40 @@
 Positive Integer</t>
   </si>
   <si>
+    <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
+  </si>
+  <si>
+    <t>Fields can be ordered on by user role</t>
+  </si>
+  <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>Yes or No, to enable or disable the banner.                          MaxLength: 30</t>
+  </si>
+  <si>
+    <t>Content to display in the banner         MaxLength: 300</t>
+  </si>
+  <si>
+    <t>Optional link text in the banner                   MaxLength:50</t>
+  </si>
+  <si>
+    <t>The URL for the link text.                                               Max Length: 1000</t>
+  </si>
+  <si>
+    <t>BannerEnabled</t>
+  </si>
+  <si>
+    <t>BannerDescription</t>
+  </si>
+  <si>
+    <t>BannerUrlText</t>
+  </si>
+  <si>
+    <t>BannerUrl</t>
+  </si>
+  <si>
     <t>WorkBasketResultFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
   </si>
   <si>
     <t>WorkBasketInputFields</t>
@@ -700,88 +797,6 @@
   <si>
     <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
-  </si>
-  <si>
-    <t>ResultsOrdering</t>
-  </si>
-  <si>
-    <t>Fields can be ordered on by user role</t>
-  </si>
-  <si>
-    <t>Shuttered</t>
-  </si>
-  <si>
-    <t>This can have value TRUE/FALSE</t>
-  </si>
-  <si>
-    <t>Banner</t>
-  </si>
-  <si>
-    <t>Yes or No, to enable or disable the banner.                          MaxLength: 30</t>
-  </si>
-  <si>
-    <t>Content to display in the banner         MaxLength: 300</t>
-  </si>
-  <si>
-    <t>Optional link text in the banner                   MaxLength:50</t>
-  </si>
-  <si>
-    <t>The URL for the link text.                                               Max Length: 1000</t>
-  </si>
-  <si>
-    <t>BannerEnabled</t>
-  </si>
-  <si>
-    <t>BannerDescription</t>
-  </si>
-  <si>
-    <t>BannerUrlText</t>
-  </si>
-  <si>
-    <t>BannerUrl</t>
-  </si>
-  <si>
-    <t>DefaultValue</t>
-  </si>
-  <si>
-    <t>SearchCasesResultFields</t>
-  </si>
-  <si>
-    <t>UseCase</t>
-  </si>
-  <si>
-    <t>Searchable</t>
-  </si>
-  <si>
-    <t>Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
-  </si>
-  <si>
-    <t>RetainHiddenValue</t>
-  </si>
-  <si>
-    <t>ChallengeQuestion</t>
-  </si>
-  <si>
-    <t>The type of the field that the answer will contain</t>
-  </si>
-  <si>
-    <t>In the form of a comma separated list of potential answer field(s) for each of the (n) litigant types on possible on the case.</t>
-  </si>
-  <si>
-    <t>QuestionText</t>
-  </si>
-  <si>
-    <t>AnswerFieldType</t>
-  </si>
-  <si>
-    <t>Answer</t>
-  </si>
-  <si>
-    <t>QuestionId</t>
-  </si>
-  <si>
-    <t>Order of fields on UI
-Positive Integer</t>
   </si>
 </sst>
 </file>
@@ -792,7 +807,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="35">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1596,13 +1611,13 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1617,7 +1632,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="126.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1634,27 +1649,27 @@
         <v>8</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>193</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1671,15 +1686,15 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1692,7 +1707,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="84.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1700,36 +1715,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1746,17 +1761,17 @@
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="14" width="10.5" customWidth="1"/>
-    <col min="15" max="15" width="26.83203125" customWidth="1"/>
+    <col min="15" max="15" width="26.875" customWidth="1"/>
     <col min="16" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="18">
       <c r="A1" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1777,7 +1792,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="409.6">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1785,87 +1800,87 @@
         <v>5</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K3" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>207</v>
+        <v>49</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>209</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1878,25 +1893,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD9C6E9-A135-BB4B-AB3F-8180231A4906}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.875" customWidth="1"/>
+    <col min="2" max="2" width="21.625" customWidth="1"/>
+    <col min="3" max="3" width="26.625" customWidth="1"/>
+    <col min="4" max="4" width="19.375" customWidth="1"/>
+    <col min="5" max="5" width="16.875" customWidth="1"/>
+    <col min="6" max="6" width="16.625" customWidth="1"/>
+    <col min="7" max="7" width="22.375" customWidth="1"/>
+    <col min="8" max="8" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="18">
       <c r="A1" s="78" t="s">
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="C1" s="79" t="s">
         <v>1</v>
@@ -1908,7 +1923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="111.95" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1916,57 +1931,57 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>217</v>
+        <v>161</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>211</v>
+        <v>162</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="82" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="83" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="82" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="82" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F3" s="82" t="s">
-        <v>213</v>
+        <v>164</v>
       </c>
       <c r="G3" s="82" t="s">
-        <v>214</v>
+        <v>165</v>
       </c>
       <c r="H3" s="82" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="I3" s="82" t="s">
-        <v>215</v>
+        <v>166</v>
       </c>
       <c r="J3" s="82" t="s">
-        <v>216</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1982,15 +1997,15 @@
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>1</v>
@@ -2004,7 +2019,7 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="113.1">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2012,36 +2027,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2058,17 +2073,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
     <col min="4" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>1</v>
@@ -2080,27 +2095,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="113.1">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D3" s="48"/>
       <c r="E3" s="10"/>
@@ -2120,80 +2135,80 @@
       <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="18">
       <c r="A3" s="72" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="72" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="72" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F3" s="72" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G3" s="72" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H3" s="72" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="I3" s="72" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="J3" s="72" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K3" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1"/>
       <c r="B4" s="73"/>
       <c r="G4" s="74"/>
       <c r="I4" s="75"/>
       <c r="K4" s="76"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="1"/>
       <c r="E5" s="77"/>
       <c r="F5" s="1"/>
       <c r="K5" s="76"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="1"/>
       <c r="B6" s="73"/>
       <c r="G6" s="74"/>
       <c r="K6" s="76"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="1"/>
       <c r="K7" s="76"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" s="1"/>
       <c r="K8" s="76"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" s="1"/>
       <c r="K9" s="76"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="1"/>
       <c r="K10" s="76"/>
     </row>
@@ -2210,15 +2225,15 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="2" t="s">
-        <v>160</v>
+        <v>179</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2232,7 +2247,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="141" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="141">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2240,48 +2255,48 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="G2" s="50" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H3" s="52" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2298,15 +2313,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -2314,34 +2329,34 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="84.95">
       <c r="A2" s="7" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
@@ -2359,9 +2374,9 @@
       <selection activeCell="H2" sqref="H2:I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="10.5" customWidth="1"/>
@@ -2371,9 +2386,9 @@
     <col min="10" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" s="2" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2389,7 +2404,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="49"/>
     </row>
-    <row r="2" spans="1:9" ht="141" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="141">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2397,54 +2412,54 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="I2" s="50" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E3" s="51" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="H3" s="52" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I3" s="52" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2461,15 +2476,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18.95">
       <c r="A1" s="53" t="s">
-        <v>166</v>
+        <v>195</v>
       </c>
       <c r="B1" s="54" t="s">
         <v>1</v>
@@ -2483,7 +2498,7 @@
       <c r="E1" s="56"/>
       <c r="F1" s="56"/>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="113.1">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2491,36 +2506,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2537,18 +2552,18 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.375" customWidth="1"/>
+    <col min="3" max="3" width="27.375" customWidth="1"/>
+    <col min="4" max="4" width="30.625" customWidth="1"/>
     <col min="5" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
@@ -2560,44 +2575,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2614,15 +2629,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>167</v>
+        <v>196</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2636,7 +2651,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="84.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2645,33 +2660,33 @@
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>169</v>
+        <v>198</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>171</v>
+        <v>200</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>172</v>
+        <v>201</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>174</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2688,15 +2703,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="18">
       <c r="A1" s="2" t="s">
-        <v>175</v>
+        <v>204</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2709,7 +2724,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="126.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2717,30 +2732,30 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2757,15 +2772,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="57" t="s">
-        <v>180</v>
+        <v>209</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2779,7 +2794,7 @@
       <c r="E1" s="58"/>
       <c r="F1" s="58"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="126.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2787,36 +2802,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>182</v>
+        <v>211</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2833,15 +2848,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>183</v>
+        <v>212</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2855,7 +2870,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="126.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2863,36 +2878,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>184</v>
+        <v>213</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2909,15 +2924,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>185</v>
+        <v>214</v>
       </c>
       <c r="B1" s="60" t="s">
         <v>1</v>
@@ -2931,7 +2946,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="126.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2939,36 +2954,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="D2" s="63" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2985,14 +3000,14 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="18">
       <c r="A1" s="64" t="s">
-        <v>188</v>
+        <v>217</v>
       </c>
       <c r="B1" s="65" t="s">
         <v>1</v>
@@ -3007,46 +3022,46 @@
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
     </row>
-    <row r="2" spans="1:7" ht="253" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="252.95">
       <c r="A2" s="68"/>
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="D2" s="69" t="s">
-        <v>189</v>
+        <v>218</v>
       </c>
       <c r="E2" s="69" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="F2" s="69" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="G2" s="69" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="70" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="70" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="71" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="71" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E3" s="71" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F3" s="70" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G3" s="70" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3067,15 +3082,15 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" s="17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3092,7 +3107,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="211" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="210.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3103,51 +3118,51 @@
         <v>6</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="43" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="42.95">
       <c r="A3" s="19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3164,15 +3179,15 @@
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="18">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3192,7 +3207,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="409.6">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3200,78 +3215,78 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="29.1">
+      <c r="A3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="K3" s="9" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>207</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -3288,18 +3303,18 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="11" width="10.5" customWidth="1"/>
     <col min="12" max="12" width="16.5" customWidth="1"/>
-    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="13" max="13" width="22.375" customWidth="1"/>
     <col min="14" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="18">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="3" t="s">
@@ -3319,7 +3334,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="183" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="183">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3327,78 +3342,78 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3415,23 +3430,23 @@
       <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="9" width="10.5" customWidth="1"/>
-    <col min="10" max="10" width="26.1640625" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" customWidth="1"/>
+    <col min="10" max="10" width="26.125" customWidth="1"/>
+    <col min="11" max="11" width="22.125" customWidth="1"/>
     <col min="12" max="14" width="10.5" customWidth="1"/>
-    <col min="15" max="15" width="24.33203125" customWidth="1"/>
+    <col min="15" max="15" width="24.375" customWidth="1"/>
     <col min="16" max="18" width="10.5" customWidth="1"/>
-    <col min="19" max="19" width="23.6640625" customWidth="1"/>
+    <col min="19" max="19" width="23.625" customWidth="1"/>
     <col min="20" max="20" width="20.5" customWidth="1"/>
     <col min="21" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="18">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3454,7 +3469,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="253" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="252.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3462,117 +3477,117 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="M3" s="24" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>209</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3589,26 +3604,26 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="19.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" style="25" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="26" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" style="26" customWidth="1"/>
-    <col min="5" max="7" width="30.1640625" style="26" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="26" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="26" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="26" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="11.125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="17.875" style="26" customWidth="1"/>
+    <col min="4" max="4" width="16.875" style="26" customWidth="1"/>
+    <col min="5" max="7" width="30.125" style="26" customWidth="1"/>
+    <col min="8" max="8" width="12.125" style="26" customWidth="1"/>
+    <col min="9" max="9" width="9.625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="14.625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="16.375" style="26" customWidth="1"/>
     <col min="12" max="12" width="16" style="26" customWidth="1"/>
-    <col min="13" max="14" width="6.33203125" style="26" customWidth="1"/>
-    <col min="15" max="1022" width="6.33203125" style="27" customWidth="1"/>
-    <col min="1023" max="1026" width="6.33203125" style="28" customWidth="1"/>
+    <col min="13" max="14" width="6.375" style="26" customWidth="1"/>
+    <col min="15" max="1022" width="6.375" style="27" customWidth="1"/>
+    <col min="1023" max="1026" width="6.375" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="18" customHeight="1">
       <c r="A1" s="29" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>1</v>
@@ -3620,7 +3635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="37" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" s="37" customFormat="1" ht="111.95">
       <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
@@ -3628,32 +3643,32 @@
         <v>5</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="G2" s="35"/>
       <c r="H2" s="35" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="L2" s="36" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="M2" s="36"/>
       <c r="N2" s="36"/>
@@ -3669,42 +3684,42 @@
       <c r="X2" s="36"/>
       <c r="Y2" s="36"/>
     </row>
-    <row r="3" spans="1:25" s="27" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:25" s="27" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G3" s="71" t="s">
-        <v>204</v>
+        <v>108</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="I3" s="40" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="K3" s="40" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="L3" s="41" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3725,15 +3740,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3749,7 +3764,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="225" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="225">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3757,48 +3772,48 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3809,21 +3824,23 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
+    <col min="3" max="19" width="10.5" customWidth="1"/>
+    <col min="20" max="20" width="14.75" customWidth="1"/>
+    <col min="21" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="18">
       <c r="A1" s="2" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3851,7 +3868,7 @@
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="333" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="306">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3859,120 +3876,126 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="51">
+      <c r="A3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="L3" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="M3" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="N3" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="O3" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="P3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="57" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="J3" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="K3" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="L3" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="M3" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="N3" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="O3" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="Q3" s="9" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="R3" s="19" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="T3" s="19" t="s">
-        <v>138</v>
+        <v>145</v>
+      </c>
+      <c r="U3" s="19" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new column to publish event
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23821"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brad.Sorour/Engine/hmcts/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C148134-567C-7947-B63A-CCF1251E7769}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{12EB3A57-41B9-487D-8977-86D9C3B5FB0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29580" windowHeight="17420" tabRatio="500" firstSheet="10" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29580" windowHeight="17420" tabRatio="500" firstSheet="11" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -39,8 +39,17 @@
     <sheet name="AuthorisationCaseState" sheetId="21" r:id="rId24"/>
     <sheet name="AuthorisationComplexType" sheetId="22" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191028" iterateDelta="1E-4" calcCompleted="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -49,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="220">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -81,6 +90,9 @@
 MaxLength: 100</t>
   </si>
   <si>
+    <t>This can have value TRUE/FALSE</t>
+  </si>
+  <si>
     <t>LiveFrom</t>
   </si>
   <si>
@@ -94,6 +106,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Shuttered</t>
   </si>
   <si>
     <t>CaseRoles</t>
@@ -185,6 +200,9 @@
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
+    <t>Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
+  </si>
+  <si>
     <t>Label</t>
   </si>
   <si>
@@ -204,6 +222,9 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>Searchable</t>
   </si>
   <si>
     <t>CaseTypeTab</t>
@@ -375,6 +396,9 @@
     <t>CaseEventFieldHint</t>
   </si>
   <si>
+    <t>RetainHiddenValue</t>
+  </si>
+  <si>
     <t>EventToComplexTypes</t>
   </si>
   <si>
@@ -392,6 +416,9 @@
   </si>
   <si>
     <t>ListElementCode</t>
+  </si>
+  <si>
+    <t>DefaultValue</t>
   </si>
   <si>
     <t>EventElementLabel</t>
@@ -485,6 +512,9 @@
 MaxLength: 200</t>
   </si>
   <si>
+    <t>Boolean value to say if an event can be published</t>
+  </si>
+  <si>
     <t>PreConditionState(s)</t>
   </si>
   <si>
@@ -519,6 +549,9 @@
   </si>
   <si>
     <t>EndButtonLabel</t>
+  </si>
+  <si>
+    <t>Publish</t>
   </si>
   <si>
     <t>FixedLists</t>
@@ -569,6 +602,31 @@
     <t>ElementLabel</t>
   </si>
   <si>
+    <t>ChallengeQuestion</t>
+  </si>
+  <si>
+    <t>Order of fields on UI
+Positive Integer</t>
+  </si>
+  <si>
+    <t>The type of the field that the answer will contain</t>
+  </si>
+  <si>
+    <t>In the form of a comma separated list of potential answer field(s) for each of the (n) litigant types on possible on the case.</t>
+  </si>
+  <si>
+    <t>QuestionText</t>
+  </si>
+  <si>
+    <t>AnswerFieldType</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>QuestionId</t>
+  </si>
+  <si>
     <t>SearchInputFields</t>
   </si>
   <si>
@@ -595,6 +653,15 @@
     <t>SearchAliasID</t>
   </si>
   <si>
+    <t>SearchCasesResultFields</t>
+  </si>
+  <si>
+    <t>ResultsOrdering</t>
+  </si>
+  <si>
+    <t>UseCase</t>
+  </si>
+  <si>
     <t>SearchResultFields</t>
   </si>
   <si>
@@ -609,10 +676,40 @@
 Positive Integer</t>
   </si>
   <si>
+    <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
+  </si>
+  <si>
+    <t>Fields can be ordered on by user role</t>
+  </si>
+  <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>Yes or No, to enable or disable the banner.                          MaxLength: 30</t>
+  </si>
+  <si>
+    <t>Content to display in the banner         MaxLength: 300</t>
+  </si>
+  <si>
+    <t>Optional link text in the banner                   MaxLength:50</t>
+  </si>
+  <si>
+    <t>The URL for the link text.                                               Max Length: 1000</t>
+  </si>
+  <si>
+    <t>BannerEnabled</t>
+  </si>
+  <si>
+    <t>BannerDescription</t>
+  </si>
+  <si>
+    <t>BannerUrlText</t>
+  </si>
+  <si>
+    <t>BannerUrl</t>
+  </si>
+  <si>
     <t>WorkBasketResultFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
   </si>
   <si>
     <t>WorkBasketInputFields</t>
@@ -700,88 +797,6 @@
   <si>
     <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
-  </si>
-  <si>
-    <t>ResultsOrdering</t>
-  </si>
-  <si>
-    <t>Fields can be ordered on by user role</t>
-  </si>
-  <si>
-    <t>Shuttered</t>
-  </si>
-  <si>
-    <t>This can have value TRUE/FALSE</t>
-  </si>
-  <si>
-    <t>Banner</t>
-  </si>
-  <si>
-    <t>Yes or No, to enable or disable the banner.                          MaxLength: 30</t>
-  </si>
-  <si>
-    <t>Content to display in the banner         MaxLength: 300</t>
-  </si>
-  <si>
-    <t>Optional link text in the banner                   MaxLength:50</t>
-  </si>
-  <si>
-    <t>The URL for the link text.                                               Max Length: 1000</t>
-  </si>
-  <si>
-    <t>BannerEnabled</t>
-  </si>
-  <si>
-    <t>BannerDescription</t>
-  </si>
-  <si>
-    <t>BannerUrlText</t>
-  </si>
-  <si>
-    <t>BannerUrl</t>
-  </si>
-  <si>
-    <t>DefaultValue</t>
-  </si>
-  <si>
-    <t>SearchCasesResultFields</t>
-  </si>
-  <si>
-    <t>UseCase</t>
-  </si>
-  <si>
-    <t>Searchable</t>
-  </si>
-  <si>
-    <t>Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
-  </si>
-  <si>
-    <t>RetainHiddenValue</t>
-  </si>
-  <si>
-    <t>ChallengeQuestion</t>
-  </si>
-  <si>
-    <t>The type of the field that the answer will contain</t>
-  </si>
-  <si>
-    <t>In the form of a comma separated list of potential answer field(s) for each of the (n) litigant types on possible on the case.</t>
-  </si>
-  <si>
-    <t>QuestionText</t>
-  </si>
-  <si>
-    <t>AnswerFieldType</t>
-  </si>
-  <si>
-    <t>Answer</t>
-  </si>
-  <si>
-    <t>QuestionId</t>
-  </si>
-  <si>
-    <t>Order of fields on UI
-Positive Integer</t>
   </si>
 </sst>
 </file>
@@ -792,7 +807,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="35">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1596,13 +1611,13 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1617,7 +1632,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="126.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1634,27 +1649,27 @@
         <v>8</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>193</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1671,15 +1686,15 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1692,7 +1707,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="84.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1700,36 +1715,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1746,17 +1761,17 @@
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="14" width="10.5" customWidth="1"/>
-    <col min="15" max="15" width="26.83203125" customWidth="1"/>
+    <col min="15" max="15" width="26.875" customWidth="1"/>
     <col min="16" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="18">
       <c r="A1" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1777,7 +1792,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="409.6">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1785,87 +1800,87 @@
         <v>5</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="I3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>40</v>
-      </c>
       <c r="K3" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>207</v>
+        <v>49</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>209</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1878,25 +1893,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD9C6E9-A135-BB4B-AB3F-8180231A4906}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.875" customWidth="1"/>
+    <col min="2" max="2" width="21.625" customWidth="1"/>
+    <col min="3" max="3" width="26.625" customWidth="1"/>
+    <col min="4" max="4" width="19.375" customWidth="1"/>
+    <col min="5" max="5" width="16.875" customWidth="1"/>
+    <col min="6" max="6" width="16.625" customWidth="1"/>
+    <col min="7" max="7" width="22.375" customWidth="1"/>
+    <col min="8" max="8" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="18">
       <c r="A1" s="78" t="s">
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="C1" s="79" t="s">
         <v>1</v>
@@ -1908,7 +1923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="111.95" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1916,57 +1931,57 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>217</v>
+        <v>161</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>211</v>
+        <v>162</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="82" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="83" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="82" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="82" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F3" s="82" t="s">
-        <v>213</v>
+        <v>164</v>
       </c>
       <c r="G3" s="82" t="s">
-        <v>214</v>
+        <v>165</v>
       </c>
       <c r="H3" s="82" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="I3" s="82" t="s">
-        <v>215</v>
+        <v>166</v>
       </c>
       <c r="J3" s="82" t="s">
-        <v>216</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1982,15 +1997,15 @@
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>1</v>
@@ -2004,7 +2019,7 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="113.1">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2012,36 +2027,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2058,17 +2073,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
     <col min="4" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>1</v>
@@ -2080,27 +2095,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="113.1">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D3" s="48"/>
       <c r="E3" s="10"/>
@@ -2120,80 +2135,80 @@
       <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="18">
       <c r="A3" s="72" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="72" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="72" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E3" s="72" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F3" s="72" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G3" s="72" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H3" s="72" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="I3" s="72" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="J3" s="72" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K3" s="72" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1"/>
       <c r="B4" s="73"/>
       <c r="G4" s="74"/>
       <c r="I4" s="75"/>
       <c r="K4" s="76"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="1"/>
       <c r="E5" s="77"/>
       <c r="F5" s="1"/>
       <c r="K5" s="76"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="1"/>
       <c r="B6" s="73"/>
       <c r="G6" s="74"/>
       <c r="K6" s="76"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="1"/>
       <c r="K7" s="76"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" s="1"/>
       <c r="K8" s="76"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" s="1"/>
       <c r="K9" s="76"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="1"/>
       <c r="K10" s="76"/>
     </row>
@@ -2210,15 +2225,15 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="2" t="s">
-        <v>160</v>
+        <v>179</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2232,7 +2247,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="141" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="141">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2240,48 +2255,48 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="G2" s="50" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="H3" s="52" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2298,15 +2313,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -2314,34 +2329,34 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="84.95">
       <c r="A2" s="7" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="20"/>
@@ -2359,9 +2374,9 @@
       <selection activeCell="H2" sqref="H2:I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="10.5" customWidth="1"/>
@@ -2371,9 +2386,9 @@
     <col min="10" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" s="2" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2389,7 +2404,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="49"/>
     </row>
-    <row r="2" spans="1:9" ht="141" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="141">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2397,54 +2412,54 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="I2" s="50" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E3" s="51" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="H3" s="52" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I3" s="52" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2461,15 +2476,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18.95">
       <c r="A1" s="53" t="s">
-        <v>166</v>
+        <v>195</v>
       </c>
       <c r="B1" s="54" t="s">
         <v>1</v>
@@ -2483,7 +2498,7 @@
       <c r="E1" s="56"/>
       <c r="F1" s="56"/>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="113.1">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2491,36 +2506,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2537,18 +2552,18 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.375" customWidth="1"/>
+    <col min="3" max="3" width="27.375" customWidth="1"/>
+    <col min="4" max="4" width="30.625" customWidth="1"/>
     <col min="5" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
@@ -2560,44 +2575,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2614,15 +2629,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>167</v>
+        <v>196</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2636,7 +2651,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="84.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2645,33 +2660,33 @@
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>169</v>
+        <v>198</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>171</v>
+        <v>200</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>172</v>
+        <v>201</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>174</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2688,15 +2703,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="18">
       <c r="A1" s="2" t="s">
-        <v>175</v>
+        <v>204</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2709,7 +2724,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="126.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2717,30 +2732,30 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2757,15 +2772,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="57" t="s">
-        <v>180</v>
+        <v>209</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2779,7 +2794,7 @@
       <c r="E1" s="58"/>
       <c r="F1" s="58"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="126.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2787,36 +2802,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>182</v>
+        <v>211</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2833,15 +2848,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>183</v>
+        <v>212</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2855,7 +2870,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="126.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2863,36 +2878,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>184</v>
+        <v>213</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2909,15 +2924,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18">
       <c r="A1" s="2" t="s">
-        <v>185</v>
+        <v>214</v>
       </c>
       <c r="B1" s="60" t="s">
         <v>1</v>
@@ -2931,7 +2946,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="126.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2939,36 +2954,36 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="D2" s="63" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2985,14 +3000,14 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="18">
       <c r="A1" s="64" t="s">
-        <v>188</v>
+        <v>217</v>
       </c>
       <c r="B1" s="65" t="s">
         <v>1</v>
@@ -3007,46 +3022,46 @@
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
     </row>
-    <row r="2" spans="1:7" ht="253" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="252.95">
       <c r="A2" s="68"/>
       <c r="B2" s="68"/>
       <c r="C2" s="69" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="D2" s="69" t="s">
-        <v>189</v>
+        <v>218</v>
       </c>
       <c r="E2" s="69" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="F2" s="69" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="G2" s="69" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="70" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="70" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="71" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="71" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E3" s="71" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F3" s="70" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G3" s="70" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3067,15 +3082,15 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" s="17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3092,7 +3107,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="211" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="210.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3103,51 +3118,51 @@
         <v>6</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="43" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="42.95">
       <c r="A3" s="19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3164,15 +3179,15 @@
       <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="18">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3192,7 +3207,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="409.6">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3200,78 +3215,78 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="29.1">
+      <c r="A3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="K3" s="9" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>207</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -3288,18 +3303,18 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="11" width="10.5" customWidth="1"/>
     <col min="12" max="12" width="16.5" customWidth="1"/>
-    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="13" max="13" width="22.375" customWidth="1"/>
     <col min="14" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="18">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="3" t="s">
@@ -3319,7 +3334,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="183" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="183">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3327,78 +3342,78 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3415,23 +3430,23 @@
       <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="9" width="10.5" customWidth="1"/>
-    <col min="10" max="10" width="26.1640625" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" customWidth="1"/>
+    <col min="10" max="10" width="26.125" customWidth="1"/>
+    <col min="11" max="11" width="22.125" customWidth="1"/>
     <col min="12" max="14" width="10.5" customWidth="1"/>
-    <col min="15" max="15" width="24.33203125" customWidth="1"/>
+    <col min="15" max="15" width="24.375" customWidth="1"/>
     <col min="16" max="18" width="10.5" customWidth="1"/>
-    <col min="19" max="19" width="23.6640625" customWidth="1"/>
+    <col min="19" max="19" width="23.625" customWidth="1"/>
     <col min="20" max="20" width="20.5" customWidth="1"/>
     <col min="21" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="18">
       <c r="A1" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3454,7 +3469,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="253" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="252.95">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3462,117 +3477,117 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="M3" s="24" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>209</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3589,26 +3604,26 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="19.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" style="25" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="26" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" style="26" customWidth="1"/>
-    <col min="5" max="7" width="30.1640625" style="26" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="26" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" style="26" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="26" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="11.125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="17.875" style="26" customWidth="1"/>
+    <col min="4" max="4" width="16.875" style="26" customWidth="1"/>
+    <col min="5" max="7" width="30.125" style="26" customWidth="1"/>
+    <col min="8" max="8" width="12.125" style="26" customWidth="1"/>
+    <col min="9" max="9" width="9.625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="14.625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="16.375" style="26" customWidth="1"/>
     <col min="12" max="12" width="16" style="26" customWidth="1"/>
-    <col min="13" max="14" width="6.33203125" style="26" customWidth="1"/>
-    <col min="15" max="1022" width="6.33203125" style="27" customWidth="1"/>
-    <col min="1023" max="1026" width="6.33203125" style="28" customWidth="1"/>
+    <col min="13" max="14" width="6.375" style="26" customWidth="1"/>
+    <col min="15" max="1022" width="6.375" style="27" customWidth="1"/>
+    <col min="1023" max="1026" width="6.375" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="18" customHeight="1">
       <c r="A1" s="29" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>1</v>
@@ -3620,7 +3635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="37" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" s="37" customFormat="1" ht="111.95">
       <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
@@ -3628,32 +3643,32 @@
         <v>5</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="G2" s="35"/>
       <c r="H2" s="35" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="L2" s="36" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="M2" s="36"/>
       <c r="N2" s="36"/>
@@ -3669,42 +3684,42 @@
       <c r="X2" s="36"/>
       <c r="Y2" s="36"/>
     </row>
-    <row r="3" spans="1:25" s="27" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:25" s="27" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G3" s="71" t="s">
-        <v>204</v>
+        <v>108</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="I3" s="40" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="K3" s="40" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="L3" s="41" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3725,15 +3740,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="2" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3749,7 +3764,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="225" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="225">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3757,48 +3772,48 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3809,21 +3824,23 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
+    <col min="1" max="2" width="10.875" style="1" customWidth="1"/>
+    <col min="3" max="19" width="10.5" customWidth="1"/>
+    <col min="20" max="20" width="14.75" customWidth="1"/>
+    <col min="21" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="18">
       <c r="A1" s="2" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3851,7 +3868,7 @@
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="333" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="306">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3859,120 +3876,126 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="51">
+      <c r="A3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="L3" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="M3" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="N3" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="O3" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="P3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="57" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="J3" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="K3" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="L3" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="M3" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="N3" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="O3" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="Q3" s="9" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="R3" s="19" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="T3" s="19" t="s">
-        <v>138</v>
+        <v>145</v>
+      </c>
+      <c r="U3" s="19" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new publish column to CaseEventToFields Tab
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23821"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23921"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brad.Sorour/Engine/hmcts/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12EB3A57-41B9-487D-8977-86D9C3B5FB0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8879E7F5-0DF0-401C-B4C3-48F80A3B3148}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29580" windowHeight="17420" tabRatio="500" firstSheet="11" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29580" windowHeight="17420" tabRatio="500" firstSheet="8" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="220">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -354,6 +354,9 @@
     <t>This is a string value overrides hint from CaseField tab</t>
   </si>
   <si>
+    <t>Boolean value to say if an event can be published</t>
+  </si>
+  <si>
     <t>CaseEventID</t>
   </si>
   <si>
@@ -397,6 +400,9 @@
   </si>
   <si>
     <t>RetainHiddenValue</t>
+  </si>
+  <si>
+    <t>Publish</t>
   </si>
   <si>
     <t>EventToComplexTypes</t>
@@ -512,9 +518,6 @@
 MaxLength: 200</t>
   </si>
   <si>
-    <t>Boolean value to say if an event can be published</t>
-  </si>
-  <si>
     <t>PreConditionState(s)</t>
   </si>
   <si>
@@ -549,9 +552,6 @@
   </si>
   <si>
     <t>EndButtonLabel</t>
-  </si>
-  <si>
-    <t>Publish</t>
   </si>
   <si>
     <t>FixedLists</t>
@@ -1738,13 +1738,13 @@
         <v>12</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>152</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1847,7 +1847,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>44</v>
@@ -1880,7 +1880,7 @@
         <v>49</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1940,7 +1940,7 @@
         <v>161</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>162</v>
@@ -1966,7 +1966,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="82" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F3" s="82" t="s">
         <v>164</v>
@@ -2056,7 +2056,7 @@
         <v>42</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2159,13 +2159,13 @@
         <v>65</v>
       </c>
       <c r="F3" s="72" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G3" s="72" t="s">
         <v>42</v>
       </c>
       <c r="H3" s="72" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I3" s="72" t="s">
         <v>177</v>
@@ -2290,7 +2290,7 @@
         <v>42</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G3" s="52" t="s">
         <v>66</v>
@@ -2447,13 +2447,13 @@
         <v>65</v>
       </c>
       <c r="E3" s="51" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>42</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H3" s="52" t="s">
         <v>66</v>
@@ -2535,7 +2535,7 @@
         <v>42</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2901,7 +2901,7 @@
         <v>19</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E3" s="59" t="s">
         <v>66</v>
@@ -3055,7 +3055,7 @@
         <v>65</v>
       </c>
       <c r="E3" s="71" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F3" s="70" t="s">
         <v>66</v>
@@ -3424,10 +3424,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
@@ -3444,7 +3444,7 @@
     <col min="21" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18">
+    <row r="1" spans="1:21" ht="18">
       <c r="A1" s="2" t="s">
         <v>71</v>
       </c>
@@ -3469,7 +3469,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:20" ht="252.95">
+    <row r="2" spans="1:21" ht="293.25">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3527,8 +3527,11 @@
       <c r="S2" s="7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="U2" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15.75">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -3539,55 +3542,58 @@
         <v>19</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>65</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>68</v>
       </c>
       <c r="M3" s="24" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
+      </c>
+      <c r="U3" s="19" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -3623,7 +3629,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="18" customHeight="1">
       <c r="A1" s="29" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>1</v>
@@ -3643,7 +3649,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D2" s="35" t="s">
         <v>72</v>
@@ -3652,14 +3658,14 @@
         <v>73</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G2" s="35"/>
       <c r="H2" s="35" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J2" s="35" t="s">
         <v>74</v>
@@ -3695,28 +3701,28 @@
         <v>12</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E3" s="39" t="s">
         <v>65</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G3" s="71" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I3" s="40" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K3" s="40" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L3" s="41" t="s">
         <v>68</v>
@@ -3748,7 +3754,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18">
       <c r="A1" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3775,19 +3781,19 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3810,10 +3816,10 @@
         <v>14</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3826,8 +3832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="I2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
@@ -3840,7 +3846,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="18">
       <c r="A1" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -3879,58 +3885,58 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>26</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>133</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="51">
@@ -3953,49 +3959,49 @@
         <v>14</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J3" s="42" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K3" s="42" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L3" s="42" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M3" s="42" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="N3" s="42" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="O3" s="42" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>30</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="R3" s="19" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="T3" s="19" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U3" s="19" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Add support for conditional events (EventEnablingCondition filed)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,40 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomaszp/fpla/ccd-definition-processor/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFF134C-2529-6947-A536-E824BEA9E2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Jurisdiction" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="CaseRoles" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="CaseType" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="CaseField" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="CaseTypeTab" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="CaseEventToFields" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="CaseEventToComplexTypes" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="State" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="CaseEvent" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="FixedLists" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="ComplexTypes" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="ChallengeQuestion" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="SearchInputFields" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="SearchAlias" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="SearchCasesResultFields" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="SearchResultFields" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="Banner" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="WorkBasketResultFields" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="WorkBasketInputFields" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="UserProfile" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="AuthorisationCaseType" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="AuthorisationCaseField" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="AuthorisationCaseState" sheetId="24" state="visible" r:id="rId25"/>
-    <sheet name="AuthorisationComplexType" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
+    <sheet name="CaseRoles" sheetId="2" r:id="rId2"/>
+    <sheet name="CaseType" sheetId="3" r:id="rId3"/>
+    <sheet name="CaseField" sheetId="4" r:id="rId4"/>
+    <sheet name="CaseTypeTab" sheetId="5" r:id="rId5"/>
+    <sheet name="CaseEventToFields" sheetId="6" r:id="rId6"/>
+    <sheet name="CaseEventToComplexTypes" sheetId="7" r:id="rId7"/>
+    <sheet name="State" sheetId="8" r:id="rId8"/>
+    <sheet name="CaseEvent" sheetId="9" r:id="rId9"/>
+    <sheet name="FixedLists" sheetId="10" r:id="rId10"/>
+    <sheet name="ComplexTypes" sheetId="11" r:id="rId11"/>
+    <sheet name="ChallengeQuestion" sheetId="12" r:id="rId12"/>
+    <sheet name="SearchInputFields" sheetId="13" r:id="rId13"/>
+    <sheet name="SearchAlias" sheetId="14" r:id="rId14"/>
+    <sheet name="SearchCasesResultFields" sheetId="15" r:id="rId15"/>
+    <sheet name="SearchResultFields" sheetId="16" r:id="rId16"/>
+    <sheet name="Banner" sheetId="17" r:id="rId17"/>
+    <sheet name="WorkBasketResultFields" sheetId="18" r:id="rId18"/>
+    <sheet name="WorkBasketInputFields" sheetId="19" r:id="rId19"/>
+    <sheet name="UserProfile" sheetId="20" r:id="rId20"/>
+    <sheet name="AuthorisationCaseType" sheetId="21" r:id="rId21"/>
+    <sheet name="AuthorisationCaseField" sheetId="22" r:id="rId22"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="23" r:id="rId23"/>
+    <sheet name="AuthorisationCaseState" sheetId="24" r:id="rId24"/>
+    <sheet name="AuthorisationComplexType" sheetId="25" r:id="rId25"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -44,760 +49,759 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="220">
-  <si>
-    <t xml:space="preserve">Jurisdiction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrimaryKeyInRed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrimaryAndForeignKey Orange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ForeignKey Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start date from which the data will be valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End date until which the data will be valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The identifier which defines the casetype code
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="221">
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t>PrimaryKeyInRed</t>
+  </si>
+  <si>
+    <t>PrimaryAndForeignKey Orange</t>
+  </si>
+  <si>
+    <t>ForeignKey Brown</t>
+  </si>
+  <si>
+    <t>Start date from which the data will be valid</t>
+  </si>
+  <si>
+    <t>End date until which the data will be valid</t>
+  </si>
+  <si>
+    <t>The identifier which defines the casetype code
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The short description to describe the jurisdiction used on UI display
+    <t>The short description to describe the jurisdiction used on UI display
 MaxLength: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">The long description to describe the jurisdiction.
+    <t>The long description to describe the jurisdiction.
 MaxLength: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">This can have value TRUE/FALSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LiveFrom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LiveTo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shuttered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseRoles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength: 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength:128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The short description to describe the case type used on the UI.
+    <t>This can have value TRUE/FALSE</t>
+  </si>
+  <si>
+    <t>LiveFrom</t>
+  </si>
+  <si>
+    <t>LiveTo</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Shuttered</t>
+  </si>
+  <si>
+    <t>CaseRoles</t>
+  </si>
+  <si>
+    <t>MaxLength: 40</t>
+  </si>
+  <si>
+    <t>MaxLength:128</t>
+  </si>
+  <si>
+    <t>CaseTypeID</t>
+  </si>
+  <si>
+    <t>CaseType</t>
+  </si>
+  <si>
+    <t>The short description to describe the case type used on the UI.
 MaxLength: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">The long description to decribe the case type.
+    <t>The long description to decribe the case type.
 MaxLength: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">The jurisdiction code should match the one defined in 'Jurisdiction' tab
+    <t>The jurisdiction code should match the one defined in 'Jurisdiction' tab
 MaxLength:70</t>
   </si>
   <si>
-    <t xml:space="preserve">The absolute URL to the microservice which lists the documents that the services wants to provide for print. 
+    <t>The absolute URL to the microservice which lists the documents that the services wants to provide for print. 
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). Max Length: 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It is a mandatory field which can define if the data classification of the field
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). Max Length: 20</t>
+  </si>
+  <si>
+    <t>It is a mandatory field which can define if the data classification of the field
 MustBe: &lt;Public, Private, Retricted&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">JurisdictionID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrintableDocumentsUrl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLPrintEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SecurityClassification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseField</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The code of casetype has to be defined in 'CaseType' tab
+    <t>JurisdictionID</t>
+  </si>
+  <si>
+    <t>PrintableDocumentsUrl</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLPrintEvent</t>
+  </si>
+  <si>
+    <t>SecurityClassification</t>
+  </si>
+  <si>
+    <t>CaseField</t>
+  </si>
+  <si>
+    <t>The code of casetype has to be defined in 'CaseType' tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The field ID should match the field attribute name used by the service team in creating the case
+    <t>The field ID should match the field attribute name used by the service team in creating the case
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
+    <t>The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
 MaxLength:&lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The hint text that is present for each field type
+    <t>The hint text that is present for each field type
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The type of field. This can be a CCD Base type (see confluence) or a ComplexType ID as per the ComplexType tab).  
+    <t>The type of field. This can be a CCD Base type (see confluence) or a ComplexType ID as per the ComplexType tab).  
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Some FieldTypes require or have an optional addition parameter that can be set (e.g. Collection - the parameter is the collecion of What FieldType ?, FixedList the parameter is the ID from the fixedList tab). See confluence for details
+    <t>Some FieldTypes require or have an optional addition parameter that can be set (e.g. Collection - the parameter is the collecion of What FieldType ?, FixedList the parameter is the ID from the fixedList tab). See confluence for details
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">The regex that can define the type of data accepted in the fields E.g: alphanumeric etc. This will override the regex, if defined internally for any type.
+    <t>The regex that can define the type of data accepted in the fields E.g: alphanumeric etc. This will override the regex, if defined internally for any type.
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The minimum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
+    <t>The minimum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The maximum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
+    <t>The maximum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HintText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldTypeParameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RegularExpression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Searchable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseTypeTab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not used yet - maybe used for roletype type view later
+    <t>Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>HintText</t>
+  </si>
+  <si>
+    <t>FieldType</t>
+  </si>
+  <si>
+    <t>FieldTypeParameter</t>
+  </si>
+  <si>
+    <t>RegularExpression</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Searchable</t>
+  </si>
+  <si>
+    <t>CaseTypeTab</t>
+  </si>
+  <si>
+    <t>Not used yet - maybe used for roletype type view later
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">Unique Id for tab. MaxLength: 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name to be displayed on the tab
+    <t>Unique Id for tab. MaxLength: 40</t>
+  </si>
+  <si>
+    <t>Name to be displayed on the tab
 MaxLengh: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">Order of Tab on screen - left to right.
+    <t>Order of Tab on screen - left to right.
 PositiveInteger</t>
   </si>
   <si>
-    <t xml:space="preserve">Unique ID for field - must match an ID on the CaseField tab or be a metadata item. 
+    <t>Unique ID for field - must match an ID on the CaseField tab or be a metadata item. 
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order of Fields within a tab - top to bottom
+    <t>MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
+  </si>
+  <si>
+    <t>Order of Fields within a tab - top to bottom
 PositiveInteger</t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
+    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
 MaxLength:1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean expression rules for hiding a tab: 
+    <t>Boolean expression rules for hiding a tab: 
 MaxLength:1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Text should begin with #LIST( or #TABLE(
+    <t>Text should begin with #LIST( or #TABLE(
 MaxLength: 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Channel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseFieldID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserRole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabFieldDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldShowCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabShowCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DisplayContextParameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventToFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique ID for the event. Not listing an case event means that All Fields are displayed. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This defines with Fields can be changed / viewed during an case event. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The order of the fields on the screen.
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>TabID</t>
+  </si>
+  <si>
+    <t>TabLabel</t>
+  </si>
+  <si>
+    <t>TabDisplayOrder</t>
+  </si>
+  <si>
+    <t>CaseFieldID</t>
+  </si>
+  <si>
+    <t>UserRole</t>
+  </si>
+  <si>
+    <t>TabFieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>FieldShowCondition</t>
+  </si>
+  <si>
+    <t>TabShowCondition</t>
+  </si>
+  <si>
+    <t>DisplayContextParameter</t>
+  </si>
+  <si>
+    <t>CaseEventToFields</t>
+  </si>
+  <si>
+    <t>Unique ID for the event. Not listing an case event means that All Fields are displayed. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>This defines with Fields can be changed / viewed during an case event. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>The order of the fields on the screen.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted Values:  for mandatory, readonly and optional data on UI
+    <t>Accepted Values:  for mandatory, readonly and optional data on UI
 MustBe: MANDATORY, READONLY, OPTIONAL</t>
   </si>
   <si>
-    <t xml:space="preserve">This is a string value which defines the Wizard pages' ID
+    <t>This is a string value which defines the Wizard pages' ID
 MaxLength:40</t>
   </si>
   <si>
-    <t xml:space="preserve">This is a string value which defines the Wizard pages' Label
+    <t>This is a string value which defines the Wizard pages' Label
 MaxLength:40</t>
   </si>
   <si>
-    <t xml:space="preserve">The order to display the pages
+    <t>The order to display the pages
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Currently blank 1 or 2.  2 currently will display the yellow review column.
+    <t>Currently blank 1 or 2.  2 currently will display the yellow review column.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
+    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
 MaxLength: 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean expression rules for hiding a page: MaxLength:1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">States a field should appear on check your answers However these fields will be considered only "ShowSummary" column in CaseEvent tab is set to Y
+    <t>Boolean expression rules for hiding a page: MaxLength:1000</t>
+  </si>
+  <si>
+    <t>States a field should appear on check your answers However these fields will be considered only "ShowSummary" column in CaseEvent tab is set to Y
 CouldBe: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">URL to call back to the service for uniqueness. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a string value overrides label from CaseField tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a string value overrides hint from CaseField tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boolean value to say if an event can be published</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageFieldDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DisplayContext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageColumnNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageShowCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowSummaryChangeOption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowSummaryContentOption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLMidEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLMidEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventFieldLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventFieldHint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetainHiddenValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Publish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventToComplexTypes</t>
+    <t>URL to call back to the service for uniqueness. </t>
+  </si>
+  <si>
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). </t>
+  </si>
+  <si>
+    <t>This is a string value overrides label from CaseField tab</t>
+  </si>
+  <si>
+    <t>This is a string value overrides hint from CaseField tab</t>
+  </si>
+  <si>
+    <t>Boolean value to say if an event can be published</t>
+  </si>
+  <si>
+    <t>CaseEventID</t>
+  </si>
+  <si>
+    <t>PageFieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>DisplayContext</t>
+  </si>
+  <si>
+    <t>PageID</t>
+  </si>
+  <si>
+    <t>PageLabel</t>
+  </si>
+  <si>
+    <t>PageDisplayOrder</t>
+  </si>
+  <si>
+    <t>PageColumnNumber</t>
+  </si>
+  <si>
+    <t>PageShowCondition</t>
+  </si>
+  <si>
+    <t>ShowSummaryChangeOption</t>
+  </si>
+  <si>
+    <t>ShowSummaryContentOption</t>
+  </si>
+  <si>
+    <t>CallBackURLMidEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLMidEvent</t>
+  </si>
+  <si>
+    <t>CaseEventFieldLabel</t>
+  </si>
+  <si>
+    <t>CaseEventFieldHint</t>
+  </si>
+  <si>
+    <t>RetainHiddenValue</t>
+  </si>
+  <si>
+    <t>Publish</t>
+  </si>
+  <si>
+    <t>EventToComplexTypes</t>
   </si>
   <si>
     <t xml:space="preserve">
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">MaxLength:70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength:200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength:300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ListElementCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DefaultValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventElementLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventHintText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State with ID '*' and Name 'DEFAULT' is a reserved state. The state can be used for events where states do not change.
+    <t>MaxLength:70</t>
+  </si>
+  <si>
+    <t>MaxLength:200</t>
+  </si>
+  <si>
+    <t>MaxLength:300</t>
+  </si>
+  <si>
+    <t>ListElementCode</t>
+  </si>
+  <si>
+    <t>DefaultValue</t>
+  </si>
+  <si>
+    <t>EventElementLabel</t>
+  </si>
+  <si>
+    <t>EventHintText</t>
+  </si>
+  <si>
+    <t>FieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>State with ID '*' and Name 'DEFAULT' is a reserved state. The state can be used for events where states do not change.
 MaxLength:70</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the name of the state as displayed on UI
+    <t>This is the name of the state as displayed on UI
 MaxLength:100</t>
   </si>
   <si>
-    <t xml:space="preserve">This gives longer decription of the case state
+    <t>This gives longer decription of the case state
 Max Length: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">The order of the states on the screen.
+    <t>The order of the states on the screen.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Optional override of title used in the CaseTabView. Markdown , concat supported
+    <t>Optional override of title used in the CaseTabView. Markdown , concat supported
 MaxLength: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">DisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TitleDisplay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique ID for the event
+    <t>DisplayOrder</t>
+  </si>
+  <si>
+    <t>TitleDisplay</t>
+  </si>
+  <si>
+    <t>CaseEvent</t>
+  </si>
+  <si>
+    <t>Unique ID for the event
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the name of the event as displayed on UI Dropdown list - hence limited to 30
+    <t>This is the name of the event as displayed on UI Dropdown list - hence limited to 30
 MaxLength: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">This gives further details of an event of a case
+    <t>This gives further details of an event of a case
 MaxLength:100</t>
   </si>
   <si>
-    <t xml:space="preserve">The display order of displaying the events in the list
+    <t>The display order of displaying the events in the list
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Future Elements not for MVP (what about multiple state) (semicolon ; seprated list).
+    <t>Future Elements not for MVP (what about multiple state) (semicolon ; seprated list).
 If '*' is provided, then precondition will not be validated and will be considered as current state
  MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Future Elements not for MVP. 
+    <t>Future Elements not for MVP. 
 If '*' is provided, then the current state will not change and will be same as pre condition state
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">URL to call back to the service for uniqueness. 
+    <t>URL to call back to the service for uniqueness. 
 Max Length: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). 
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). 
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Y, N and empty. TheCheck your answer section will be shown on Y (true) and empty(null) values, but not shown on N (false) values. Fields on CaseEventTo Field tab have Y in "ShowSummaryChangeOption" column.
+    <t>Y, N and empty. TheCheck your answer section will be shown on Y (true) and empty(null) values, but not shown on N (false) values. Fields on CaseEventTo Field tab have Y in "ShowSummaryChangeOption" column.
 CouldBe: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean value to say if the enter summary and event description fields are to be shown
+    <t>Boolean value to say if the enter summary and event description fields are to be shown
 CouldBeh: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean value to say if a draft of a create event can be saved
+    <t>Boolean value to say if a draft of a create event can be saved
 CouldBe: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The label of the button on the final event screen - default is Submit
+    <t>The label of the button on the final event screen - default is Submit
 MaxLength: 200</t>
   </si>
   <si>
-    <t xml:space="preserve">PreConditionState(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PostConditionState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLAboutToStartEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutAboutToStartEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLAboutToSubmitEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLAboutToSubmitEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLSubmittedEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLSubmittedEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowSummary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowEventNotes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CanSaveDraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndButtonLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FixedLists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The unique identifier of the Fixed list
+    <t>PreConditionState(s)</t>
+  </si>
+  <si>
+    <t>PostConditionState</t>
+  </si>
+  <si>
+    <t>CallBackURLAboutToStartEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutAboutToStartEvent</t>
+  </si>
+  <si>
+    <t>CallBackURLAboutToSubmitEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLAboutToSubmitEvent</t>
+  </si>
+  <si>
+    <t>CallBackURLSubmittedEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLSubmittedEvent</t>
+  </si>
+  <si>
+    <t>ShowSummary</t>
+  </si>
+  <si>
+    <t>ShowEventNotes</t>
+  </si>
+  <si>
+    <t>CanSaveDraft</t>
+  </si>
+  <si>
+    <t>EndButtonLabel</t>
+  </si>
+  <si>
+    <t>FixedLists</t>
+  </si>
+  <si>
+    <t>The unique identifier of the Fixed list
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">The unque ID of an element in the list (ID)
+    <t>The unque ID of an element in the list (ID)
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">The Display name for the list item
+    <t>The Display name for the list item
 MaxLength: 250</t>
   </si>
   <si>
-    <t xml:space="preserve">The display order of list items. Positive integers e.g 1, 2, 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ListElement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ComplexTypes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The ComplexType ID should match the field attribute name on the CaseField Tab
+    <t>The display order of list items. Positive integers e.g 1, 2, 3</t>
+  </si>
+  <si>
+    <t>ListElement</t>
+  </si>
+  <si>
+    <t>ComplexTypes</t>
+  </si>
+  <si>
+    <t>The ComplexType ID should match the field attribute name on the CaseField Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The complex type element (field) ID (ListElementId) should match the field attribute name used by the service team in creating the case
+    <t>The complex type element (field) ID (ListElementId) should match the field attribute name used by the service team in creating the case
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
+    <t>The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
 MaxLength:200</t>
   </si>
   <si>
-    <t xml:space="preserve">Within a complex type any field can be hidden or shown based on another field's values in the same level.
+    <t>Within a complex type any field can be hidden or shown based on another field's values in the same level.
 Currently only single boolean or string conditions are supported. Eg: country="Italy" or country startWith: "Uni"
 MaxLength: 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">The hint text that is present for each field type
+    <t>The hint text that is present for each field type
 MaxLength: &lt;unlmited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">ElementLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChallengeQuestion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order of fields on UI
+    <t>ElementLabel</t>
+  </si>
+  <si>
+    <t>ChallengeQuestion</t>
+  </si>
+  <si>
+    <t>Order of fields on UI
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">The type of the field that the answer will contain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In the form of a comma separated list of potential answer field(s) for each of the (n) litigant types on possible on the case.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QuestionText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AnswerFieldType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QuestionId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchInputFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fields that can be searched on. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label next to search field on UI.
+    <t>The type of the field that the answer will contain</t>
+  </si>
+  <si>
+    <t>In the form of a comma separated list of potential answer field(s) for each of the (n) litigant types on possible on the case.</t>
+  </si>
+  <si>
+    <t>QuestionText</t>
+  </si>
+  <si>
+    <t>AnswerFieldType</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>QuestionId</t>
+  </si>
+  <si>
+    <t>SearchInputFields</t>
+  </si>
+  <si>
+    <t>Fields that can be searched on. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Label next to search field on UI.
 MaxLength: 200</t>
   </si>
   <si>
-    <t xml:space="preserve">Order of fields on UI 
+    <t>Order of fields on UI 
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">SearchAlias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique alias id for a case field of a case type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is just the CaseField ID for top level fields, or object notation pointing to a complex type field e.g. applicantAddress.AddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchAliasID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchCasesResultFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ResultsOrdering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UseCase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchResultFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fields to be displayed in results list. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name on the results column.for the field
+    <t>SearchAlias</t>
+  </si>
+  <si>
+    <t>Unique alias id for a case field of a case type</t>
+  </si>
+  <si>
+    <t>This is just the CaseField ID for top level fields, or object notation pointing to a complex type field e.g. applicantAddress.AddressLine1</t>
+  </si>
+  <si>
+    <t>SearchAliasID</t>
+  </si>
+  <si>
+    <t>SearchCasesResultFields</t>
+  </si>
+  <si>
+    <t>ResultsOrdering</t>
+  </si>
+  <si>
+    <t>UseCase</t>
+  </si>
+  <si>
+    <t>SearchResultFields</t>
+  </si>
+  <si>
+    <t>Fields to be displayed in results list. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Name on the results column.for the field
 MaxLength: 200</t>
   </si>
   <si>
-    <t xml:space="preserve">Order the columns are displayed.
+    <t>Order the columns are displayed.
 Positive Integer</t>
   </si>
   <si>
     <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
   </si>
   <si>
-    <t xml:space="preserve">Fields can be ordered on by user role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Banner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes or No, to enable or disable the banner.                          MaxLength: 30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Content to display in the banner         MaxLength: 300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optional link text in the banner                   MaxLength:50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The URL for the link text.                                               Max Length: 1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BannerEnabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BannerDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BannerUrlText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BannerUrl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketResultFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketInputFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserProfile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID from Jurisdiction Tab
+    <t>Fields can be ordered on by user role</t>
+  </si>
+  <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>Yes or No, to enable or disable the banner.                          MaxLength: 30</t>
+  </si>
+  <si>
+    <t>Content to display in the banner         MaxLength: 300</t>
+  </si>
+  <si>
+    <t>Optional link text in the banner                   MaxLength:50</t>
+  </si>
+  <si>
+    <t>The URL for the link text.                                               Max Length: 1000</t>
+  </si>
+  <si>
+    <t>BannerEnabled</t>
+  </si>
+  <si>
+    <t>BannerDescription</t>
+  </si>
+  <si>
+    <t>BannerUrlText</t>
+  </si>
+  <si>
+    <t>BannerUrl</t>
+  </si>
+  <si>
+    <t>WorkBasketResultFields</t>
+  </si>
+  <si>
+    <t>WorkBasketInputFields</t>
+  </si>
+  <si>
+    <t>UserProfile</t>
+  </si>
+  <si>
+    <t>Must match ID from Jurisdiction Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID from CaseType Tab
+    <t>Must match ID from CaseType Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID from State Tab
+    <t>Must match ID from State Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">UserIDAMId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketDefaultJurisdiction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketDefaultCaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketDefaultState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthorisationCaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID in 'CaseType' tab
+    <t>UserIDAMId</t>
+  </si>
+  <si>
+    <t>WorkBasketDefaultJurisdiction</t>
+  </si>
+  <si>
+    <t>WorkBasketDefaultCaseType</t>
+  </si>
+  <si>
+    <t>WorkBasketDefaultState</t>
+  </si>
+  <si>
+    <t>AuthorisationCaseType</t>
+  </si>
+  <si>
+    <t>Must match ID in 'CaseType' tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID role.  If a role doesn’t have a Row below that mean no access to.
+    <t>Must match ID role.  If a role doesn’t have a Row below that mean no access to.
 MaxLength: 100.</t>
   </si>
   <si>
-    <t xml:space="preserve">C - Create, R - Read, U - Update, D - Delete
+    <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">CRUD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthorisationCaseField</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID on 'CaseType' tab
+    <t>CRUD</t>
+  </si>
+  <si>
+    <t>AuthorisationCaseField</t>
+  </si>
+  <si>
+    <t>Must match ID on 'CaseType' tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID on CaseField tab.
+    <t>Must match ID on CaseField tab.
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">AuthorisationCaseEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID on Event tabe.
+    <t>AuthorisationCaseEvent</t>
+  </si>
+  <si>
+    <t>Must match ID on Event tabe.
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">AuthorisationCaseState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Muust match an ID on State tab.
+    <t>AuthorisationCaseState</t>
+  </si>
+  <si>
+    <t>Muust match an ID on State tab.
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">CaseStateID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthorisationComplexType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Field ID should match an ID in the CaseField Tab
+    <t>CaseStateID</t>
+  </si>
+  <si>
+    <t>AuthorisationComplexType</t>
+  </si>
+  <si>
+    <t>The Field ID should match an ID in the CaseField Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">C - Create, R - Read, U - Update, D - Delete
+    <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
+  </si>
+  <si>
+    <t>EventEnablingCondition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY;@"/>
-    <numFmt numFmtId="166" formatCode="@"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="168" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="169" formatCode="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -806,22 +810,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -855,14 +844,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -870,14 +859,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -885,7 +874,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -893,7 +882,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -908,7 +897,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFFC000"/>
       <name val="Arial"/>
@@ -916,7 +905,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFF6600"/>
       <name val="Arial"/>
@@ -924,7 +913,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF984807"/>
       <name val="Arial"/>
@@ -932,7 +921,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
@@ -940,7 +929,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -968,7 +957,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFC000"/>
       <name val="Calibri"/>
@@ -1004,7 +993,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
@@ -1028,14 +1017,14 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF000080"/>
       </left>
@@ -1050,386 +1039,152 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="84">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="83">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1488,29 +1243,337 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    <sheetView topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1525,7 +1588,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="126.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1545,7 +1608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -1566,34 +1629,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>147</v>
       </c>
@@ -1608,7 +1663,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1628,7 +1683,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -1649,36 +1704,28 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="14" width="10.5" customWidth="1"/>
+    <col min="15" max="15" width="26.83203125" customWidth="1"/>
+    <col min="16" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>153</v>
       </c>
@@ -1701,7 +1748,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="409.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1745,7 +1792,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -1793,41 +1840,33 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
         <v>160</v>
       </c>
@@ -1841,7 +1880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="111.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1870,7 +1909,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -1903,34 +1942,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>168</v>
       </c>
@@ -1946,7 +1977,7 @@
       <c r="E1" s="54"/>
       <c r="F1" s="54"/>
     </row>
-    <row r="2" customFormat="false" ht="113.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1966,7 +1997,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -1987,36 +2018,28 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.5"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>172</v>
       </c>
@@ -2030,7 +2053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="113.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
         <v>173</v>
@@ -2042,7 +2065,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>19</v>
       </c>
@@ -2057,38 +2080,30 @@
       <c r="F3" s="10"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11"/>
+    <col min="1" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="56" t="s">
         <v>10</v>
       </c>
@@ -2123,7 +2138,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="57"/>
       <c r="G4" s="58"/>
@@ -2131,34 +2146,26 @@
       <c r="K4" s="60"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>179</v>
       </c>
@@ -2174,7 +2181,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="141" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2200,7 +2207,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2227,34 +2234,24 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>185</v>
       </c>
@@ -2264,7 +2261,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>186</v>
       </c>
@@ -2280,7 +2277,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>190</v>
       </c>
@@ -2297,40 +2294,32 @@
       <c r="F3" s="20"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>194</v>
       </c>
@@ -2348,7 +2337,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="63"/>
     </row>
-    <row r="2" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" ht="141" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2377,7 +2366,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2407,34 +2396,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
         <v>195</v>
       </c>
@@ -2450,7 +2431,7 @@
       <c r="E1" s="68"/>
       <c r="F1" s="68"/>
     </row>
-    <row r="2" customFormat="false" ht="113.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2470,7 +2451,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2491,37 +2472,29 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.5"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>16</v>
       </c>
@@ -2535,7 +2508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>17</v>
       </c>
@@ -2555,11 +2528,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -2576,34 +2549,24 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>196</v>
       </c>
@@ -2619,7 +2582,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2637,7 +2600,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2658,34 +2621,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>204</v>
       </c>
@@ -2700,7 +2655,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="126.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2717,7 +2672,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -2735,34 +2690,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="69" t="s">
         <v>209</v>
       </c>
@@ -2778,7 +2725,7 @@
       <c r="E1" s="70"/>
       <c r="F1" s="70"/>
     </row>
-    <row r="2" customFormat="false" ht="126.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2798,7 +2745,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>10</v>
       </c>
@@ -2819,34 +2766,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>212</v>
       </c>
@@ -2862,7 +2801,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="126.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2882,7 +2821,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -2903,34 +2842,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>214</v>
       </c>
@@ -2946,7 +2877,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="126.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2966,7 +2897,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -2987,33 +2918,25 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.5"/>
+    <col min="1" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="76" t="s">
         <v>217</v>
       </c>
@@ -3030,7 +2953,7 @@
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
     </row>
-    <row r="2" customFormat="false" ht="252.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" ht="253" x14ac:dyDescent="0.2">
       <c r="A2" s="80"/>
       <c r="B2" s="80"/>
       <c r="C2" s="81" t="s">
@@ -3049,7 +2972,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="82" t="s">
         <v>10</v>
       </c>
@@ -3073,10 +2996,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
@@ -3084,23 +3006,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>20</v>
       </c>
@@ -3119,7 +3038,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="210.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" ht="211" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3148,7 +3067,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="42.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" ht="43" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
@@ -3178,34 +3097,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -3227,7 +3138,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="409.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3268,7 +3179,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -3310,37 +3221,29 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="11" width="10.5" customWidth="1"/>
+    <col min="12" max="12" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="14" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -3362,7 +3265,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="183" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13" ht="183" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3403,7 +3306,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -3445,42 +3348,35 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U11" activeCellId="0" sqref="U11"/>
+    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="23.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="9" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="26.1640625" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" customWidth="1"/>
+    <col min="13" max="14" width="10.5" customWidth="1"/>
+    <col min="15" max="15" width="24.33203125" customWidth="1"/>
+    <col min="16" max="18" width="10.5" customWidth="1"/>
+    <col min="19" max="19" width="23.6640625" customWidth="1"/>
+    <col min="20" max="20" width="20.5" customWidth="1"/>
+    <col min="21" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>71</v>
       </c>
@@ -3505,7 +3401,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:21" ht="253" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3567,7 +3463,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -3633,45 +3529,37 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:Y3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AMK3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="11.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="17.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="26" width="30.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="26" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="26" width="9.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="26" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="26" width="16.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="26" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="26" width="6.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="15" style="27" width="6.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="28" width="6.38"/>
+    <col min="1" max="1" width="19.5" style="25" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="26" customWidth="1"/>
+    <col min="5" max="7" width="30.1640625" style="26" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="26" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" style="26" customWidth="1"/>
+    <col min="12" max="12" width="16" style="26" customWidth="1"/>
+    <col min="13" max="14" width="6.33203125" style="26" customWidth="1"/>
+    <col min="15" max="1022" width="6.33203125" style="27" customWidth="1"/>
+    <col min="1023" max="1025" width="6.33203125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>104</v>
       </c>
@@ -3685,7 +3573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" s="37" customFormat="true" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:25" s="37" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
@@ -3736,7 +3624,7 @@
       <c r="X2" s="36"/>
       <c r="Y2" s="36"/>
     </row>
-    <row r="3" s="27" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:25" s="27" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="38" t="s">
         <v>10</v>
       </c>
@@ -3778,10 +3666,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
@@ -3789,23 +3676,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>114</v>
       </c>
@@ -3823,7 +3707,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="225" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="225" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3849,7 +3733,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -3876,36 +3760,30 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:U3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="19" width="10.5" customWidth="1"/>
+    <col min="20" max="20" width="14.6640625" customWidth="1"/>
+    <col min="21" max="21" width="10.5" customWidth="1"/>
+    <col min="22" max="22" width="29.33203125" customWidth="1"/>
+    <col min="23" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>122</v>
       </c>
@@ -3935,7 +3813,7 @@
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="306" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:22" ht="333" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3999,8 +3877,11 @@
       <c r="U2" s="7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V2" s="83" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="57" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -4064,14 +3945,12 @@
       <c r="U3" s="19" t="s">
         <v>103</v>
       </c>
+      <c r="V3" s="19" t="s">
+        <v>220</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Add support for conditional events (EventEnablingCondition field) (#151)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,40 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomaszp/fpla/ccd-definition-processor/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFF134C-2529-6947-A536-E824BEA9E2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Jurisdiction" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="CaseRoles" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="CaseType" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="CaseField" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="CaseTypeTab" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="CaseEventToFields" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="CaseEventToComplexTypes" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="State" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="CaseEvent" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="FixedLists" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="ComplexTypes" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="ChallengeQuestion" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="SearchInputFields" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="SearchAlias" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="SearchCasesResultFields" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="SearchResultFields" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="Banner" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="WorkBasketResultFields" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="WorkBasketInputFields" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="UserProfile" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="AuthorisationCaseType" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="AuthorisationCaseField" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="AuthorisationCaseState" sheetId="24" state="visible" r:id="rId25"/>
-    <sheet name="AuthorisationComplexType" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
+    <sheet name="CaseRoles" sheetId="2" r:id="rId2"/>
+    <sheet name="CaseType" sheetId="3" r:id="rId3"/>
+    <sheet name="CaseField" sheetId="4" r:id="rId4"/>
+    <sheet name="CaseTypeTab" sheetId="5" r:id="rId5"/>
+    <sheet name="CaseEventToFields" sheetId="6" r:id="rId6"/>
+    <sheet name="CaseEventToComplexTypes" sheetId="7" r:id="rId7"/>
+    <sheet name="State" sheetId="8" r:id="rId8"/>
+    <sheet name="CaseEvent" sheetId="9" r:id="rId9"/>
+    <sheet name="FixedLists" sheetId="10" r:id="rId10"/>
+    <sheet name="ComplexTypes" sheetId="11" r:id="rId11"/>
+    <sheet name="ChallengeQuestion" sheetId="12" r:id="rId12"/>
+    <sheet name="SearchInputFields" sheetId="13" r:id="rId13"/>
+    <sheet name="SearchAlias" sheetId="14" r:id="rId14"/>
+    <sheet name="SearchCasesResultFields" sheetId="15" r:id="rId15"/>
+    <sheet name="SearchResultFields" sheetId="16" r:id="rId16"/>
+    <sheet name="Banner" sheetId="17" r:id="rId17"/>
+    <sheet name="WorkBasketResultFields" sheetId="18" r:id="rId18"/>
+    <sheet name="WorkBasketInputFields" sheetId="19" r:id="rId19"/>
+    <sheet name="UserProfile" sheetId="20" r:id="rId20"/>
+    <sheet name="AuthorisationCaseType" sheetId="21" r:id="rId21"/>
+    <sheet name="AuthorisationCaseField" sheetId="22" r:id="rId22"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="23" r:id="rId23"/>
+    <sheet name="AuthorisationCaseState" sheetId="24" r:id="rId24"/>
+    <sheet name="AuthorisationComplexType" sheetId="25" r:id="rId25"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -44,760 +49,759 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="220">
-  <si>
-    <t xml:space="preserve">Jurisdiction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrimaryKeyInRed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrimaryAndForeignKey Orange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ForeignKey Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start date from which the data will be valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End date until which the data will be valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The identifier which defines the casetype code
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="221">
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t>PrimaryKeyInRed</t>
+  </si>
+  <si>
+    <t>PrimaryAndForeignKey Orange</t>
+  </si>
+  <si>
+    <t>ForeignKey Brown</t>
+  </si>
+  <si>
+    <t>Start date from which the data will be valid</t>
+  </si>
+  <si>
+    <t>End date until which the data will be valid</t>
+  </si>
+  <si>
+    <t>The identifier which defines the casetype code
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The short description to describe the jurisdiction used on UI display
+    <t>The short description to describe the jurisdiction used on UI display
 MaxLength: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">The long description to describe the jurisdiction.
+    <t>The long description to describe the jurisdiction.
 MaxLength: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">This can have value TRUE/FALSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LiveFrom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LiveTo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shuttered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseRoles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength: 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength:128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The short description to describe the case type used on the UI.
+    <t>This can have value TRUE/FALSE</t>
+  </si>
+  <si>
+    <t>LiveFrom</t>
+  </si>
+  <si>
+    <t>LiveTo</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Shuttered</t>
+  </si>
+  <si>
+    <t>CaseRoles</t>
+  </si>
+  <si>
+    <t>MaxLength: 40</t>
+  </si>
+  <si>
+    <t>MaxLength:128</t>
+  </si>
+  <si>
+    <t>CaseTypeID</t>
+  </si>
+  <si>
+    <t>CaseType</t>
+  </si>
+  <si>
+    <t>The short description to describe the case type used on the UI.
 MaxLength: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">The long description to decribe the case type.
+    <t>The long description to decribe the case type.
 MaxLength: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">The jurisdiction code should match the one defined in 'Jurisdiction' tab
+    <t>The jurisdiction code should match the one defined in 'Jurisdiction' tab
 MaxLength:70</t>
   </si>
   <si>
-    <t xml:space="preserve">The absolute URL to the microservice which lists the documents that the services wants to provide for print. 
+    <t>The absolute URL to the microservice which lists the documents that the services wants to provide for print. 
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). Max Length: 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It is a mandatory field which can define if the data classification of the field
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). Max Length: 20</t>
+  </si>
+  <si>
+    <t>It is a mandatory field which can define if the data classification of the field
 MustBe: &lt;Public, Private, Retricted&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">JurisdictionID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrintableDocumentsUrl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLPrintEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SecurityClassification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseField</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The code of casetype has to be defined in 'CaseType' tab
+    <t>JurisdictionID</t>
+  </si>
+  <si>
+    <t>PrintableDocumentsUrl</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLPrintEvent</t>
+  </si>
+  <si>
+    <t>SecurityClassification</t>
+  </si>
+  <si>
+    <t>CaseField</t>
+  </si>
+  <si>
+    <t>The code of casetype has to be defined in 'CaseType' tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The field ID should match the field attribute name used by the service team in creating the case
+    <t>The field ID should match the field attribute name used by the service team in creating the case
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
+    <t>The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
 MaxLength:&lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The hint text that is present for each field type
+    <t>The hint text that is present for each field type
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The type of field. This can be a CCD Base type (see confluence) or a ComplexType ID as per the ComplexType tab).  
+    <t>The type of field. This can be a CCD Base type (see confluence) or a ComplexType ID as per the ComplexType tab).  
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Some FieldTypes require or have an optional addition parameter that can be set (e.g. Collection - the parameter is the collecion of What FieldType ?, FixedList the parameter is the ID from the fixedList tab). See confluence for details
+    <t>Some FieldTypes require or have an optional addition parameter that can be set (e.g. Collection - the parameter is the collecion of What FieldType ?, FixedList the parameter is the ID from the fixedList tab). See confluence for details
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">The regex that can define the type of data accepted in the fields E.g: alphanumeric etc. This will override the regex, if defined internally for any type.
+    <t>The regex that can define the type of data accepted in the fields E.g: alphanumeric etc. This will override the regex, if defined internally for any type.
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The minimum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
+    <t>The minimum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The maximum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
+    <t>The maximum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HintText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldTypeParameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RegularExpression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Searchable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseTypeTab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not used yet - maybe used for roletype type view later
+    <t>Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>HintText</t>
+  </si>
+  <si>
+    <t>FieldType</t>
+  </si>
+  <si>
+    <t>FieldTypeParameter</t>
+  </si>
+  <si>
+    <t>RegularExpression</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Searchable</t>
+  </si>
+  <si>
+    <t>CaseTypeTab</t>
+  </si>
+  <si>
+    <t>Not used yet - maybe used for roletype type view later
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">Unique Id for tab. MaxLength: 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name to be displayed on the tab
+    <t>Unique Id for tab. MaxLength: 40</t>
+  </si>
+  <si>
+    <t>Name to be displayed on the tab
 MaxLengh: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">Order of Tab on screen - left to right.
+    <t>Order of Tab on screen - left to right.
 PositiveInteger</t>
   </si>
   <si>
-    <t xml:space="preserve">Unique ID for field - must match an ID on the CaseField tab or be a metadata item. 
+    <t>Unique ID for field - must match an ID on the CaseField tab or be a metadata item. 
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order of Fields within a tab - top to bottom
+    <t>MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
+  </si>
+  <si>
+    <t>Order of Fields within a tab - top to bottom
 PositiveInteger</t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
+    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
 MaxLength:1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean expression rules for hiding a tab: 
+    <t>Boolean expression rules for hiding a tab: 
 MaxLength:1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Text should begin with #LIST( or #TABLE(
+    <t>Text should begin with #LIST( or #TABLE(
 MaxLength: 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Channel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseFieldID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserRole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabFieldDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldShowCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabShowCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DisplayContextParameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventToFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique ID for the event. Not listing an case event means that All Fields are displayed. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This defines with Fields can be changed / viewed during an case event. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The order of the fields on the screen.
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>TabID</t>
+  </si>
+  <si>
+    <t>TabLabel</t>
+  </si>
+  <si>
+    <t>TabDisplayOrder</t>
+  </si>
+  <si>
+    <t>CaseFieldID</t>
+  </si>
+  <si>
+    <t>UserRole</t>
+  </si>
+  <si>
+    <t>TabFieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>FieldShowCondition</t>
+  </si>
+  <si>
+    <t>TabShowCondition</t>
+  </si>
+  <si>
+    <t>DisplayContextParameter</t>
+  </si>
+  <si>
+    <t>CaseEventToFields</t>
+  </si>
+  <si>
+    <t>Unique ID for the event. Not listing an case event means that All Fields are displayed. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>This defines with Fields can be changed / viewed during an case event. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>The order of the fields on the screen.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted Values:  for mandatory, readonly and optional data on UI
+    <t>Accepted Values:  for mandatory, readonly and optional data on UI
 MustBe: MANDATORY, READONLY, OPTIONAL</t>
   </si>
   <si>
-    <t xml:space="preserve">This is a string value which defines the Wizard pages' ID
+    <t>This is a string value which defines the Wizard pages' ID
 MaxLength:40</t>
   </si>
   <si>
-    <t xml:space="preserve">This is a string value which defines the Wizard pages' Label
+    <t>This is a string value which defines the Wizard pages' Label
 MaxLength:40</t>
   </si>
   <si>
-    <t xml:space="preserve">The order to display the pages
+    <t>The order to display the pages
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Currently blank 1 or 2.  2 currently will display the yellow review column.
+    <t>Currently blank 1 or 2.  2 currently will display the yellow review column.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
+    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
 MaxLength: 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean expression rules for hiding a page: MaxLength:1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">States a field should appear on check your answers However these fields will be considered only "ShowSummary" column in CaseEvent tab is set to Y
+    <t>Boolean expression rules for hiding a page: MaxLength:1000</t>
+  </si>
+  <si>
+    <t>States a field should appear on check your answers However these fields will be considered only "ShowSummary" column in CaseEvent tab is set to Y
 CouldBe: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">URL to call back to the service for uniqueness. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a string value overrides label from CaseField tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a string value overrides hint from CaseField tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boolean value to say if an event can be published</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageFieldDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DisplayContext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageColumnNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageShowCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowSummaryChangeOption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowSummaryContentOption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLMidEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLMidEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventFieldLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventFieldHint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetainHiddenValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Publish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventToComplexTypes</t>
+    <t>URL to call back to the service for uniqueness. </t>
+  </si>
+  <si>
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). </t>
+  </si>
+  <si>
+    <t>This is a string value overrides label from CaseField tab</t>
+  </si>
+  <si>
+    <t>This is a string value overrides hint from CaseField tab</t>
+  </si>
+  <si>
+    <t>Boolean value to say if an event can be published</t>
+  </si>
+  <si>
+    <t>CaseEventID</t>
+  </si>
+  <si>
+    <t>PageFieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>DisplayContext</t>
+  </si>
+  <si>
+    <t>PageID</t>
+  </si>
+  <si>
+    <t>PageLabel</t>
+  </si>
+  <si>
+    <t>PageDisplayOrder</t>
+  </si>
+  <si>
+    <t>PageColumnNumber</t>
+  </si>
+  <si>
+    <t>PageShowCondition</t>
+  </si>
+  <si>
+    <t>ShowSummaryChangeOption</t>
+  </si>
+  <si>
+    <t>ShowSummaryContentOption</t>
+  </si>
+  <si>
+    <t>CallBackURLMidEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLMidEvent</t>
+  </si>
+  <si>
+    <t>CaseEventFieldLabel</t>
+  </si>
+  <si>
+    <t>CaseEventFieldHint</t>
+  </si>
+  <si>
+    <t>RetainHiddenValue</t>
+  </si>
+  <si>
+    <t>Publish</t>
+  </si>
+  <si>
+    <t>EventToComplexTypes</t>
   </si>
   <si>
     <t xml:space="preserve">
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">MaxLength:70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength:200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength:300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ListElementCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DefaultValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventElementLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventHintText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State with ID '*' and Name 'DEFAULT' is a reserved state. The state can be used for events where states do not change.
+    <t>MaxLength:70</t>
+  </si>
+  <si>
+    <t>MaxLength:200</t>
+  </si>
+  <si>
+    <t>MaxLength:300</t>
+  </si>
+  <si>
+    <t>ListElementCode</t>
+  </si>
+  <si>
+    <t>DefaultValue</t>
+  </si>
+  <si>
+    <t>EventElementLabel</t>
+  </si>
+  <si>
+    <t>EventHintText</t>
+  </si>
+  <si>
+    <t>FieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>State with ID '*' and Name 'DEFAULT' is a reserved state. The state can be used for events where states do not change.
 MaxLength:70</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the name of the state as displayed on UI
+    <t>This is the name of the state as displayed on UI
 MaxLength:100</t>
   </si>
   <si>
-    <t xml:space="preserve">This gives longer decription of the case state
+    <t>This gives longer decription of the case state
 Max Length: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">The order of the states on the screen.
+    <t>The order of the states on the screen.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Optional override of title used in the CaseTabView. Markdown , concat supported
+    <t>Optional override of title used in the CaseTabView. Markdown , concat supported
 MaxLength: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">DisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TitleDisplay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique ID for the event
+    <t>DisplayOrder</t>
+  </si>
+  <si>
+    <t>TitleDisplay</t>
+  </si>
+  <si>
+    <t>CaseEvent</t>
+  </si>
+  <si>
+    <t>Unique ID for the event
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the name of the event as displayed on UI Dropdown list - hence limited to 30
+    <t>This is the name of the event as displayed on UI Dropdown list - hence limited to 30
 MaxLength: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">This gives further details of an event of a case
+    <t>This gives further details of an event of a case
 MaxLength:100</t>
   </si>
   <si>
-    <t xml:space="preserve">The display order of displaying the events in the list
+    <t>The display order of displaying the events in the list
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Future Elements not for MVP (what about multiple state) (semicolon ; seprated list).
+    <t>Future Elements not for MVP (what about multiple state) (semicolon ; seprated list).
 If '*' is provided, then precondition will not be validated and will be considered as current state
  MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Future Elements not for MVP. 
+    <t>Future Elements not for MVP. 
 If '*' is provided, then the current state will not change and will be same as pre condition state
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">URL to call back to the service for uniqueness. 
+    <t>URL to call back to the service for uniqueness. 
 Max Length: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). 
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). 
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Y, N and empty. TheCheck your answer section will be shown on Y (true) and empty(null) values, but not shown on N (false) values. Fields on CaseEventTo Field tab have Y in "ShowSummaryChangeOption" column.
+    <t>Y, N and empty. TheCheck your answer section will be shown on Y (true) and empty(null) values, but not shown on N (false) values. Fields on CaseEventTo Field tab have Y in "ShowSummaryChangeOption" column.
 CouldBe: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean value to say if the enter summary and event description fields are to be shown
+    <t>Boolean value to say if the enter summary and event description fields are to be shown
 CouldBeh: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean value to say if a draft of a create event can be saved
+    <t>Boolean value to say if a draft of a create event can be saved
 CouldBe: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The label of the button on the final event screen - default is Submit
+    <t>The label of the button on the final event screen - default is Submit
 MaxLength: 200</t>
   </si>
   <si>
-    <t xml:space="preserve">PreConditionState(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PostConditionState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLAboutToStartEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutAboutToStartEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLAboutToSubmitEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLAboutToSubmitEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLSubmittedEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLSubmittedEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowSummary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowEventNotes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CanSaveDraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndButtonLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FixedLists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The unique identifier of the Fixed list
+    <t>PreConditionState(s)</t>
+  </si>
+  <si>
+    <t>PostConditionState</t>
+  </si>
+  <si>
+    <t>CallBackURLAboutToStartEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutAboutToStartEvent</t>
+  </si>
+  <si>
+    <t>CallBackURLAboutToSubmitEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLAboutToSubmitEvent</t>
+  </si>
+  <si>
+    <t>CallBackURLSubmittedEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLSubmittedEvent</t>
+  </si>
+  <si>
+    <t>ShowSummary</t>
+  </si>
+  <si>
+    <t>ShowEventNotes</t>
+  </si>
+  <si>
+    <t>CanSaveDraft</t>
+  </si>
+  <si>
+    <t>EndButtonLabel</t>
+  </si>
+  <si>
+    <t>FixedLists</t>
+  </si>
+  <si>
+    <t>The unique identifier of the Fixed list
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">The unque ID of an element in the list (ID)
+    <t>The unque ID of an element in the list (ID)
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">The Display name for the list item
+    <t>The Display name for the list item
 MaxLength: 250</t>
   </si>
   <si>
-    <t xml:space="preserve">The display order of list items. Positive integers e.g 1, 2, 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ListElement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ComplexTypes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The ComplexType ID should match the field attribute name on the CaseField Tab
+    <t>The display order of list items. Positive integers e.g 1, 2, 3</t>
+  </si>
+  <si>
+    <t>ListElement</t>
+  </si>
+  <si>
+    <t>ComplexTypes</t>
+  </si>
+  <si>
+    <t>The ComplexType ID should match the field attribute name on the CaseField Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The complex type element (field) ID (ListElementId) should match the field attribute name used by the service team in creating the case
+    <t>The complex type element (field) ID (ListElementId) should match the field attribute name used by the service team in creating the case
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
+    <t>The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
 MaxLength:200</t>
   </si>
   <si>
-    <t xml:space="preserve">Within a complex type any field can be hidden or shown based on another field's values in the same level.
+    <t>Within a complex type any field can be hidden or shown based on another field's values in the same level.
 Currently only single boolean or string conditions are supported. Eg: country="Italy" or country startWith: "Uni"
 MaxLength: 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">The hint text that is present for each field type
+    <t>The hint text that is present for each field type
 MaxLength: &lt;unlmited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">ElementLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChallengeQuestion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order of fields on UI
+    <t>ElementLabel</t>
+  </si>
+  <si>
+    <t>ChallengeQuestion</t>
+  </si>
+  <si>
+    <t>Order of fields on UI
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">The type of the field that the answer will contain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In the form of a comma separated list of potential answer field(s) for each of the (n) litigant types on possible on the case.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QuestionText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AnswerFieldType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QuestionId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchInputFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fields that can be searched on. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label next to search field on UI.
+    <t>The type of the field that the answer will contain</t>
+  </si>
+  <si>
+    <t>In the form of a comma separated list of potential answer field(s) for each of the (n) litigant types on possible on the case.</t>
+  </si>
+  <si>
+    <t>QuestionText</t>
+  </si>
+  <si>
+    <t>AnswerFieldType</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>QuestionId</t>
+  </si>
+  <si>
+    <t>SearchInputFields</t>
+  </si>
+  <si>
+    <t>Fields that can be searched on. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Label next to search field on UI.
 MaxLength: 200</t>
   </si>
   <si>
-    <t xml:space="preserve">Order of fields on UI 
+    <t>Order of fields on UI 
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">SearchAlias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique alias id for a case field of a case type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is just the CaseField ID for top level fields, or object notation pointing to a complex type field e.g. applicantAddress.AddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchAliasID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchCasesResultFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ResultsOrdering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UseCase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchResultFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fields to be displayed in results list. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name on the results column.for the field
+    <t>SearchAlias</t>
+  </si>
+  <si>
+    <t>Unique alias id for a case field of a case type</t>
+  </si>
+  <si>
+    <t>This is just the CaseField ID for top level fields, or object notation pointing to a complex type field e.g. applicantAddress.AddressLine1</t>
+  </si>
+  <si>
+    <t>SearchAliasID</t>
+  </si>
+  <si>
+    <t>SearchCasesResultFields</t>
+  </si>
+  <si>
+    <t>ResultsOrdering</t>
+  </si>
+  <si>
+    <t>UseCase</t>
+  </si>
+  <si>
+    <t>SearchResultFields</t>
+  </si>
+  <si>
+    <t>Fields to be displayed in results list. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Name on the results column.for the field
 MaxLength: 200</t>
   </si>
   <si>
-    <t xml:space="preserve">Order the columns are displayed.
+    <t>Order the columns are displayed.
 Positive Integer</t>
   </si>
   <si>
     <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
   </si>
   <si>
-    <t xml:space="preserve">Fields can be ordered on by user role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Banner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes or No, to enable or disable the banner.                          MaxLength: 30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Content to display in the banner         MaxLength: 300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optional link text in the banner                   MaxLength:50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The URL for the link text.                                               Max Length: 1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BannerEnabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BannerDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BannerUrlText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BannerUrl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketResultFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketInputFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserProfile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID from Jurisdiction Tab
+    <t>Fields can be ordered on by user role</t>
+  </si>
+  <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>Yes or No, to enable or disable the banner.                          MaxLength: 30</t>
+  </si>
+  <si>
+    <t>Content to display in the banner         MaxLength: 300</t>
+  </si>
+  <si>
+    <t>Optional link text in the banner                   MaxLength:50</t>
+  </si>
+  <si>
+    <t>The URL for the link text.                                               Max Length: 1000</t>
+  </si>
+  <si>
+    <t>BannerEnabled</t>
+  </si>
+  <si>
+    <t>BannerDescription</t>
+  </si>
+  <si>
+    <t>BannerUrlText</t>
+  </si>
+  <si>
+    <t>BannerUrl</t>
+  </si>
+  <si>
+    <t>WorkBasketResultFields</t>
+  </si>
+  <si>
+    <t>WorkBasketInputFields</t>
+  </si>
+  <si>
+    <t>UserProfile</t>
+  </si>
+  <si>
+    <t>Must match ID from Jurisdiction Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID from CaseType Tab
+    <t>Must match ID from CaseType Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID from State Tab
+    <t>Must match ID from State Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">UserIDAMId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketDefaultJurisdiction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketDefaultCaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketDefaultState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthorisationCaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID in 'CaseType' tab
+    <t>UserIDAMId</t>
+  </si>
+  <si>
+    <t>WorkBasketDefaultJurisdiction</t>
+  </si>
+  <si>
+    <t>WorkBasketDefaultCaseType</t>
+  </si>
+  <si>
+    <t>WorkBasketDefaultState</t>
+  </si>
+  <si>
+    <t>AuthorisationCaseType</t>
+  </si>
+  <si>
+    <t>Must match ID in 'CaseType' tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID role.  If a role doesn’t have a Row below that mean no access to.
+    <t>Must match ID role.  If a role doesn’t have a Row below that mean no access to.
 MaxLength: 100.</t>
   </si>
   <si>
-    <t xml:space="preserve">C - Create, R - Read, U - Update, D - Delete
+    <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">CRUD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthorisationCaseField</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID on 'CaseType' tab
+    <t>CRUD</t>
+  </si>
+  <si>
+    <t>AuthorisationCaseField</t>
+  </si>
+  <si>
+    <t>Must match ID on 'CaseType' tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID on CaseField tab.
+    <t>Must match ID on CaseField tab.
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">AuthorisationCaseEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID on Event tabe.
+    <t>AuthorisationCaseEvent</t>
+  </si>
+  <si>
+    <t>Must match ID on Event tabe.
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">AuthorisationCaseState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Muust match an ID on State tab.
+    <t>AuthorisationCaseState</t>
+  </si>
+  <si>
+    <t>Muust match an ID on State tab.
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">CaseStateID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthorisationComplexType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Field ID should match an ID in the CaseField Tab
+    <t>CaseStateID</t>
+  </si>
+  <si>
+    <t>AuthorisationComplexType</t>
+  </si>
+  <si>
+    <t>The Field ID should match an ID in the CaseField Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">C - Create, R - Read, U - Update, D - Delete
+    <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
+  </si>
+  <si>
+    <t>EventEnablingCondition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY;@"/>
-    <numFmt numFmtId="166" formatCode="@"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="168" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="169" formatCode="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -806,22 +810,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -855,14 +844,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -870,14 +859,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -885,7 +874,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -893,7 +882,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -908,7 +897,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFFC000"/>
       <name val="Arial"/>
@@ -916,7 +905,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFF6600"/>
       <name val="Arial"/>
@@ -924,7 +913,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF984807"/>
       <name val="Arial"/>
@@ -932,7 +921,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
@@ -940,7 +929,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -968,7 +957,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFC000"/>
       <name val="Calibri"/>
@@ -1004,7 +993,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
@@ -1028,14 +1017,14 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF000080"/>
       </left>
@@ -1050,386 +1039,152 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="84">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="83">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1488,29 +1243,337 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    <sheetView topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1525,7 +1588,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="126.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1545,7 +1608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -1566,34 +1629,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>147</v>
       </c>
@@ -1608,7 +1663,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1628,7 +1683,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -1649,36 +1704,28 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="14" width="10.5" customWidth="1"/>
+    <col min="15" max="15" width="26.83203125" customWidth="1"/>
+    <col min="16" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>153</v>
       </c>
@@ -1701,7 +1748,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="409.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1745,7 +1792,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -1793,41 +1840,33 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
         <v>160</v>
       </c>
@@ -1841,7 +1880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="111.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1870,7 +1909,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -1903,34 +1942,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>168</v>
       </c>
@@ -1946,7 +1977,7 @@
       <c r="E1" s="54"/>
       <c r="F1" s="54"/>
     </row>
-    <row r="2" customFormat="false" ht="113.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1966,7 +1997,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -1987,36 +2018,28 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.5"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>172</v>
       </c>
@@ -2030,7 +2053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="113.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
         <v>173</v>
@@ -2042,7 +2065,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>19</v>
       </c>
@@ -2057,38 +2080,30 @@
       <c r="F3" s="10"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I36" activeCellId="0" sqref="I36"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11"/>
+    <col min="1" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="56" t="s">
         <v>10</v>
       </c>
@@ -2123,7 +2138,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="57"/>
       <c r="G4" s="58"/>
@@ -2131,34 +2146,26 @@
       <c r="K4" s="60"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>179</v>
       </c>
@@ -2174,7 +2181,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="141" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2200,7 +2207,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2227,34 +2234,24 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>185</v>
       </c>
@@ -2264,7 +2261,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>186</v>
       </c>
@@ -2280,7 +2277,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>190</v>
       </c>
@@ -2297,40 +2294,32 @@
       <c r="F3" s="20"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>194</v>
       </c>
@@ -2348,7 +2337,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="63"/>
     </row>
-    <row r="2" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" ht="141" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2377,7 +2366,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2407,34 +2396,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
         <v>195</v>
       </c>
@@ -2450,7 +2431,7 @@
       <c r="E1" s="68"/>
       <c r="F1" s="68"/>
     </row>
-    <row r="2" customFormat="false" ht="113.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2470,7 +2451,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2491,37 +2472,29 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.5"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>16</v>
       </c>
@@ -2535,7 +2508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>17</v>
       </c>
@@ -2555,11 +2528,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -2576,34 +2549,24 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>196</v>
       </c>
@@ -2619,7 +2582,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="84.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2637,7 +2600,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2658,34 +2621,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>204</v>
       </c>
@@ -2700,7 +2655,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="126.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2717,7 +2672,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -2735,34 +2690,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="69" t="s">
         <v>209</v>
       </c>
@@ -2778,7 +2725,7 @@
       <c r="E1" s="70"/>
       <c r="F1" s="70"/>
     </row>
-    <row r="2" customFormat="false" ht="126.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2798,7 +2745,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>10</v>
       </c>
@@ -2819,34 +2766,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>212</v>
       </c>
@@ -2862,7 +2801,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="126.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2882,7 +2821,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -2903,34 +2842,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>214</v>
       </c>
@@ -2946,7 +2877,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="126.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2966,7 +2897,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -2987,33 +2918,25 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.5"/>
+    <col min="1" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="76" t="s">
         <v>217</v>
       </c>
@@ -3030,7 +2953,7 @@
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
     </row>
-    <row r="2" customFormat="false" ht="252.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" ht="253" x14ac:dyDescent="0.2">
       <c r="A2" s="80"/>
       <c r="B2" s="80"/>
       <c r="C2" s="81" t="s">
@@ -3049,7 +2972,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="82" t="s">
         <v>10</v>
       </c>
@@ -3073,10 +2996,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
@@ -3084,23 +3006,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>20</v>
       </c>
@@ -3119,7 +3038,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="210.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" ht="211" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3148,7 +3067,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="42.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" ht="43" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
@@ -3178,34 +3097,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -3227,7 +3138,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="409.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3268,7 +3179,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -3310,37 +3221,29 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="11" width="10.5" customWidth="1"/>
+    <col min="12" max="12" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="14" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -3362,7 +3265,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="183" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13" ht="183" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3403,7 +3306,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -3445,42 +3348,35 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U11" activeCellId="0" sqref="U11"/>
+    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="23.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="9" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="26.1640625" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" customWidth="1"/>
+    <col min="13" max="14" width="10.5" customWidth="1"/>
+    <col min="15" max="15" width="24.33203125" customWidth="1"/>
+    <col min="16" max="18" width="10.5" customWidth="1"/>
+    <col min="19" max="19" width="23.6640625" customWidth="1"/>
+    <col min="20" max="20" width="20.5" customWidth="1"/>
+    <col min="21" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>71</v>
       </c>
@@ -3505,7 +3401,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:21" ht="253" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3567,7 +3463,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -3633,45 +3529,37 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:Y3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AMK3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N8" activeCellId="0" sqref="N8"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="11.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="17.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="26" width="30.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="26" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="26" width="9.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="26" width="14.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="26" width="16.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="26" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="26" width="6.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="15" style="27" width="6.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="28" width="6.38"/>
+    <col min="1" max="1" width="19.5" style="25" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="26" customWidth="1"/>
+    <col min="5" max="7" width="30.1640625" style="26" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="26" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" style="26" customWidth="1"/>
+    <col min="12" max="12" width="16" style="26" customWidth="1"/>
+    <col min="13" max="14" width="6.33203125" style="26" customWidth="1"/>
+    <col min="15" max="1022" width="6.33203125" style="27" customWidth="1"/>
+    <col min="1023" max="1025" width="6.33203125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>104</v>
       </c>
@@ -3685,7 +3573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" s="37" customFormat="true" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:25" s="37" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
@@ -3736,7 +3624,7 @@
       <c r="X2" s="36"/>
       <c r="Y2" s="36"/>
     </row>
-    <row r="3" s="27" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:25" s="27" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="38" t="s">
         <v>10</v>
       </c>
@@ -3778,10 +3666,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
@@ -3789,23 +3676,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>114</v>
       </c>
@@ -3823,7 +3707,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="225" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="225" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3849,7 +3733,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -3876,36 +3760,30 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:U3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="19" width="10.5" customWidth="1"/>
+    <col min="20" max="20" width="14.6640625" customWidth="1"/>
+    <col min="21" max="21" width="10.5" customWidth="1"/>
+    <col min="22" max="22" width="29.33203125" customWidth="1"/>
+    <col min="23" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>122</v>
       </c>
@@ -3935,7 +3813,7 @@
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="306" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:22" ht="333" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3999,8 +3877,11 @@
       <c r="U2" s="7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V2" s="83" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="57" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -4064,14 +3945,12 @@
       <c r="U3" s="19" t="s">
         <v>103</v>
       </c>
+      <c r="V3" s="19" t="s">
+        <v>220</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RPET-849 Add FieldShowCondition to WorkBasketInputFields
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomaszp/fpla/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anatolysanataly/Downloads/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFF134C-2529-6947-A536-E824BEA9E2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085A56B4-7AAF-6242-8AE0-2B43662D3887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" tabRatio="500" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="221">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -801,7 +801,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1007,6 +1007,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF172B4D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1059,7 +1066,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1178,6 +1185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -2403,19 +2411,22 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
+    <col min="3" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
         <v>195</v>
       </c>
@@ -2431,7 +2442,7 @@
       <c r="E1" s="68"/>
       <c r="F1" s="68"/>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2451,7 +2462,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2469,6 +2480,9 @@
       </c>
       <c r="F3" s="10" t="s">
         <v>120</v>
+      </c>
+      <c r="G3" s="84" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3358,7 +3372,7 @@
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3368,7 +3382,8 @@
     <col min="10" max="10" width="26.1640625" customWidth="1"/>
     <col min="11" max="11" width="22.1640625" customWidth="1"/>
     <col min="12" max="12" width="30.6640625" customWidth="1"/>
-    <col min="13" max="14" width="10.5" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5" customWidth="1"/>
     <col min="15" max="15" width="24.33203125" customWidth="1"/>
     <col min="16" max="18" width="10.5" customWidth="1"/>
     <col min="19" max="19" width="23.6640625" customWidth="1"/>
@@ -3539,7 +3554,7 @@
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3553,7 +3568,7 @@
     <col min="9" max="9" width="9.6640625" style="26" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" style="26" customWidth="1"/>
     <col min="11" max="11" width="16.33203125" style="26" customWidth="1"/>
-    <col min="12" max="12" width="16" style="26" customWidth="1"/>
+    <col min="12" max="12" width="17.5" style="26" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="6.33203125" style="26" customWidth="1"/>
     <col min="15" max="1022" width="6.33203125" style="27" customWidth="1"/>
     <col min="1023" max="1025" width="6.33203125" style="28" customWidth="1"/>
@@ -3769,8 +3784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
RPET-849 Add FieldShowCondition to WorkBasketInputFields (#157)
* RPET-849 Add FieldShowCondition to WorkBasketInputFields

* Add description
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomaszp/fpla/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anatolysanataly/Downloads/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFF134C-2529-6947-A536-E824BEA9E2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE1D1C0-0125-C34E-9FB0-BC8511FAD720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" tabRatio="500" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="222">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -791,6 +791,10 @@
   </si>
   <si>
     <t>EventEnablingCondition</t>
+  </si>
+  <si>
+    <t>"Accepted single or multiple conditions in the format &lt;Field A&gt;=""Text""OR&lt;Field B&gt;=&lt;Yes/No&gt;
+MaxLength: 1000"</t>
   </si>
 </sst>
 </file>
@@ -801,7 +805,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1007,6 +1011,20 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF172B4D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1059,7 +1077,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1176,6 +1194,10 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2403,19 +2425,22 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="10.5" customWidth="1"/>
+    <col min="3" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
         <v>195</v>
       </c>
@@ -2431,7 +2456,7 @@
       <c r="E1" s="68"/>
       <c r="F1" s="68"/>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2450,8 +2475,11 @@
       <c r="F2" s="8" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="85" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2469,6 +2497,9 @@
       </c>
       <c r="F3" s="10" t="s">
         <v>120</v>
+      </c>
+      <c r="G3" s="84" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3358,7 +3389,7 @@
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3368,7 +3399,8 @@
     <col min="10" max="10" width="26.1640625" customWidth="1"/>
     <col min="11" max="11" width="22.1640625" customWidth="1"/>
     <col min="12" max="12" width="30.6640625" customWidth="1"/>
-    <col min="13" max="14" width="10.5" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5" customWidth="1"/>
     <col min="15" max="15" width="24.33203125" customWidth="1"/>
     <col min="16" max="18" width="10.5" customWidth="1"/>
     <col min="19" max="19" width="23.6640625" customWidth="1"/>
@@ -3539,7 +3571,7 @@
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3553,7 +3585,7 @@
     <col min="9" max="9" width="9.6640625" style="26" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" style="26" customWidth="1"/>
     <col min="11" max="11" width="16.33203125" style="26" customWidth="1"/>
-    <col min="12" max="12" width="16" style="26" customWidth="1"/>
+    <col min="12" max="12" width="17.5" style="26" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="6.33203125" style="26" customWidth="1"/>
     <col min="15" max="1022" width="6.33203125" style="27" customWidth="1"/>
     <col min="1023" max="1025" width="6.33203125" style="28" customWidth="1"/>
@@ -3769,8 +3801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Format SearchCasesResultFields LiveFrom as General
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anatolysanataly/Downloads/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E81F16-713D-F244-958D-879BFFD8B306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029DA3D5-331E-6549-A096-7E1011F24ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" tabRatio="500" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" tabRatio="500" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -2107,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2423,7 +2423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
RPET-849 Change description (#158)
* RPET-849 Change description

* Format SearchCasesResultFields LiveFrom as General
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anatolysanataly/Downloads/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE1D1C0-0125-C34E-9FB0-BC8511FAD720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029DA3D5-331E-6549-A096-7E1011F24ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" tabRatio="500" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" tabRatio="500" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="221">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -791,10 +791,6 @@
   </si>
   <si>
     <t>EventEnablingCondition</t>
-  </si>
-  <si>
-    <t>"Accepted single or multiple conditions in the format &lt;Field A&gt;=""Text""OR&lt;Field B&gt;=&lt;Yes/No&gt;
-MaxLength: 1000"</t>
   </si>
 </sst>
 </file>
@@ -2111,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2427,8 +2423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2476,7 +2472,7 @@
         <v>171</v>
       </c>
       <c r="G2" s="85" t="s">
-        <v>221</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
RPET-849 Format SearchCasesResultFields LiveFrom as General
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anatolysanataly/Downloads/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029DA3D5-331E-6549-A096-7E1011F24ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1C8461-5466-0542-ACEC-0307E716284C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" tabRatio="500" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21340" tabRatio="500" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -1073,7 +1073,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1196,6 +1196,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -2108,7 +2109,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2157,7 +2158,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+      <c r="A4" s="86"/>
       <c r="B4" s="57"/>
       <c r="G4" s="58"/>
       <c r="I4" s="59"/>

</xml_diff>

<commit_message>
DFR-19 Set LiveFrom column in SearchCasesResultFields to Date
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anatolysanataly/Downloads/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029DA3D5-331E-6549-A096-7E1011F24ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B079A6-2AAA-F64D-9003-8F2E5D41325A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" tabRatio="500" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21440" tabRatio="500" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <sheet name="AuthorisationCaseState" sheetId="24" r:id="rId24"/>
     <sheet name="AuthorisationComplexType" sheetId="25" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -2108,12 +2108,13 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="11" customWidth="1"/>
+    <col min="1" max="1" width="11" style="57" customWidth="1"/>
+    <col min="2" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -2121,6 +2122,9 @@
         <v>176</v>
       </c>
     </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2"/>
+    </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="56" t="s">
         <v>10</v>
@@ -2157,7 +2161,6 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
       <c r="B4" s="57"/>
       <c r="G4" s="58"/>
       <c r="I4" s="59"/>

</xml_diff>

<commit_message>
DFR-19 Set LiveFrom column in SearchCasesResultFields to Date (#167)
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,40 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anatolysanataly/Downloads/ccd-definition-processor/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1921B4-D7FC-CC4D-A910-DDF15295B251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21420" tabRatio="500" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Jurisdiction" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="CaseRoles" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="CaseType" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="CaseField" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="CaseTypeTab" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="CaseEventToFields" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="CaseEventToComplexTypes" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="State" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="CaseEvent" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="FixedLists" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="ComplexTypes" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="ChallengeQuestion" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="SearchInputFields" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="SearchAlias" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="SearchCasesResultFields" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="SearchResultFields" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="Banner" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="WorkBasketResultFields" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="WorkBasketInputFields" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="UserProfile" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="AuthorisationCaseType" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="AuthorisationCaseField" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="AuthorisationCaseState" sheetId="24" state="visible" r:id="rId25"/>
-    <sheet name="AuthorisationComplexType" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
+    <sheet name="CaseRoles" sheetId="2" r:id="rId2"/>
+    <sheet name="CaseType" sheetId="3" r:id="rId3"/>
+    <sheet name="CaseField" sheetId="4" r:id="rId4"/>
+    <sheet name="CaseTypeTab" sheetId="5" r:id="rId5"/>
+    <sheet name="CaseEventToFields" sheetId="6" r:id="rId6"/>
+    <sheet name="CaseEventToComplexTypes" sheetId="7" r:id="rId7"/>
+    <sheet name="State" sheetId="8" r:id="rId8"/>
+    <sheet name="CaseEvent" sheetId="9" r:id="rId9"/>
+    <sheet name="FixedLists" sheetId="10" r:id="rId10"/>
+    <sheet name="ComplexTypes" sheetId="11" r:id="rId11"/>
+    <sheet name="ChallengeQuestion" sheetId="12" r:id="rId12"/>
+    <sheet name="SearchInputFields" sheetId="13" r:id="rId13"/>
+    <sheet name="SearchAlias" sheetId="14" r:id="rId14"/>
+    <sheet name="SearchCasesResultFields" sheetId="15" r:id="rId15"/>
+    <sheet name="SearchResultFields" sheetId="16" r:id="rId16"/>
+    <sheet name="Banner" sheetId="17" r:id="rId17"/>
+    <sheet name="WorkBasketResultFields" sheetId="18" r:id="rId18"/>
+    <sheet name="WorkBasketInputFields" sheetId="19" r:id="rId19"/>
+    <sheet name="UserProfile" sheetId="20" r:id="rId20"/>
+    <sheet name="AuthorisationCaseType" sheetId="21" r:id="rId21"/>
+    <sheet name="AuthorisationCaseField" sheetId="22" r:id="rId22"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="23" r:id="rId23"/>
+    <sheet name="AuthorisationCaseState" sheetId="24" r:id="rId24"/>
+    <sheet name="AuthorisationComplexType" sheetId="25" r:id="rId25"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -46,761 +51,757 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="221">
   <si>
-    <t xml:space="preserve">Jurisdiction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrimaryKeyInRed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrimaryAndForeignKey Orange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ForeignKey Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start date from which the data will be valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End date until which the data will be valid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The identifier which defines the casetype code
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t>PrimaryKeyInRed</t>
+  </si>
+  <si>
+    <t>PrimaryAndForeignKey Orange</t>
+  </si>
+  <si>
+    <t>ForeignKey Brown</t>
+  </si>
+  <si>
+    <t>Start date from which the data will be valid</t>
+  </si>
+  <si>
+    <t>End date until which the data will be valid</t>
+  </si>
+  <si>
+    <t>The identifier which defines the casetype code
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The short description to describe the jurisdiction used on UI display
+    <t>The short description to describe the jurisdiction used on UI display
 MaxLength: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">The long description to describe the jurisdiction.
+    <t>The long description to describe the jurisdiction.
 MaxLength: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">This can have value TRUE/FALSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LiveFrom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LiveTo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shuttered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseRoles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength: 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength:128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseTypeID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The short description to describe the case type used on the UI.
+    <t>This can have value TRUE/FALSE</t>
+  </si>
+  <si>
+    <t>LiveFrom</t>
+  </si>
+  <si>
+    <t>LiveTo</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Shuttered</t>
+  </si>
+  <si>
+    <t>CaseRoles</t>
+  </si>
+  <si>
+    <t>MaxLength: 40</t>
+  </si>
+  <si>
+    <t>MaxLength:128</t>
+  </si>
+  <si>
+    <t>CaseTypeID</t>
+  </si>
+  <si>
+    <t>CaseType</t>
+  </si>
+  <si>
+    <t>The short description to describe the case type used on the UI.
 MaxLength: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">The long description to decribe the case type.
+    <t>The long description to decribe the case type.
 MaxLength: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">The jurisdiction code should match the one defined in 'Jurisdiction' tab
+    <t>The jurisdiction code should match the one defined in 'Jurisdiction' tab
 MaxLength:70</t>
   </si>
   <si>
-    <t xml:space="preserve">The absolute URL to the microservice which lists the documents that the services wants to provide for print. 
+    <t>The absolute URL to the microservice which lists the documents that the services wants to provide for print. 
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). Max Length: 20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It is a mandatory field which can define if the data classification of the field
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). Max Length: 20</t>
+  </si>
+  <si>
+    <t>It is a mandatory field which can define if the data classification of the field
 MustBe: &lt;Public, Private, Retricted&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">JurisdictionID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PrintableDocumentsUrl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLPrintEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SecurityClassification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseField</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The code of casetype has to be defined in 'CaseType' tab
+    <t>JurisdictionID</t>
+  </si>
+  <si>
+    <t>PrintableDocumentsUrl</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLPrintEvent</t>
+  </si>
+  <si>
+    <t>SecurityClassification</t>
+  </si>
+  <si>
+    <t>CaseField</t>
+  </si>
+  <si>
+    <t>The code of casetype has to be defined in 'CaseType' tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The field ID should match the field attribute name used by the service team in creating the case
+    <t>The field ID should match the field attribute name used by the service team in creating the case
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
+    <t>The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
 MaxLength:&lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The hint text that is present for each field type
+    <t>The hint text that is present for each field type
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The type of field. This can be a CCD Base type (see confluence) or a ComplexType ID as per the ComplexType tab).  
+    <t>The type of field. This can be a CCD Base type (see confluence) or a ComplexType ID as per the ComplexType tab).  
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Some FieldTypes require or have an optional addition parameter that can be set (e.g. Collection - the parameter is the collecion of What FieldType ?, FixedList the parameter is the ID from the fixedList tab). See confluence for details
+    <t>Some FieldTypes require or have an optional addition parameter that can be set (e.g. Collection - the parameter is the collecion of What FieldType ?, FixedList the parameter is the ID from the fixedList tab). See confluence for details
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">The regex that can define the type of data accepted in the fields E.g: alphanumeric etc. This will override the regex, if defined internally for any type.
+    <t>The regex that can define the type of data accepted in the fields E.g: alphanumeric etc. This will override the regex, if defined internally for any type.
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The minimum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
+    <t>The minimum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The maximum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
+    <t>The maximum that the field Value should support for the FieldType (e.g. for Text its length, for Number it’s a value)
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HintText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldTypeParameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RegularExpression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Searchable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseTypeTab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not used yet - maybe used for roletype type view later
+    <t>Yes/Y/True if field should be included in ES index. No/N/False if filed should be excluded from ES index.</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>HintText</t>
+  </si>
+  <si>
+    <t>FieldType</t>
+  </si>
+  <si>
+    <t>FieldTypeParameter</t>
+  </si>
+  <si>
+    <t>RegularExpression</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Searchable</t>
+  </si>
+  <si>
+    <t>CaseTypeTab</t>
+  </si>
+  <si>
+    <t>Not used yet - maybe used for roletype type view later
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">Unique Id for tab. MaxLength: 40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name to be displayed on the tab
+    <t>Unique Id for tab. MaxLength: 40</t>
+  </si>
+  <si>
+    <t>Name to be displayed on the tab
 MaxLengh: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">Order of Tab on screen - left to right.
+    <t>Order of Tab on screen - left to right.
 PositiveInteger</t>
   </si>
   <si>
-    <t xml:space="preserve">Unique ID for field - must match an ID on the CaseField tab or be a metadata item. 
+    <t>Unique ID for field - must match an ID on the CaseField tab or be a metadata item. 
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order of Fields within a tab - top to bottom
+    <t>MaxLength: 100. No entry for role means no role restriction for that tab. Enter role on a single row per tab</t>
+  </si>
+  <si>
+    <t>Order of Fields within a tab - top to bottom
 PositiveInteger</t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
+    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
 MaxLength:1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean expression rules for hiding a tab: 
+    <t>Boolean expression rules for hiding a tab: 
 MaxLength:1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Text should begin with #LIST( or #TABLE(
+    <t>Text should begin with #LIST( or #TABLE(
 MaxLength: 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Channel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseFieldID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserRole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabFieldDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldShowCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TabShowCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DisplayContextParameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventToFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique ID for the event. Not listing an case event means that All Fields are displayed. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This defines with Fields can be changed / viewed during an case event. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The order of the fields on the screen.
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>TabID</t>
+  </si>
+  <si>
+    <t>TabLabel</t>
+  </si>
+  <si>
+    <t>TabDisplayOrder</t>
+  </si>
+  <si>
+    <t>CaseFieldID</t>
+  </si>
+  <si>
+    <t>UserRole</t>
+  </si>
+  <si>
+    <t>TabFieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>FieldShowCondition</t>
+  </si>
+  <si>
+    <t>TabShowCondition</t>
+  </si>
+  <si>
+    <t>DisplayContextParameter</t>
+  </si>
+  <si>
+    <t>CaseEventToFields</t>
+  </si>
+  <si>
+    <t>Unique ID for the event. Not listing an case event means that All Fields are displayed. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>This defines with Fields can be changed / viewed during an case event. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>The order of the fields on the screen.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted Values:  for mandatory, readonly and optional data on UI
+    <t>Accepted Values:  for mandatory, readonly and optional data on UI
 MustBe: MANDATORY, READONLY, OPTIONAL</t>
   </si>
   <si>
-    <t xml:space="preserve">This is a string value which defines the Wizard pages' ID
+    <t>This is a string value which defines the Wizard pages' ID
 MaxLength:40</t>
   </si>
   <si>
-    <t xml:space="preserve">This is a string value which defines the Wizard pages' Label
+    <t>This is a string value which defines the Wizard pages' Label
 MaxLength:40</t>
   </si>
   <si>
-    <t xml:space="preserve">The order to display the pages
+    <t>The order to display the pages
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Currently blank 1 or 2.  2 currently will display the yellow review column.
+    <t>Currently blank 1 or 2.  2 currently will display the yellow review column.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
+    <t>Accepted single or multiple conditions in the format &lt;Field A&gt;="Text"OR&lt;Field B&gt;=&lt;Yes/No&gt;
 MaxLength: 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean expression rules for hiding a page: MaxLength:1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">States a field should appear on check your answers However these fields will be considered only "ShowSummary" column in CaseEvent tab is set to Y
+    <t>Boolean expression rules for hiding a page: MaxLength:1000</t>
+  </si>
+  <si>
+    <t>States a field should appear on check your answers However these fields will be considered only "ShowSummary" column in CaseEvent tab is set to Y
 CouldBe: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">URL to call back to the service for uniqueness. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a string value overrides label from CaseField tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is a string value overrides hint from CaseField tab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boolean value to say if an event can be published</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageFieldDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DisplayContext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageColumnNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PageShowCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowSummaryChangeOption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowSummaryContentOption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLMidEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLMidEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventFieldLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEventFieldHint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetainHiddenValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Publish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventToComplexTypes</t>
+    <t>URL to call back to the service for uniqueness. </t>
+  </si>
+  <si>
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). </t>
+  </si>
+  <si>
+    <t>This is a string value overrides label from CaseField tab</t>
+  </si>
+  <si>
+    <t>This is a string value overrides hint from CaseField tab</t>
+  </si>
+  <si>
+    <t>Boolean value to say if an event can be published</t>
+  </si>
+  <si>
+    <t>CaseEventID</t>
+  </si>
+  <si>
+    <t>PageFieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>DisplayContext</t>
+  </si>
+  <si>
+    <t>PageID</t>
+  </si>
+  <si>
+    <t>PageLabel</t>
+  </si>
+  <si>
+    <t>PageDisplayOrder</t>
+  </si>
+  <si>
+    <t>PageColumnNumber</t>
+  </si>
+  <si>
+    <t>PageShowCondition</t>
+  </si>
+  <si>
+    <t>ShowSummaryChangeOption</t>
+  </si>
+  <si>
+    <t>ShowSummaryContentOption</t>
+  </si>
+  <si>
+    <t>CallBackURLMidEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLMidEvent</t>
+  </si>
+  <si>
+    <t>CaseEventFieldLabel</t>
+  </si>
+  <si>
+    <t>CaseEventFieldHint</t>
+  </si>
+  <si>
+    <t>RetainHiddenValue</t>
+  </si>
+  <si>
+    <t>Publish</t>
+  </si>
+  <si>
+    <t>EventToComplexTypes</t>
   </si>
   <si>
     <t xml:space="preserve">
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">MaxLength:70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength:200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxLength:300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ListElementCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DefaultValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventElementLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventHintText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FieldDisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State with ID '*' and Name 'DEFAULT' is a reserved state. The state can be used for events where states do not change.
+    <t>MaxLength:70</t>
+  </si>
+  <si>
+    <t>MaxLength:200</t>
+  </si>
+  <si>
+    <t>MaxLength:300</t>
+  </si>
+  <si>
+    <t>ListElementCode</t>
+  </si>
+  <si>
+    <t>DefaultValue</t>
+  </si>
+  <si>
+    <t>EventElementLabel</t>
+  </si>
+  <si>
+    <t>EventHintText</t>
+  </si>
+  <si>
+    <t>FieldDisplayOrder</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>State with ID '*' and Name 'DEFAULT' is a reserved state. The state can be used for events where states do not change.
 MaxLength:70</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the name of the state as displayed on UI
+    <t>This is the name of the state as displayed on UI
 MaxLength:100</t>
   </si>
   <si>
-    <t xml:space="preserve">This gives longer decription of the case state
+    <t>This gives longer decription of the case state
 Max Length: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">The order of the states on the screen.
+    <t>The order of the states on the screen.
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Optional override of title used in the CaseTabView. Markdown , concat supported
+    <t>Optional override of title used in the CaseTabView. Markdown , concat supported
 MaxLength: 100</t>
   </si>
   <si>
-    <t xml:space="preserve">DisplayOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TitleDisplay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CaseEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique ID for the event
+    <t>DisplayOrder</t>
+  </si>
+  <si>
+    <t>TitleDisplay</t>
+  </si>
+  <si>
+    <t>CaseEvent</t>
+  </si>
+  <si>
+    <t>Unique ID for the event
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the name of the event as displayed on UI Dropdown list - hence limited to 30
+    <t>This is the name of the event as displayed on UI Dropdown list - hence limited to 30
 MaxLength: 30</t>
   </si>
   <si>
-    <t xml:space="preserve">This gives further details of an event of a case
+    <t>This gives further details of an event of a case
 MaxLength:100</t>
   </si>
   <si>
-    <t xml:space="preserve">The display order of displaying the events in the list
+    <t>The display order of displaying the events in the list
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">Future Elements not for MVP (what about multiple state) (semicolon ; seprated list).
+    <t>Future Elements not for MVP (what about multiple state) (semicolon ; seprated list).
 If '*' is provided, then precondition will not be validated and will be considered as current state
  MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Future Elements not for MVP. 
+    <t>Future Elements not for MVP. 
 If '*' is provided, then the current state will not change and will be same as pre condition state
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">URL to call back to the service for uniqueness. 
+    <t>URL to call back to the service for uniqueness. 
 Max Length: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). 
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). 
 MaxLength: &lt;unlimited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Y, N and empty. TheCheck your answer section will be shown on Y (true) and empty(null) values, but not shown on N (false) values. Fields on CaseEventTo Field tab have Y in "ShowSummaryChangeOption" column.
+    <t>Y, N and empty. TheCheck your answer section will be shown on Y (true) and empty(null) values, but not shown on N (false) values. Fields on CaseEventTo Field tab have Y in "ShowSummaryChangeOption" column.
 CouldBe: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean value to say if the enter summary and event description fields are to be shown
+    <t>Boolean value to say if the enter summary and event description fields are to be shown
 CouldBeh: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Boolean value to say if a draft of a create event can be saved
+    <t>Boolean value to say if a draft of a create event can be saved
 CouldBe: &lt;Y,N&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">The label of the button on the final event screen - default is Submit
+    <t>The label of the button on the final event screen - default is Submit
 MaxLength: 200</t>
   </si>
   <si>
-    <t xml:space="preserve">PreConditionState(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PostConditionState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLAboutToStartEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutAboutToStartEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLAboutToSubmitEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLAboutToSubmitEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CallBackURLSubmittedEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RetriesTimeoutURLSubmittedEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowSummary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShowEventNotes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CanSaveDraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndButtonLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EventEnablingCondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FixedLists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The unique identifier of the Fixed list
+    <t>PreConditionState(s)</t>
+  </si>
+  <si>
+    <t>PostConditionState</t>
+  </si>
+  <si>
+    <t>CallBackURLAboutToStartEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutAboutToStartEvent</t>
+  </si>
+  <si>
+    <t>CallBackURLAboutToSubmitEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLAboutToSubmitEvent</t>
+  </si>
+  <si>
+    <t>CallBackURLSubmittedEvent</t>
+  </si>
+  <si>
+    <t>RetriesTimeoutURLSubmittedEvent</t>
+  </si>
+  <si>
+    <t>ShowSummary</t>
+  </si>
+  <si>
+    <t>ShowEventNotes</t>
+  </si>
+  <si>
+    <t>CanSaveDraft</t>
+  </si>
+  <si>
+    <t>EndButtonLabel</t>
+  </si>
+  <si>
+    <t>EventEnablingCondition</t>
+  </si>
+  <si>
+    <t>FixedLists</t>
+  </si>
+  <si>
+    <t>The unique identifier of the Fixed list
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">The unque ID of an element in the list (ID)
+    <t>The unque ID of an element in the list (ID)
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">The Display name for the list item
+    <t>The Display name for the list item
 MaxLength: 250</t>
   </si>
   <si>
-    <t xml:space="preserve">The display order of list items. Positive integers e.g 1, 2, 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ListElement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ComplexTypes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The ComplexType ID should match the field attribute name on the CaseField Tab
+    <t>The display order of list items. Positive integers e.g 1, 2, 3</t>
+  </si>
+  <si>
+    <t>ListElement</t>
+  </si>
+  <si>
+    <t>ComplexTypes</t>
+  </si>
+  <si>
+    <t>The ComplexType ID should match the field attribute name on the CaseField Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The complex type element (field) ID (ListElementId) should match the field attribute name used by the service team in creating the case
+    <t>The complex type element (field) ID (ListElementId) should match the field attribute name used by the service team in creating the case
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
+    <t>The lable that will be used on the UI for the case field. It is possible to add Markdown to the label element. This feature allows to provide html styling (limited) and interpolate the value of another case field. See the feature in details on confluence (Label Markdown and interpolation)
 MaxLength:200</t>
   </si>
   <si>
-    <t xml:space="preserve">Within a complex type any field can be hidden or shown based on another field's values in the same level.
+    <t>Within a complex type any field can be hidden or shown based on another field's values in the same level.
 Currently only single boolean or string conditions are supported. Eg: country="Italy" or country startWith: "Uni"
 MaxLength: 1000</t>
   </si>
   <si>
-    <t xml:space="preserve">The hint text that is present for each field type
+    <t>The hint text that is present for each field type
 MaxLength: &lt;unlmited&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">ElementLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ChallengeQuestion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order of fields on UI
+    <t>ElementLabel</t>
+  </si>
+  <si>
+    <t>ChallengeQuestion</t>
+  </si>
+  <si>
+    <t>Order of fields on UI
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">The type of the field that the answer will contain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In the form of a comma separated list of potential answer field(s) for each of the (n) litigant types on possible on the case.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QuestionText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AnswerFieldType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QuestionId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchInputFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fields that can be searched on. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Label next to search field on UI.
+    <t>The type of the field that the answer will contain</t>
+  </si>
+  <si>
+    <t>In the form of a comma separated list of potential answer field(s) for each of the (n) litigant types on possible on the case.</t>
+  </si>
+  <si>
+    <t>QuestionText</t>
+  </si>
+  <si>
+    <t>AnswerFieldType</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>QuestionId</t>
+  </si>
+  <si>
+    <t>SearchInputFields</t>
+  </si>
+  <si>
+    <t>Fields that can be searched on. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Label next to search field on UI.
 MaxLength: 200</t>
   </si>
   <si>
-    <t xml:space="preserve">Order of fields on UI 
+    <t>Order of fields on UI 
 Positive Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">SearchAlias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique alias id for a case field of a case type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is just the CaseField ID for top level fields, or object notation pointing to a complex type field e.g. applicantAddress.AddressLine1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchAliasID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchCasesResultFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ResultsOrdering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UseCase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SearchResultFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fields to be displayed in results list. MaxLength: 70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name on the results column.for the field
+    <t>SearchAlias</t>
+  </si>
+  <si>
+    <t>Unique alias id for a case field of a case type</t>
+  </si>
+  <si>
+    <t>This is just the CaseField ID for top level fields, or object notation pointing to a complex type field e.g. applicantAddress.AddressLine1</t>
+  </si>
+  <si>
+    <t>SearchAliasID</t>
+  </si>
+  <si>
+    <t>SearchCasesResultFields</t>
+  </si>
+  <si>
+    <t>ResultsOrdering</t>
+  </si>
+  <si>
+    <t>UseCase</t>
+  </si>
+  <si>
+    <t>SearchResultFields</t>
+  </si>
+  <si>
+    <t>Fields to be displayed in results list. MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Name on the results column.for the field
 MaxLength: 200</t>
   </si>
   <si>
-    <t xml:space="preserve">Order the columns are displayed.
+    <t>Order the columns are displayed.
 Positive Integer</t>
   </si>
   <si>
     <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
   </si>
   <si>
-    <t xml:space="preserve">Fields can be ordered on by user role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Banner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes or No, to enable or disable the banner.                          MaxLength: 30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Content to display in the banner         MaxLength: 300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optional link text in the banner                   MaxLength:50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The URL for the link text.                                               Max Length: 1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BannerEnabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BannerDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BannerUrlText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BannerUrl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketResultFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketInputFields</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UserProfile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID from Jurisdiction Tab
+    <t>Fields can be ordered on by user role</t>
+  </si>
+  <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>Yes or No, to enable or disable the banner.                          MaxLength: 30</t>
+  </si>
+  <si>
+    <t>Content to display in the banner         MaxLength: 300</t>
+  </si>
+  <si>
+    <t>Optional link text in the banner                   MaxLength:50</t>
+  </si>
+  <si>
+    <t>The URL for the link text.                                               Max Length: 1000</t>
+  </si>
+  <si>
+    <t>BannerEnabled</t>
+  </si>
+  <si>
+    <t>BannerDescription</t>
+  </si>
+  <si>
+    <t>BannerUrlText</t>
+  </si>
+  <si>
+    <t>BannerUrl</t>
+  </si>
+  <si>
+    <t>WorkBasketResultFields</t>
+  </si>
+  <si>
+    <t>WorkBasketInputFields</t>
+  </si>
+  <si>
+    <t>UserProfile</t>
+  </si>
+  <si>
+    <t>Must match ID from Jurisdiction Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID from CaseType Tab
+    <t>Must match ID from CaseType Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID from State Tab
+    <t>Must match ID from State Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">UserIDAMId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketDefaultJurisdiction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketDefaultCaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WorkBasketDefaultState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthorisationCaseType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID in 'CaseType' tab
+    <t>UserIDAMId</t>
+  </si>
+  <si>
+    <t>WorkBasketDefaultJurisdiction</t>
+  </si>
+  <si>
+    <t>WorkBasketDefaultCaseType</t>
+  </si>
+  <si>
+    <t>WorkBasketDefaultState</t>
+  </si>
+  <si>
+    <t>AuthorisationCaseType</t>
+  </si>
+  <si>
+    <t>Must match ID in 'CaseType' tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID role.  If a role doesn’t have a Row below that mean no access to.
+    <t>Must match ID role.  If a role doesn’t have a Row below that mean no access to.
 MaxLength: 100.</t>
   </si>
   <si>
-    <t xml:space="preserve">C - Create, R - Read, U - Update, D - Delete
+    <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">CRUD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthorisationCaseField</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID on 'CaseType' tab
+    <t>CRUD</t>
+  </si>
+  <si>
+    <t>AuthorisationCaseField</t>
+  </si>
+  <si>
+    <t>Must match ID on 'CaseType' tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">Must match ID on CaseField tab.
+    <t>Must match ID on CaseField tab.
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">AuthorisationCaseEvent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Must match ID on Event tabe.
+    <t>AuthorisationCaseEvent</t>
+  </si>
+  <si>
+    <t>Must match ID on Event tabe.
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">AuthorisationCaseState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Muust match an ID on State tab.
+    <t>AuthorisationCaseState</t>
+  </si>
+  <si>
+    <t>Muust match an ID on State tab.
 MaxLength: 40</t>
   </si>
   <si>
-    <t xml:space="preserve">CaseStateID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AuthorisationComplexType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Field ID should match an ID in the CaseField Tab
+    <t>CaseStateID</t>
+  </si>
+  <si>
+    <t>AuthorisationComplexType</t>
+  </si>
+  <si>
+    <t>The Field ID should match an ID in the CaseField Tab
 MaxLength: 70</t>
   </si>
   <si>
-    <t xml:space="preserve">C - Create, R - Read, U - Update, D - Delete
+    <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY;@"/>
-    <numFmt numFmtId="166" formatCode="@"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="168" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="169" formatCode="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -809,22 +810,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -858,14 +844,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
+      <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -873,14 +859,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -888,7 +874,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -896,7 +882,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -911,7 +897,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFFC000"/>
       <name val="Arial"/>
@@ -919,7 +905,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFF6600"/>
       <name val="Arial"/>
@@ -927,7 +913,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF984807"/>
       <name val="Arial"/>
@@ -935,7 +921,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
@@ -943,7 +929,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -971,7 +957,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFC000"/>
       <name val="Calibri"/>
@@ -1007,7 +993,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
@@ -1022,7 +1008,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF172B4D"/>
       <name val="Arial"/>
@@ -1039,14 +1025,14 @@
     </fill>
   </fills>
   <borders count="3">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF000080"/>
       </left>
@@ -1061,394 +1047,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="85">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1507,29 +1252,337 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    <sheetView topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1544,7 +1597,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1564,7 +1617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -1585,34 +1638,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>148</v>
       </c>
@@ -1627,7 +1672,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1647,7 +1692,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -1668,36 +1713,28 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="14" width="10.5" customWidth="1"/>
+    <col min="15" max="15" width="26.83203125" customWidth="1"/>
+    <col min="16" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>154</v>
       </c>
@@ -1720,7 +1757,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="409.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1764,7 +1801,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -1812,41 +1849,33 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="46" t="s">
         <v>161</v>
       </c>
@@ -1860,7 +1889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="112" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1889,7 +1918,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -1922,34 +1951,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>169</v>
       </c>
@@ -1965,7 +1986,7 @@
       <c r="E1" s="55"/>
       <c r="F1" s="55"/>
     </row>
-    <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1985,7 +2006,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2006,36 +2027,28 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.5"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>173</v>
       </c>
@@ -2049,7 +2062,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
         <v>174</v>
@@ -2061,7 +2074,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="56" t="s">
         <v>19</v>
       </c>
@@ -2076,38 +2089,34 @@
       <c r="F3" s="10"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11"/>
+    <col min="1" max="1" width="11" style="1" customWidth="1"/>
+    <col min="2" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="57" t="s">
         <v>10</v>
       </c>
@@ -2142,42 +2151,33 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="58"/>
       <c r="G4" s="59"/>
       <c r="I4" s="60"/>
       <c r="K4" s="61"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>180</v>
       </c>
@@ -2193,7 +2193,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="141" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2246,34 +2246,24 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>186</v>
       </c>
@@ -2283,7 +2273,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>187</v>
       </c>
@@ -2299,7 +2289,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>191</v>
       </c>
@@ -2316,40 +2306,32 @@
       <c r="F3" s="20"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>195</v>
       </c>
@@ -2367,7 +2349,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="64"/>
     </row>
-    <row r="2" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" ht="141" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2396,7 +2378,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2426,39 +2408,31 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="9" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="66" t="s">
         <v>196</v>
       </c>
@@ -2475,7 +2449,7 @@
       <c r="F1" s="69"/>
       <c r="G1" s="69"/>
     </row>
-    <row r="2" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="141" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2501,7 +2475,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2528,37 +2502,29 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.5"/>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>16</v>
       </c>
@@ -2572,7 +2538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>17</v>
       </c>
@@ -2592,11 +2558,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -2613,34 +2579,24 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>197</v>
       </c>
@@ -2656,7 +2612,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2674,7 +2630,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2695,34 +2651,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>205</v>
       </c>
@@ -2737,7 +2685,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2754,7 +2702,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -2772,34 +2720,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="71" t="s">
         <v>210</v>
       </c>
@@ -2815,7 +2755,7 @@
       <c r="E1" s="72"/>
       <c r="F1" s="72"/>
     </row>
-    <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2835,7 +2775,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>10</v>
       </c>
@@ -2856,34 +2796,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>213</v>
       </c>
@@ -2899,7 +2831,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2919,7 +2851,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -2940,34 +2872,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>215</v>
       </c>
@@ -2983,7 +2907,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="127" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3003,7 +2927,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -3024,33 +2948,25 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.5"/>
+    <col min="1" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="78" t="s">
         <v>218</v>
       </c>
@@ -3067,7 +2983,7 @@
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
     </row>
-    <row r="2" customFormat="false" ht="253" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" ht="253" x14ac:dyDescent="0.2">
       <c r="A2" s="82"/>
       <c r="B2" s="82"/>
       <c r="C2" s="83" t="s">
@@ -3086,7 +3002,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="84" t="s">
         <v>10</v>
       </c>
@@ -3110,10 +3026,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
@@ -3121,23 +3036,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>20</v>
       </c>
@@ -3156,7 +3068,7 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="211" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" ht="211" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3185,7 +3097,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="43" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" ht="43" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
@@ -3215,34 +3127,26 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -3264,7 +3168,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="409.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3305,7 +3209,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -3347,37 +3251,29 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="11" width="10.5" customWidth="1"/>
+    <col min="12" max="12" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" customWidth="1"/>
+    <col min="14" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -3399,7 +3295,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="183" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13" ht="183" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3440,7 +3336,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -3482,44 +3378,36 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
+    <sheetView topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="30.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="23.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="9" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="26.1640625" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10.5" customWidth="1"/>
+    <col min="15" max="15" width="24.33203125" customWidth="1"/>
+    <col min="16" max="18" width="10.5" customWidth="1"/>
+    <col min="19" max="19" width="23.6640625" customWidth="1"/>
+    <col min="20" max="20" width="20.5" customWidth="1"/>
+    <col min="21" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>71</v>
       </c>
@@ -3544,7 +3432,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="253" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:21" ht="253" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3606,7 +3494,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -3672,45 +3560,37 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:Y3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AMK3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="25" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="26" width="30.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="26" width="12.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="26" width="9.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="26" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="26" width="16.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="26" width="17.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="26" width="6.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="15" style="27" width="6.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="28" width="6.33"/>
+    <col min="1" max="1" width="19.5" style="25" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" style="26" customWidth="1"/>
+    <col min="5" max="7" width="30.1640625" style="26" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="26" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="26" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" style="26" customWidth="1"/>
+    <col min="12" max="12" width="17.5" style="26" customWidth="1"/>
+    <col min="13" max="14" width="6.33203125" style="26" customWidth="1"/>
+    <col min="15" max="1022" width="6.33203125" style="27" customWidth="1"/>
+    <col min="1023" max="1025" width="6.33203125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>104</v>
       </c>
@@ -3724,7 +3604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" s="37" customFormat="true" ht="140" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:25" s="37" customFormat="1" ht="140" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
@@ -3775,7 +3655,7 @@
       <c r="X2" s="36"/>
       <c r="Y2" s="36"/>
     </row>
-    <row r="3" s="27" customFormat="true" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:25" s="27" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="38" t="s">
         <v>10</v>
       </c>
@@ -3817,10 +3697,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
@@ -3828,23 +3707,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>114</v>
       </c>
@@ -3862,7 +3738,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="225" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="225" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -3888,7 +3764,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -3915,38 +3791,30 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
+    <sheetView topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="3" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="29.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="10.5"/>
+    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="19" width="10.5" customWidth="1"/>
+    <col min="20" max="20" width="14.6640625" customWidth="1"/>
+    <col min="21" max="21" width="10.5" customWidth="1"/>
+    <col min="22" max="22" width="29.33203125" customWidth="1"/>
+    <col min="23" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>122</v>
       </c>
@@ -3976,7 +3844,7 @@
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="333" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:22" ht="333" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -4044,7 +3912,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:22" ht="57" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -4113,12 +3981,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tempalte update for display parameter
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anatolysanataly/Downloads/ccd-definition-processor/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdullah/Desktop/probate-repos/ccd-definition-processor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1921B4-D7FC-CC4D-A910-DDF15295B251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3045D6F-1449-2E45-B7EC-2EC5C60C9E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21420" tabRatio="500" firstSheet="12" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20320" tabRatio="500" firstSheet="12" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="222">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -791,6 +791,9 @@
   <si>
     <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
+  </si>
+  <si>
+    <t>Format of the fields</t>
   </si>
 </sst>
 </file>
@@ -1958,10 +1961,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1970,7 +1973,7 @@
     <col min="3" max="1025" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>169</v>
       </c>
@@ -1986,7 +1989,7 @@
       <c r="E1" s="55"/>
       <c r="F1" s="55"/>
     </row>
-    <row r="2" spans="1:6" ht="113" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="113" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2005,8 +2008,11 @@
       <c r="F2" s="8" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2024,6 +2030,9 @@
       </c>
       <c r="F3" s="10" t="s">
         <v>120</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2098,7 +2107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:A1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update SearchInputFields and WorkBasketInputFields
- Add ListElementCode, FieldShowCondition and UserRole to SearchInputFields
- Add UserRole to WorkBasketInputFields
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="225">
   <si>
     <t xml:space="preserve">Jurisdiction</t>
   </si>
@@ -642,6 +642,9 @@
 Positive Integer</t>
   </si>
   <si>
+    <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
+  </si>
+  <si>
     <t xml:space="preserve">SearchAlias</t>
   </si>
   <si>
@@ -675,9 +678,6 @@
   <si>
     <t xml:space="preserve">Order the columns are displayed.
 Positive Integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
   </si>
   <si>
     <t xml:space="preserve">Fields can be ordered on by user role</t>
@@ -1075,6 +1075,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FF000080"/>
       </left>
@@ -1087,13 +1094,6 @@
       <bottom style="thin">
         <color rgb="FF000080"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -1126,7 +1126,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="90">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1359,6 +1359,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1375,7 +1391,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1383,19 +1399,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1559,7 +1571,7 @@
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -1621,8 +1633,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1641,7 +1653,7 @@
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -1703,8 +1715,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1723,7 +1735,7 @@
       <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.83"/>
@@ -1845,8 +1857,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1865,7 +1877,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0078125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.66"/>
@@ -1954,8 +1966,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1968,18 +1980,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>173</v>
       </c>
@@ -1995,7 +2008,7 @@
       <c r="E1" s="57"/>
       <c r="F1" s="57"/>
     </row>
-    <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2008,37 +2021,53 @@
       <c r="D2" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="61" t="s">
         <v>124</v>
+      </c>
+      <c r="H3" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="61" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2057,7 +2086,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.84"/>
@@ -2066,7 +2095,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B1" s="54" t="s">
         <v>1</v>
@@ -2081,33 +2110,33 @@
     <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="58" t="s">
-        <v>180</v>
-      </c>
-      <c r="C3" s="58" t="s">
+      <c r="B3" s="62" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="58"/>
+      <c r="D3" s="62"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2126,61 +2155,61 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0078125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="59" t="s">
+      <c r="G3" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="59" t="s">
+      <c r="H3" s="63" t="s">
         <v>124</v>
       </c>
-      <c r="I3" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="J3" s="59" t="s">
+      <c r="I3" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="J3" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="59" t="s">
-        <v>183</v>
+      <c r="K3" s="63" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="60"/>
-      <c r="G4" s="61"/>
-      <c r="I4" s="62"/>
-      <c r="K4" s="63"/>
+      <c r="B4" s="64"/>
+      <c r="G4" s="65"/>
+      <c r="I4" s="66"/>
+      <c r="K4" s="67"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2199,14 +2228,14 @@
       <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2231,18 +2260,18 @@
         <v>36</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="G2" s="64" t="s">
         <v>188</v>
       </c>
-      <c r="H2" s="64" t="s">
+      <c r="G2" s="59" t="s">
+        <v>177</v>
+      </c>
+      <c r="H2" s="59" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2253,10 +2282,10 @@
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="62" t="s">
         <v>69</v>
       </c>
       <c r="E3" s="10" t="s">
@@ -2265,17 +2294,17 @@
       <c r="F3" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="65" t="s">
-        <v>182</v>
+      <c r="H3" s="68" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2294,7 +2323,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -2343,8 +2372,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2363,7 +2392,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15"/>
@@ -2384,10 +2413,10 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66"/>
+      <c r="E1" s="69"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="66"/>
+      <c r="H1" s="69"/>
     </row>
     <row r="2" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
@@ -2400,21 +2429,21 @@
         <v>36</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E2" s="64" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="59" t="s">
         <v>160</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="H2" s="64" t="s">
         <v>188</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="H2" s="59" t="s">
+        <v>177</v>
+      </c>
+      <c r="I2" s="59" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2425,13 +2454,13 @@
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="67" t="s">
+      <c r="E3" s="70" t="s">
         <v>113</v>
       </c>
       <c r="F3" s="10" t="s">
@@ -2440,17 +2469,17 @@
       <c r="G3" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="H3" s="65" t="s">
+      <c r="H3" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="65" t="s">
-        <v>182</v>
+      <c r="I3" s="68" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2463,13 +2492,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15"/>
@@ -2477,24 +2506,24 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="68" t="s">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="71" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-    </row>
-    <row r="2" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="69"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+    </row>
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2507,7 +2536,7 @@
       <c r="D2" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="59" t="s">
         <v>160</v>
       </c>
       <c r="F2" s="8" t="s">
@@ -2519,21 +2548,24 @@
       <c r="H2" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I2" s="59" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="67" t="s">
+      <c r="E3" s="70" t="s">
         <v>113</v>
       </c>
       <c r="F3" s="10" t="s">
@@ -2542,14 +2574,18 @@
       <c r="G3" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="H3" s="72" t="s">
+      <c r="H3" s="75" t="s">
         <v>72</v>
       </c>
-    </row>
+      <c r="I3" s="61" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2568,7 +2604,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.33"/>
@@ -2632,8 +2668,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2652,7 +2688,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -2713,8 +2749,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2733,7 +2769,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -2789,8 +2825,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2809,13 +2845,13 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="76" t="s">
         <v>214</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -2827,8 +2863,8 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
     </row>
     <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
@@ -2857,13 +2893,13 @@
       <c r="B3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="78" t="s">
         <v>70</v>
       </c>
       <c r="F3" s="26" t="s">
@@ -2872,8 +2908,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2892,7 +2928,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -2940,13 +2976,13 @@
       <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="78" t="s">
         <v>70</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -2955,8 +2991,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2975,7 +3011,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -2984,13 +3020,13 @@
       <c r="A1" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="81" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="6"/>
@@ -3006,7 +3042,7 @@
       <c r="C2" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="82" t="s">
         <v>220</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -3023,13 +3059,13 @@
       <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="78" t="s">
         <v>221</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="78" t="s">
         <v>70</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -3038,8 +3074,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3058,19 +3094,19 @@
       <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="83" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="83" t="s">
+      <c r="D1" s="86" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="30"/>
@@ -3078,29 +3114,29 @@
       <c r="G1" s="30"/>
     </row>
     <row r="2" customFormat="false" ht="253" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="84"/>
-      <c r="B2" s="84"/>
-      <c r="C2" s="85" t="s">
+      <c r="A2" s="87"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="88" t="s">
         <v>215</v>
       </c>
-      <c r="D2" s="85" t="s">
+      <c r="D2" s="88" t="s">
         <v>223</v>
       </c>
-      <c r="E2" s="85" t="s">
+      <c r="E2" s="88" t="s">
         <v>160</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="88" t="s">
         <v>211</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="88" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="89" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="42" t="s">
@@ -3112,17 +3148,17 @@
       <c r="E3" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="F3" s="86" t="s">
+      <c r="F3" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="86" t="s">
+      <c r="G3" s="89" t="s">
         <v>213</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -3137,11 +3173,11 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -3237,8 +3273,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3257,7 +3293,7 @@
       <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -3368,8 +3404,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3388,7 +3424,7 @@
       <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.5"/>
@@ -3501,8 +3537,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3521,7 +3557,7 @@
       <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.16"/>
@@ -3687,8 +3723,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3833,7 +3869,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -3852,7 +3888,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -3929,8 +3965,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3949,7 +3985,7 @@
       <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.66"/>
@@ -4124,8 +4160,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Update SearchInputFields and WorkBasketInputFields (#212)
- Add ListElementCode, FieldShowCondition and UserRole to SearchInputFields
- Add UserRole to WorkBasketInputFields
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="225">
   <si>
     <t xml:space="preserve">Jurisdiction</t>
   </si>
@@ -642,6 +642,9 @@
 Positive Integer</t>
   </si>
   <si>
+    <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
+  </si>
+  <si>
     <t xml:space="preserve">SearchAlias</t>
   </si>
   <si>
@@ -675,9 +678,6 @@
   <si>
     <t xml:space="preserve">Order the columns are displayed.
 Positive Integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fields that can be searched on by user role. If blank, available to all. Must match ID role. </t>
   </si>
   <si>
     <t xml:space="preserve">Fields can be ordered on by user role</t>
@@ -1075,6 +1075,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
         <color rgb="FF000080"/>
       </left>
@@ -1087,13 +1094,6 @@
       <bottom style="thin">
         <color rgb="FF000080"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -1126,7 +1126,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="90">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1359,6 +1359,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1375,7 +1391,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1383,19 +1399,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1559,7 +1571,7 @@
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -1621,8 +1633,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1641,7 +1653,7 @@
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -1703,8 +1715,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1723,7 +1735,7 @@
       <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.83"/>
@@ -1845,8 +1857,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1865,7 +1877,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0078125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.66"/>
@@ -1954,8 +1966,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1968,18 +1980,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>173</v>
       </c>
@@ -1995,7 +2008,7 @@
       <c r="E1" s="57"/>
       <c r="F1" s="57"/>
     </row>
-    <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2008,37 +2021,53 @@
       <c r="D2" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="61" t="s">
         <v>124</v>
+      </c>
+      <c r="H3" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="61" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2057,7 +2086,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.84"/>
@@ -2066,7 +2095,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B1" s="54" t="s">
         <v>1</v>
@@ -2081,33 +2110,33 @@
     <row r="2" customFormat="false" ht="113" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="58" t="s">
-        <v>180</v>
-      </c>
-      <c r="C3" s="58" t="s">
+      <c r="B3" s="62" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="58"/>
+      <c r="D3" s="62"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2126,61 +2155,61 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.0078125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="59" t="s">
+      <c r="G3" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="59" t="s">
+      <c r="H3" s="63" t="s">
         <v>124</v>
       </c>
-      <c r="I3" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="J3" s="59" t="s">
+      <c r="I3" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="J3" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="59" t="s">
-        <v>183</v>
+      <c r="K3" s="63" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="60"/>
-      <c r="G4" s="61"/>
-      <c r="I4" s="62"/>
-      <c r="K4" s="63"/>
+      <c r="B4" s="64"/>
+      <c r="G4" s="65"/>
+      <c r="I4" s="66"/>
+      <c r="K4" s="67"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2199,14 +2228,14 @@
       <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2231,18 +2260,18 @@
         <v>36</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="G2" s="64" t="s">
         <v>188</v>
       </c>
-      <c r="H2" s="64" t="s">
+      <c r="G2" s="59" t="s">
+        <v>177</v>
+      </c>
+      <c r="H2" s="59" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2253,10 +2282,10 @@
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="62" t="s">
         <v>69</v>
       </c>
       <c r="E3" s="10" t="s">
@@ -2265,17 +2294,17 @@
       <c r="F3" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="65" t="s">
-        <v>182</v>
+      <c r="H3" s="68" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2294,7 +2323,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -2343,8 +2372,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2363,7 +2392,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15"/>
@@ -2384,10 +2413,10 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66"/>
+      <c r="E1" s="69"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="66"/>
+      <c r="H1" s="69"/>
     </row>
     <row r="2" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
@@ -2400,21 +2429,21 @@
         <v>36</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E2" s="64" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="59" t="s">
         <v>160</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="H2" s="64" t="s">
         <v>188</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="H2" s="59" t="s">
+        <v>177</v>
+      </c>
+      <c r="I2" s="59" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2425,13 +2454,13 @@
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="67" t="s">
+      <c r="E3" s="70" t="s">
         <v>113</v>
       </c>
       <c r="F3" s="10" t="s">
@@ -2440,17 +2469,17 @@
       <c r="G3" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="H3" s="65" t="s">
+      <c r="H3" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="65" t="s">
-        <v>182</v>
+      <c r="I3" s="68" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2463,13 +2492,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15"/>
@@ -2477,24 +2506,24 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="68" t="s">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="71" t="s">
         <v>200</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-    </row>
-    <row r="2" customFormat="false" ht="141" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="69"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+    </row>
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2507,7 +2536,7 @@
       <c r="D2" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="59" t="s">
         <v>160</v>
       </c>
       <c r="F2" s="8" t="s">
@@ -2519,21 +2548,24 @@
       <c r="H2" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I2" s="59" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="67" t="s">
+      <c r="E3" s="70" t="s">
         <v>113</v>
       </c>
       <c r="F3" s="10" t="s">
@@ -2542,14 +2574,18 @@
       <c r="G3" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="H3" s="72" t="s">
+      <c r="H3" s="75" t="s">
         <v>72</v>
       </c>
-    </row>
+      <c r="I3" s="61" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2568,7 +2604,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.33"/>
@@ -2632,8 +2668,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2652,7 +2688,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -2713,8 +2749,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2733,7 +2769,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -2789,8 +2825,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2809,13 +2845,13 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="76" t="s">
         <v>214</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -2827,8 +2863,8 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
     </row>
     <row r="2" customFormat="false" ht="127" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
@@ -2857,13 +2893,13 @@
       <c r="B3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="78" t="s">
         <v>70</v>
       </c>
       <c r="F3" s="26" t="s">
@@ -2872,8 +2908,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2892,7 +2928,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -2940,13 +2976,13 @@
       <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="78" t="s">
         <v>70</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -2955,8 +2991,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2975,7 +3011,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -2984,13 +3020,13 @@
       <c r="A1" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="81" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="6"/>
@@ -3006,7 +3042,7 @@
       <c r="C2" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="82" t="s">
         <v>220</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -3023,13 +3059,13 @@
       <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="78" t="s">
         <v>221</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="78" t="s">
         <v>70</v>
       </c>
       <c r="F3" s="9" t="s">
@@ -3038,8 +3074,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3058,19 +3094,19 @@
       <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="83" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="83" t="s">
+      <c r="D1" s="86" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="30"/>
@@ -3078,29 +3114,29 @@
       <c r="G1" s="30"/>
     </row>
     <row r="2" customFormat="false" ht="253" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="84"/>
-      <c r="B2" s="84"/>
-      <c r="C2" s="85" t="s">
+      <c r="A2" s="87"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="88" t="s">
         <v>215</v>
       </c>
-      <c r="D2" s="85" t="s">
+      <c r="D2" s="88" t="s">
         <v>223</v>
       </c>
-      <c r="E2" s="85" t="s">
+      <c r="E2" s="88" t="s">
         <v>160</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="88" t="s">
         <v>211</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="88" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="86" t="s">
+      <c r="B3" s="89" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="42" t="s">
@@ -3112,17 +3148,17 @@
       <c r="E3" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="F3" s="86" t="s">
+      <c r="F3" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="86" t="s">
+      <c r="G3" s="89" t="s">
         <v>213</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -3137,11 +3173,11 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -3237,8 +3273,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3257,7 +3293,7 @@
       <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -3368,8 +3404,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3388,7 +3424,7 @@
       <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.5"/>
@@ -3501,8 +3537,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3521,7 +3557,7 @@
       <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.16"/>
@@ -3687,8 +3723,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3833,7 +3869,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -3852,7 +3888,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
   </cols>
@@ -3929,8 +3965,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3949,7 +3985,7 @@
       <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.66"/>
@@ -4124,8 +4160,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
CIV-2248 : New tab added to handle role to access profile mapping
</commit_message>
<xml_diff>
--- a/data/ccd-template.xlsx
+++ b/data/ccd-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\civil\ccd-definition-processor\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drummondm\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E654D2-CE35-4D64-BBE0-2419468AD243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{3A43FD02-4488-48BD-9F15-1F556946B988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B35E4443-8BB5-401D-8B53-03226C96752B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23136" yWindow="936" windowWidth="18444" windowHeight="11256" tabRatio="500" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -40,8 +40,18 @@
     <sheet name="AuthorisationCaseState" sheetId="24" r:id="rId25"/>
     <sheet name="AuthorisationComplexType" sheetId="25" r:id="rId26"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -50,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="231">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -163,6 +173,24 @@
   </si>
   <si>
     <t>RetriesGetCaseUrl</t>
+  </si>
+  <si>
+    <t>RoleToAccessProfiles</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>Authorisation</t>
+  </si>
+  <si>
+    <t>ReadOnly</t>
+  </si>
+  <si>
+    <t>AccessProfiles</t>
+  </si>
+  <si>
+    <t>Disabled</t>
   </si>
   <si>
     <t>CaseField</t>
@@ -804,39 +832,6 @@
   <si>
     <t>C - Create, R - Read, U - Update, D - Delete
 MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
-  </si>
-  <si>
-    <t>Disabled</t>
-  </si>
-  <si>
-    <t>RoleToAccessProfiles</t>
-  </si>
-  <si>
-    <t>RoleName</t>
-  </si>
-  <si>
-    <t>Authorisation</t>
-  </si>
-  <si>
-    <t>AccessProfiles</t>
-  </si>
-  <si>
-    <t>ReadOnly</t>
-  </si>
-  <si>
-    <t>Role Name</t>
-  </si>
-  <si>
-    <t>Case Type Id</t>
-  </si>
-  <si>
-    <t>Access Profiles</t>
-  </si>
-  <si>
-    <t>Read Only</t>
-  </si>
-  <si>
-    <t>CaseAccessCategories</t>
   </si>
 </sst>
 </file>
@@ -847,7 +842,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="33">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1083,27 +1078,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1158,7 +1135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1202,47 +1179,38 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1265,7 +1233,6 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1275,35 +1242,12 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1693,12 +1637,12 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1713,7 +1657,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="117.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="119.45">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1733,7 +1677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -1756,6 +1700,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1767,16 +1714,16 @@
       <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="14.6640625" customWidth="1"/>
-    <col min="22" max="22" width="29.33203125" customWidth="1"/>
+    <col min="1" max="2" width="10.75" style="1" customWidth="1"/>
+    <col min="20" max="20" width="14.75" customWidth="1"/>
+    <col min="22" max="22" width="29.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:22" ht="17.45">
       <c r="A1" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1804,7 +1751,7 @@
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
     </row>
-    <row r="2" spans="1:22" ht="286.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" ht="304.14999999999998">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1812,67 +1759,67 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>26</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="V2" s="45" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="52.5" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="V2" s="41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="53.45">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -1892,57 +1839,60 @@
         <v>14</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="J3" s="46" t="s">
-        <v>141</v>
-      </c>
-      <c r="K3" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="L3" s="46" t="s">
-        <v>143</v>
-      </c>
-      <c r="M3" s="46" t="s">
-        <v>144</v>
-      </c>
-      <c r="N3" s="46" t="s">
-        <v>145</v>
-      </c>
-      <c r="O3" s="46" t="s">
         <v>146</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="L3" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="M3" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="N3" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="O3" s="42" t="s">
+        <v>152</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>32</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="S3" s="20" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="T3" s="20" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="U3" s="20" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="V3" s="20" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1954,14 +1904,14 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17.45">
       <c r="A1" s="2" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -1974,7 +1924,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="78.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="79.900000000000006">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1982,19 +1932,19 @@
         <v>5</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -2005,18 +1955,21 @@
         <v>12</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2028,15 +1981,15 @@
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="26.83203125" customWidth="1"/>
+    <col min="1" max="2" width="10.75" style="1" customWidth="1"/>
+    <col min="15" max="15" width="26.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="17.45">
       <c r="A1" s="2" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2057,7 +2010,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:15" ht="390.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="396.6">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2065,92 +2018,95 @@
         <v>5</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="K2" s="18" t="s">
         <v>26</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="47" t="s">
-        <v>113</v>
+      <c r="D3" s="43" t="s">
+        <v>119</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2162,33 +2118,32 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.75" customWidth="1"/>
+    <col min="2" max="2" width="21.75" customWidth="1"/>
+    <col min="3" max="3" width="26.75" customWidth="1"/>
+    <col min="4" max="4" width="19.25" customWidth="1"/>
+    <col min="5" max="6" width="16.75" customWidth="1"/>
+    <col min="7" max="7" width="22.25" customWidth="1"/>
+    <col min="8" max="8" width="16.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="48" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" s="49" t="s">
+    <row r="1" spans="1:10" ht="17.45">
+      <c r="A1" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="112" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="112.15" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2196,62 +2151,65 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="52" t="s">
-        <v>124</v>
-      </c>
-      <c r="F3" s="52" t="s">
-        <v>169</v>
-      </c>
-      <c r="G3" s="52" t="s">
-        <v>170</v>
-      </c>
-      <c r="H3" s="52" t="s">
-        <v>74</v>
-      </c>
-      <c r="I3" s="52" t="s">
-        <v>171</v>
-      </c>
-      <c r="J3" s="52" t="s">
-        <v>172</v>
+      <c r="E3" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="H3" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="J3" s="44" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2263,28 +2221,28 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17.45">
       <c r="A1" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B1" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-    </row>
-    <row r="2" spans="1:6" ht="104.5" x14ac:dyDescent="0.35">
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+    </row>
+    <row r="2" spans="1:6" ht="106.15">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2292,41 +2250,44 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="58" t="s">
-        <v>69</v>
+      <c r="D3" s="49" t="s">
+        <v>75</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2338,56 +2299,59 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.75" customWidth="1"/>
+    <col min="2" max="2" width="15.75" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17.45">
       <c r="A1" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B1" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="91.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="93">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="58" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="58" t="s">
-        <v>180</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="58"/>
+      <c r="B3" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="49"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2399,60 +2363,63 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="17.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="59" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="17.45">
+      <c r="A3" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="59" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="59" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>113</v>
-      </c>
-      <c r="G3" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="59" t="s">
-        <v>124</v>
-      </c>
-      <c r="I3" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="J3" s="59" t="s">
-        <v>74</v>
-      </c>
-      <c r="K3" s="59" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B4" s="60"/>
-      <c r="G4" s="61"/>
-      <c r="I4" s="62"/>
-      <c r="K4" s="63"/>
+      <c r="D3" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="I3" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="J3" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" s="50" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="B4" s="51"/>
+      <c r="G4" s="52"/>
+      <c r="I4" s="53"/>
+      <c r="K4" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2464,14 +2431,14 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="17.45">
       <c r="A1" s="2" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2485,7 +2452,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="117.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="132.6">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2493,53 +2460,56 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="G2" s="64" t="s">
-        <v>188</v>
-      </c>
-      <c r="H2" s="64" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>193</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>194</v>
+      </c>
+      <c r="H2" s="55" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="58" t="s">
-        <v>69</v>
+      <c r="D3" s="49" t="s">
+        <v>75</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="G3" s="65" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="65" t="s">
-        <v>182</v>
+        <v>130</v>
+      </c>
+      <c r="G3" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="56" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2549,14 +2519,14 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17.45">
       <c r="A1" s="2" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -2564,34 +2534,34 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="78.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="79.900000000000006">
       <c r="A2" s="7" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
@@ -2599,6 +2569,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2610,17 +2583,17 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.75" style="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="17.45">
       <c r="A1" s="2" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2631,12 +2604,12 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-      <c r="H1" s="66"/>
-    </row>
-    <row r="2" spans="1:9" ht="117.5" x14ac:dyDescent="0.35">
+      <c r="H1" s="57"/>
+    </row>
+    <row r="2" spans="1:9" ht="132.6">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2644,59 +2617,62 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E2" s="64" t="s">
-        <v>160</v>
+        <v>191</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>166</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="H2" s="64" t="s">
-        <v>188</v>
-      </c>
-      <c r="I2" s="64" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>193</v>
+      </c>
+      <c r="H2" s="55" t="s">
+        <v>194</v>
+      </c>
+      <c r="I2" s="55" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="67" t="s">
-        <v>113</v>
+      <c r="D3" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>119</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="H3" s="65" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3" s="65" t="s">
-        <v>182</v>
+        <v>130</v>
+      </c>
+      <c r="H3" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="56" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2708,15 +2684,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.25" customWidth="1"/>
+    <col min="3" max="3" width="27.25" customWidth="1"/>
+    <col min="4" max="4" width="30.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17.45">
       <c r="A1" s="12" t="s">
         <v>16</v>
       </c>
@@ -2730,7 +2706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6">
       <c r="A2" s="14" t="s">
         <v>17</v>
       </c>
@@ -2750,7 +2726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2773,6 +2749,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2784,32 +2763,32 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.75" style="1" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="68" t="s">
-        <v>200</v>
-      </c>
-      <c r="B1" s="69" t="s">
+    <row r="1" spans="1:8" ht="18">
+      <c r="A1" s="59" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-    </row>
-    <row r="2" spans="1:8" ht="117.5" x14ac:dyDescent="0.35">
+      <c r="E1" s="57"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+    </row>
+    <row r="2" spans="1:8" ht="119.45">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2817,53 +2796,56 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="E2" s="64" t="s">
-        <v>160</v>
+        <v>180</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>166</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="67" t="s">
-        <v>113</v>
+      <c r="D3" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>119</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="H3" s="72" t="s">
-        <v>72</v>
+        <v>130</v>
+      </c>
+      <c r="H3" s="63" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2873,14 +2855,14 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="17.45">
       <c r="A1" s="2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2894,7 +2876,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="78.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="79.900000000000006">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2903,16 +2885,16 @@
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -2920,21 +2902,24 @@
         <v>11</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2946,14 +2931,14 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1" max="2" width="10.75" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="17.45">
       <c r="A1" s="2" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -2966,7 +2951,7 @@
       </c>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" ht="117.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="119.45">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2974,16 +2959,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
@@ -2994,15 +2979,18 @@
         <v>19</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;6&amp;KFF0000 Classification: Controlled</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3014,14 +3002,14 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="1